<commit_message>
Create function to compute number of individuals per year/species/gender. Begin adding to sample record.
</commit_message>
<xml_diff>
--- a/data/sampleTable.xlsx
+++ b/data/sampleTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17420" windowHeight="21060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18040" windowHeight="20700" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -423,8 +423,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -553,7 +559,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -561,6 +567,9 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -568,6 +577,9 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1225,7 +1237,7 @@
   <dimension ref="A1:AC36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1425,18 +1437,42 @@
       <c r="D4" s="38">
         <v>453</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
+      <c r="E4" s="39">
+        <v>83</v>
+      </c>
+      <c r="F4" s="39">
+        <v>51</v>
+      </c>
+      <c r="G4" s="39">
+        <v>1</v>
+      </c>
+      <c r="H4" s="39">
+        <v>0</v>
+      </c>
+      <c r="I4" s="39">
+        <v>0</v>
+      </c>
+      <c r="J4" s="39">
+        <v>0</v>
+      </c>
+      <c r="K4" s="39">
+        <v>1</v>
+      </c>
+      <c r="L4" s="39">
+        <v>1</v>
+      </c>
+      <c r="M4" s="39">
+        <v>15</v>
+      </c>
+      <c r="N4" s="39">
+        <v>27</v>
+      </c>
+      <c r="O4" s="39">
+        <v>0</v>
+      </c>
+      <c r="P4" s="39">
+        <v>0</v>
+      </c>
       <c r="Q4" s="39"/>
       <c r="R4" s="39"/>
       <c r="S4" s="39"/>

</xml_diff>

<commit_message>
Update sample table based on new lengths.
</commit_message>
<xml_diff>
--- a/data/sampleTable.xlsx
+++ b/data/sampleTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="17540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="28180" yWindow="220" windowWidth="26700" windowHeight="20520" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -684,17 +684,26 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -708,26 +717,17 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1439,11 +1439,11 @@
   <dimension ref="A1:AC36"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1458,97 +1458,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="15" customFormat="1" ht="25">
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="71">
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="82">
         <v>2015</v>
       </c>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="73">
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="84">
         <v>2016</v>
       </c>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="75">
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="78">
         <v>2017</v>
       </c>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="75"/>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="77">
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="80">
         <v>2018</v>
       </c>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="80"/>
+      <c r="AA1" s="80"/>
+      <c r="AB1" s="80"/>
       <c r="AC1" s="13"/>
     </row>
     <row r="2" spans="1:29" s="16" customFormat="1" ht="23">
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="72" t="s">
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72" t="s">
+      <c r="F2" s="83"/>
+      <c r="G2" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72" t="s">
+      <c r="H2" s="83"/>
+      <c r="I2" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="72"/>
-      <c r="K2" s="74" t="s">
+      <c r="J2" s="83"/>
+      <c r="K2" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74" t="s">
+      <c r="L2" s="85"/>
+      <c r="M2" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74" t="s">
+      <c r="N2" s="85"/>
+      <c r="O2" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="76" t="s">
+      <c r="P2" s="85"/>
+      <c r="Q2" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="76"/>
-      <c r="S2" s="76" t="s">
+      <c r="R2" s="79"/>
+      <c r="S2" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="76"/>
-      <c r="U2" s="76" t="s">
+      <c r="T2" s="79"/>
+      <c r="U2" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="76"/>
-      <c r="W2" s="78" t="s">
+      <c r="V2" s="79"/>
+      <c r="W2" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="78"/>
-      <c r="Y2" s="78" t="s">
+      <c r="X2" s="81"/>
+      <c r="Y2" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="Z2" s="78"/>
-      <c r="AA2" s="78" t="s">
+      <c r="Z2" s="81"/>
+      <c r="AA2" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="78"/>
+      <c r="AB2" s="81"/>
       <c r="AC2" s="14"/>
     </row>
     <row r="3" spans="1:29" s="22" customFormat="1" ht="20">
@@ -1639,13 +1639,13 @@
       <c r="AC3" s="21"/>
     </row>
     <row r="4" spans="1:29">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="72" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="23">
@@ -1701,9 +1701,9 @@
       <c r="AB4" s="24"/>
     </row>
     <row r="5" spans="1:29">
-      <c r="A5" s="79"/>
-      <c r="B5" s="79"/>
-      <c r="C5" s="81"/>
+      <c r="A5" s="73"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="23">
         <v>183</v>
       </c>
@@ -1733,8 +1733,8 @@
       <c r="AB5" s="24"/>
     </row>
     <row r="6" spans="1:29">
-      <c r="A6" s="79"/>
-      <c r="B6" s="79"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="25" t="s">
         <v>3</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>193</v>
       </c>
       <c r="F6" s="26">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="G6" s="26">
         <v>0</v>
@@ -1791,8 +1791,8 @@
       <c r="AB6" s="26"/>
     </row>
     <row r="7" spans="1:29">
-      <c r="A7" s="79"/>
-      <c r="B7" s="79" t="s">
+      <c r="A7" s="73"/>
+      <c r="B7" s="73" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="23" t="s">
@@ -1827,9 +1827,9 @@
       <c r="AB7" s="24"/>
     </row>
     <row r="8" spans="1:29">
-      <c r="A8" s="79"/>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79" t="s">
+      <c r="A8" s="73"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="25">
@@ -1885,9 +1885,9 @@
       </c>
     </row>
     <row r="9" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A9" s="80"/>
-      <c r="B9" s="80"/>
-      <c r="C9" s="80"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
       <c r="D9" s="29">
         <v>171</v>
       </c>
@@ -1918,13 +1918,13 @@
       <c r="AC9" s="31"/>
     </row>
     <row r="10" spans="1:29" ht="16" thickTop="1">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="77" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="27">
@@ -1956,9 +1956,9 @@
       <c r="AB10" s="28"/>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="79"/>
-      <c r="B11" s="79"/>
-      <c r="C11" s="81"/>
+      <c r="A11" s="73"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="72"/>
       <c r="D11" s="23">
         <v>139</v>
       </c>
@@ -1988,9 +1988,9 @@
       <c r="AB11" s="24"/>
     </row>
     <row r="12" spans="1:29">
-      <c r="A12" s="79"/>
-      <c r="B12" s="79"/>
-      <c r="C12" s="79" t="s">
+      <c r="A12" s="73"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="25">
@@ -2022,9 +2022,9 @@
       <c r="AB12" s="26"/>
     </row>
     <row r="13" spans="1:29">
-      <c r="A13" s="79"/>
-      <c r="B13" s="79"/>
-      <c r="C13" s="79"/>
+      <c r="A13" s="73"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
       <c r="D13" s="25">
         <v>156</v>
       </c>
@@ -2054,11 +2054,11 @@
       <c r="AB13" s="26"/>
     </row>
     <row r="14" spans="1:29">
-      <c r="A14" s="79"/>
-      <c r="B14" s="79" t="s">
+      <c r="A14" s="73"/>
+      <c r="B14" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="81" t="s">
+      <c r="C14" s="72" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="23">
@@ -2090,9 +2090,9 @@
       <c r="AB14" s="24"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="A15" s="79"/>
-      <c r="B15" s="79"/>
-      <c r="C15" s="81"/>
+      <c r="A15" s="73"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="72"/>
       <c r="D15" s="23">
         <v>132</v>
       </c>
@@ -2122,8 +2122,8 @@
       <c r="AB15" s="24"/>
     </row>
     <row r="16" spans="1:29">
-      <c r="A16" s="79"/>
-      <c r="B16" s="79"/>
+      <c r="A16" s="73"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="25" t="s">
         <v>3</v>
       </c>
@@ -2180,8 +2180,8 @@
       <c r="AB16" s="26"/>
     </row>
     <row r="17" spans="1:29">
-      <c r="A17" s="79"/>
-      <c r="B17" s="79" t="s">
+      <c r="A17" s="73"/>
+      <c r="B17" s="73" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="23" t="s">
@@ -2228,8 +2228,8 @@
       <c r="AB17" s="24"/>
     </row>
     <row r="18" spans="1:29">
-      <c r="A18" s="79"/>
-      <c r="B18" s="79"/>
+      <c r="A18" s="73"/>
+      <c r="B18" s="73"/>
       <c r="C18" s="25" t="s">
         <v>3</v>
       </c>
@@ -2261,10 +2261,10 @@
         <v>1</v>
       </c>
       <c r="Q18" s="26">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="R18" s="26">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="S18" s="26">
         <v>1</v>
@@ -2286,11 +2286,11 @@
       <c r="AB18" s="26"/>
     </row>
     <row r="19" spans="1:29">
-      <c r="A19" s="79"/>
-      <c r="B19" s="79" t="s">
+      <c r="A19" s="73"/>
+      <c r="B19" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="81" t="s">
+      <c r="C19" s="72" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="23">
@@ -2302,14 +2302,24 @@
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
       <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
+      <c r="K19" s="24">
+        <v>81</v>
+      </c>
+      <c r="L19" s="24">
+        <v>60</v>
+      </c>
+      <c r="M19" s="24">
+        <v>19</v>
+      </c>
       <c r="N19" s="24">
-        <v>1</v>
-      </c>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
+        <v>9</v>
+      </c>
+      <c r="O19" s="24">
+        <v>2</v>
+      </c>
+      <c r="P19" s="24">
+        <v>0</v>
+      </c>
       <c r="Q19" s="24"/>
       <c r="R19" s="24"/>
       <c r="S19" s="24"/>
@@ -2324,9 +2334,9 @@
       <c r="AB19" s="24"/>
     </row>
     <row r="20" spans="1:29">
-      <c r="A20" s="79"/>
-      <c r="B20" s="79"/>
-      <c r="C20" s="81"/>
+      <c r="A20" s="73"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="72"/>
       <c r="D20" s="23">
         <v>112</v>
       </c>
@@ -2356,9 +2366,9 @@
       <c r="AB20" s="24"/>
     </row>
     <row r="21" spans="1:29">
-      <c r="A21" s="79"/>
-      <c r="B21" s="79"/>
-      <c r="C21" s="79" t="s">
+      <c r="A21" s="73"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="73" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="25">
@@ -2402,9 +2412,9 @@
       <c r="AB21" s="26"/>
     </row>
     <row r="22" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A22" s="80"/>
-      <c r="B22" s="80"/>
-      <c r="C22" s="80"/>
+      <c r="A22" s="74"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
       <c r="D22" s="29">
         <v>117</v>
       </c>
@@ -2459,10 +2469,10 @@
       <c r="AC22" s="31"/>
     </row>
     <row r="23" spans="1:29" ht="16" thickTop="1">
-      <c r="A23" s="82" t="s">
+      <c r="A23" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="82" t="s">
+      <c r="B23" s="75" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="35" t="s">
@@ -2525,16 +2535,28 @@
       <c r="V23" s="28">
         <v>0</v>
       </c>
-      <c r="W23" s="28"/>
-      <c r="X23" s="28"/>
-      <c r="Y23" s="28"/>
-      <c r="Z23" s="28"/>
-      <c r="AA23" s="28"/>
-      <c r="AB23" s="28"/>
+      <c r="W23" s="28">
+        <v>40</v>
+      </c>
+      <c r="X23" s="28">
+        <v>20</v>
+      </c>
+      <c r="Y23" s="28">
+        <v>22</v>
+      </c>
+      <c r="Z23" s="28">
+        <v>21</v>
+      </c>
+      <c r="AA23" s="28">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="28">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:29">
-      <c r="A24" s="79"/>
-      <c r="B24" s="79"/>
+      <c r="A24" s="73"/>
+      <c r="B24" s="73"/>
       <c r="C24" s="25" t="s">
         <v>3</v>
       </c>
@@ -2565,12 +2587,24 @@
       <c r="P24" s="26">
         <v>25</v>
       </c>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
+      <c r="Q24" s="26">
+        <v>89</v>
+      </c>
+      <c r="R24" s="26">
+        <v>32</v>
+      </c>
+      <c r="S24" s="26">
+        <v>0</v>
+      </c>
+      <c r="T24" s="26">
+        <v>0</v>
+      </c>
+      <c r="U24" s="26">
+        <v>0</v>
+      </c>
+      <c r="V24" s="26">
+        <v>0</v>
+      </c>
       <c r="W24" s="26"/>
       <c r="X24" s="26"/>
       <c r="Y24" s="26"/>
@@ -2579,8 +2613,8 @@
       <c r="AB24" s="26"/>
     </row>
     <row r="25" spans="1:29">
-      <c r="A25" s="79"/>
-      <c r="B25" s="79" t="s">
+      <c r="A25" s="73"/>
+      <c r="B25" s="73" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="23" t="s">
@@ -2615,8 +2649,8 @@
       <c r="AB25" s="24"/>
     </row>
     <row r="26" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A26" s="80"/>
-      <c r="B26" s="80"/>
+      <c r="A26" s="74"/>
+      <c r="B26" s="74"/>
       <c r="C26" s="29" t="s">
         <v>3</v>
       </c>
@@ -2641,20 +2675,30 @@
       <c r="J26" s="30">
         <v>5</v>
       </c>
-      <c r="K26" s="30">
-        <v>51</v>
-      </c>
+      <c r="K26" s="30"/>
       <c r="L26" s="30"/>
       <c r="M26" s="30"/>
       <c r="N26" s="30"/>
       <c r="O26" s="30"/>
       <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="30"/>
-      <c r="U26" s="30"/>
-      <c r="V26" s="30"/>
+      <c r="Q26" s="30">
+        <v>0</v>
+      </c>
+      <c r="R26" s="30">
+        <v>0</v>
+      </c>
+      <c r="S26" s="30">
+        <v>5</v>
+      </c>
+      <c r="T26" s="30">
+        <v>23</v>
+      </c>
+      <c r="U26" s="30">
+        <v>10</v>
+      </c>
+      <c r="V26" s="30">
+        <v>3</v>
+      </c>
       <c r="W26" s="30">
         <v>65</v>
       </c>
@@ -2676,10 +2720,10 @@
       <c r="AC26" s="31"/>
     </row>
     <row r="27" spans="1:29" ht="16" thickTop="1">
-      <c r="A27" s="83" t="s">
+      <c r="A27" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="83" t="s">
+      <c r="B27" s="76" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="27" t="s">
@@ -2724,12 +2768,24 @@
       <c r="P27" s="28">
         <v>8</v>
       </c>
-      <c r="Q27" s="28"/>
-      <c r="R27" s="28"/>
-      <c r="S27" s="28"/>
-      <c r="T27" s="28"/>
-      <c r="U27" s="28"/>
-      <c r="V27" s="28"/>
+      <c r="Q27" s="28">
+        <v>76</v>
+      </c>
+      <c r="R27" s="28">
+        <v>25</v>
+      </c>
+      <c r="S27" s="28">
+        <v>84</v>
+      </c>
+      <c r="T27" s="28">
+        <v>0</v>
+      </c>
+      <c r="U27" s="28">
+        <v>1</v>
+      </c>
+      <c r="V27" s="28">
+        <v>2</v>
+      </c>
       <c r="W27" s="28"/>
       <c r="X27" s="28"/>
       <c r="Y27" s="28"/>
@@ -2738,8 +2794,8 @@
       <c r="AB27" s="28"/>
     </row>
     <row r="28" spans="1:29">
-      <c r="A28" s="79"/>
-      <c r="B28" s="79"/>
+      <c r="A28" s="73"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="25" t="s">
         <v>3</v>
       </c>
@@ -2782,12 +2838,24 @@
       <c r="P28" s="26">
         <v>15</v>
       </c>
-      <c r="Q28" s="26"/>
-      <c r="R28" s="26"/>
-      <c r="S28" s="26"/>
-      <c r="T28" s="26"/>
-      <c r="U28" s="26"/>
-      <c r="V28" s="26"/>
+      <c r="Q28" s="26">
+        <v>33</v>
+      </c>
+      <c r="R28" s="26">
+        <v>0</v>
+      </c>
+      <c r="S28" s="26">
+        <v>6</v>
+      </c>
+      <c r="T28" s="26">
+        <v>0</v>
+      </c>
+      <c r="U28" s="26">
+        <v>8</v>
+      </c>
+      <c r="V28" s="26">
+        <v>4</v>
+      </c>
       <c r="W28" s="26"/>
       <c r="X28" s="26"/>
       <c r="Y28" s="26"/>
@@ -2796,11 +2864,11 @@
       <c r="AB28" s="26"/>
     </row>
     <row r="29" spans="1:29">
-      <c r="A29" s="79"/>
-      <c r="B29" s="79" t="s">
+      <c r="A29" s="73"/>
+      <c r="B29" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="81" t="s">
+      <c r="C29" s="72" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="23">
@@ -2856,9 +2924,9 @@
       <c r="AB29" s="24"/>
     </row>
     <row r="30" spans="1:29">
-      <c r="A30" s="79"/>
-      <c r="B30" s="79"/>
-      <c r="C30" s="81"/>
+      <c r="A30" s="73"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="72"/>
       <c r="D30" s="23">
         <v>412</v>
       </c>
@@ -2888,9 +2956,9 @@
       <c r="AB30" s="24"/>
     </row>
     <row r="31" spans="1:29">
-      <c r="A31" s="79"/>
-      <c r="B31" s="79"/>
-      <c r="C31" s="79" t="s">
+      <c r="A31" s="73"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="73" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="25">
@@ -2934,9 +3002,9 @@
       <c r="AB31" s="26"/>
     </row>
     <row r="32" spans="1:29">
-      <c r="A32" s="79"/>
-      <c r="B32" s="79"/>
-      <c r="C32" s="79"/>
+      <c r="A32" s="73"/>
+      <c r="B32" s="73"/>
+      <c r="C32" s="73"/>
       <c r="D32" s="25">
         <v>414</v>
       </c>
@@ -2978,11 +3046,11 @@
       <c r="AB32" s="26"/>
     </row>
     <row r="33" spans="1:29">
-      <c r="A33" s="79"/>
-      <c r="B33" s="79" t="s">
+      <c r="A33" s="73"/>
+      <c r="B33" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="81" t="s">
+      <c r="C33" s="72" t="s">
         <v>2</v>
       </c>
       <c r="D33" s="23">
@@ -3014,9 +3082,9 @@
       <c r="AB33" s="24"/>
     </row>
     <row r="34" spans="1:29">
-      <c r="A34" s="79"/>
-      <c r="B34" s="79"/>
-      <c r="C34" s="81"/>
+      <c r="A34" s="73"/>
+      <c r="B34" s="73"/>
+      <c r="C34" s="72"/>
       <c r="D34" s="23">
         <v>482</v>
       </c>
@@ -3070,8 +3138,8 @@
       <c r="AB34" s="24"/>
     </row>
     <row r="35" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A35" s="80"/>
-      <c r="B35" s="80"/>
+      <c r="A35" s="74"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="29" t="s">
         <v>3</v>
       </c>
@@ -3131,12 +3199,27 @@
     <row r="36" spans="1:29" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W1:AB1"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B7:B9"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A27:A35"/>
     <mergeCell ref="C21:C22"/>
@@ -3152,27 +3235,12 @@
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W1:AB1"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K1:P1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B33:B35"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3189,10 +3257,10 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3283,10 +3351,10 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="72" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="23">
@@ -3342,8 +3410,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A5" s="79"/>
-      <c r="B5" s="81"/>
+      <c r="A5" s="73"/>
+      <c r="B5" s="72"/>
       <c r="C5" s="42">
         <v>183</v>
       </c>
@@ -3397,7 +3465,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A6" s="79"/>
+      <c r="A6" s="73"/>
       <c r="B6" s="44" t="s">
         <v>3</v>
       </c>
@@ -3406,7 +3474,7 @@
       </c>
       <c r="D6" s="49">
         <f>SUM(Individuals!E6:F6)</f>
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="E6" s="50">
         <f>SUM(Individuals!G6:H6)</f>
@@ -3454,7 +3522,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="73" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="45" t="s">
@@ -3513,8 +3581,8 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="16" thickTop="1">
-      <c r="A8" s="79"/>
-      <c r="B8" s="79" t="s">
+      <c r="A8" s="73"/>
+      <c r="B8" s="73" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="33">
@@ -3570,8 +3638,8 @@
       </c>
     </row>
     <row r="9" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A9" s="79"/>
-      <c r="B9" s="79"/>
+      <c r="A9" s="73"/>
+      <c r="B9" s="73"/>
       <c r="C9" s="34">
         <v>171</v>
       </c>
@@ -3625,10 +3693,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="16" thickTop="1">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="72" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="27">
@@ -3684,8 +3752,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A11" s="79"/>
-      <c r="B11" s="81"/>
+      <c r="A11" s="73"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="42">
         <v>139</v>
       </c>
@@ -3739,8 +3807,8 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="16" thickTop="1">
-      <c r="A12" s="79"/>
-      <c r="B12" s="79" t="s">
+      <c r="A12" s="73"/>
+      <c r="B12" s="73" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="33">
@@ -3796,8 +3864,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A13" s="79"/>
-      <c r="B13" s="79"/>
+      <c r="A13" s="73"/>
+      <c r="B13" s="73"/>
       <c r="C13" s="34">
         <v>156</v>
       </c>
@@ -3851,10 +3919,10 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" thickTop="1">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="72" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="27">
@@ -3910,8 +3978,8 @@
       </c>
     </row>
     <row r="15" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A15" s="79"/>
-      <c r="B15" s="81"/>
+      <c r="A15" s="73"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="42">
         <v>132</v>
       </c>
@@ -3965,7 +4033,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A16" s="79"/>
+      <c r="A16" s="73"/>
       <c r="B16" s="44" t="s">
         <v>3</v>
       </c>
@@ -4022,7 +4090,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A17" s="79" t="s">
+      <c r="A17" s="73" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="45" t="s">
@@ -4081,7 +4149,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A18" s="79"/>
+      <c r="A18" s="73"/>
       <c r="B18" s="44" t="s">
         <v>3</v>
       </c>
@@ -4114,7 +4182,7 @@
       </c>
       <c r="J18" s="49">
         <f>SUM(Individuals!Q18:R18)</f>
-        <v>133</v>
+        <v>183</v>
       </c>
       <c r="K18" s="50">
         <f>SUM(Individuals!S18:T18)</f>
@@ -4138,10 +4206,10 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="16" thickTop="1">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="72" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="27">
@@ -4159,17 +4227,17 @@
         <f>SUM(Individuals!I19:J19)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="54">
+      <c r="G19" s="53">
         <f>SUM(Individuals!K19:L19)</f>
-        <v>0</v>
+        <v>141</v>
       </c>
       <c r="H19" s="54">
         <f>SUM(Individuals!M19:N19)</f>
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="I19" s="54">
         <f>SUM(Individuals!O19:P19)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J19" s="61">
         <f>SUM(Individuals!Q19:R19)</f>
@@ -4197,8 +4265,8 @@
       </c>
     </row>
     <row r="20" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A20" s="79"/>
-      <c r="B20" s="81"/>
+      <c r="A20" s="73"/>
+      <c r="B20" s="72"/>
       <c r="C20" s="42">
         <v>112</v>
       </c>
@@ -4252,8 +4320,8 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="16" thickTop="1">
-      <c r="A21" s="79"/>
-      <c r="B21" s="79" t="s">
+      <c r="A21" s="73"/>
+      <c r="B21" s="73" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="33">
@@ -4309,8 +4377,8 @@
       </c>
     </row>
     <row r="22" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A22" s="79"/>
-      <c r="B22" s="79"/>
+      <c r="A22" s="73"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="34">
         <v>117</v>
       </c>
@@ -4364,7 +4432,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A23" s="79" t="s">
+      <c r="A23" s="73" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="45" t="s">
@@ -4409,21 +4477,21 @@
         <f>SUM(Individuals!U23:V23)</f>
         <v>0</v>
       </c>
-      <c r="M23" s="51">
+      <c r="M23" s="49">
         <f>SUM(Individuals!W23:X23)</f>
-        <v>0</v>
-      </c>
-      <c r="N23" s="51">
+        <v>60</v>
+      </c>
+      <c r="N23" s="49">
         <f>SUM(Individuals!Y23:Z23)</f>
-        <v>0</v>
-      </c>
-      <c r="O23" s="51">
+        <v>43</v>
+      </c>
+      <c r="O23" s="50">
         <f>SUM(Individuals!AA23:BB23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A24" s="79"/>
+      <c r="A24" s="73"/>
       <c r="B24" s="44" t="s">
         <v>3</v>
       </c>
@@ -4454,15 +4522,15 @@
         <f>SUM(Individuals!O24:P24)</f>
         <v>84</v>
       </c>
-      <c r="J24" s="51">
+      <c r="J24" s="49">
         <f>SUM(Individuals!Q24:R24)</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="51">
+        <v>121</v>
+      </c>
+      <c r="K24" s="50">
         <f>SUM(Individuals!S24:T24)</f>
         <v>0</v>
       </c>
-      <c r="L24" s="51">
+      <c r="L24" s="50">
         <f>SUM(Individuals!U24:V24)</f>
         <v>0</v>
       </c>
@@ -4480,7 +4548,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A25" s="79" t="s">
+      <c r="A25" s="73" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="45" t="s">
@@ -4539,7 +4607,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A26" s="79"/>
+      <c r="A26" s="73"/>
       <c r="B26" s="44" t="s">
         <v>3</v>
       </c>
@@ -4560,7 +4628,7 @@
       </c>
       <c r="G26" s="49">
         <f>SUM(Individuals!K26:L26)</f>
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="H26" s="50">
         <f>SUM(Individuals!M26:N26)</f>
@@ -4570,17 +4638,17 @@
         <f>SUM(Individuals!O26:P26)</f>
         <v>0</v>
       </c>
-      <c r="J26" s="51">
+      <c r="J26" s="50">
         <f>SUM(Individuals!Q26:R26)</f>
         <v>0</v>
       </c>
-      <c r="K26" s="51">
+      <c r="K26" s="50">
         <f>SUM(Individuals!S26:T26)</f>
-        <v>0</v>
-      </c>
-      <c r="L26" s="51">
+        <v>28</v>
+      </c>
+      <c r="L26" s="50">
         <f>SUM(Individuals!U26:V26)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="M26" s="49">
         <f>SUM(Individuals!W26:X26)</f>
@@ -4596,7 +4664,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A27" s="79" t="s">
+      <c r="A27" s="73" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="45" t="s">
@@ -4629,17 +4697,17 @@
         <f>SUM(Individuals!O27:P27)</f>
         <v>24</v>
       </c>
-      <c r="J27" s="51">
+      <c r="J27" s="49">
         <f>SUM(Individuals!Q27:R27)</f>
-        <v>0</v>
-      </c>
-      <c r="K27" s="51">
+        <v>101</v>
+      </c>
+      <c r="K27" s="49">
         <f>SUM(Individuals!S27:T27)</f>
-        <v>0</v>
-      </c>
-      <c r="L27" s="51">
+        <v>84</v>
+      </c>
+      <c r="L27" s="50">
         <f>SUM(Individuals!U27:V27)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M27" s="51">
         <f>SUM(Individuals!W27:X27)</f>
@@ -4655,7 +4723,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A28" s="79"/>
+      <c r="A28" s="73"/>
       <c r="B28" s="44" t="s">
         <v>3</v>
       </c>
@@ -4686,17 +4754,17 @@
         <f>SUM(Individuals!O28:P28)</f>
         <v>100</v>
       </c>
-      <c r="J28" s="51">
+      <c r="J28" s="49">
         <f>SUM(Individuals!Q28:R28)</f>
-        <v>0</v>
-      </c>
-      <c r="K28" s="51">
+        <v>33</v>
+      </c>
+      <c r="K28" s="50">
         <f>SUM(Individuals!S28:T28)</f>
-        <v>0</v>
-      </c>
-      <c r="L28" s="51">
+        <v>6</v>
+      </c>
+      <c r="L28" s="50">
         <f>SUM(Individuals!U28:V28)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M28" s="51">
         <f>SUM(Individuals!W28:X28)</f>
@@ -4712,10 +4780,10 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="16" thickTop="1">
-      <c r="A29" s="79" t="s">
+      <c r="A29" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="81" t="s">
+      <c r="B29" s="72" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="27">
@@ -4771,8 +4839,8 @@
       </c>
     </row>
     <row r="30" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A30" s="79"/>
-      <c r="B30" s="81"/>
+      <c r="A30" s="73"/>
+      <c r="B30" s="72"/>
       <c r="C30" s="42">
         <v>412</v>
       </c>
@@ -4826,8 +4894,8 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="16" thickTop="1">
-      <c r="A31" s="79"/>
-      <c r="B31" s="79" t="s">
+      <c r="A31" s="73"/>
+      <c r="B31" s="73" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="33">
@@ -4883,8 +4951,8 @@
       </c>
     </row>
     <row r="32" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A32" s="79"/>
-      <c r="B32" s="79"/>
+      <c r="A32" s="73"/>
+      <c r="B32" s="73"/>
       <c r="C32" s="34">
         <v>414</v>
       </c>
@@ -4938,10 +5006,10 @@
       </c>
     </row>
     <row r="33" spans="1:15" ht="16" thickTop="1">
-      <c r="A33" s="79" t="s">
+      <c r="A33" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="81" t="s">
+      <c r="B33" s="72" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="27">
@@ -4997,8 +5065,8 @@
       </c>
     </row>
     <row r="34" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A34" s="79"/>
-      <c r="B34" s="81"/>
+      <c r="A34" s="73"/>
+      <c r="B34" s="72"/>
       <c r="C34" s="42">
         <v>482</v>
       </c>
@@ -5052,7 +5120,7 @@
       </c>
     </row>
     <row r="35" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A35" s="79"/>
+      <c r="A35" s="73"/>
       <c r="B35" s="44" t="s">
         <v>3</v>
       </c>
@@ -5111,6 +5179,16 @@
     <row r="36" spans="1:15" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="A4:A6"/>
@@ -5127,16 +5205,6 @@
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Update sample table with regional summary for number of individual krill measured.
</commit_message>
<xml_diff>
--- a/data/sampleTable.xlsx
+++ b/data/sampleTable.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28180" yWindow="220" windowWidth="26700" windowHeight="20520" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37620" windowHeight="21140" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
     <sheet name="Individuals" sheetId="2" r:id="rId2"/>
     <sheet name="Ind_Summary" sheetId="3" r:id="rId3"/>
+    <sheet name="Ind_Summary_Region" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="31">
   <si>
     <t>Year</t>
   </si>
@@ -341,7 +342,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -530,8 +531,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -569,8 +603,62 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -684,26 +772,17 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -717,17 +796,26 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -744,8 +832,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="91">
     <cellStyle name="Bad" xfId="22" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -763,6 +875,33 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="21" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -780,6 +919,33 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="23" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="24" builtinId="21"/>
@@ -1439,11 +1605,11 @@
   <dimension ref="A1:AC36"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="Q19" sqref="Q19"/>
+      <selection pane="bottomRight" activeCell="E9" activeCellId="2" sqref="E6 F6 E8:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1458,97 +1624,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="15" customFormat="1" ht="25">
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="82">
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="71">
         <v>2015</v>
       </c>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="84">
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="73">
         <v>2016</v>
       </c>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="78">
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="75">
         <v>2017</v>
       </c>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="80">
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
+      <c r="U1" s="75"/>
+      <c r="V1" s="75"/>
+      <c r="W1" s="77">
         <v>2018</v>
       </c>
-      <c r="X1" s="80"/>
-      <c r="Y1" s="80"/>
-      <c r="Z1" s="80"/>
-      <c r="AA1" s="80"/>
-      <c r="AB1" s="80"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
       <c r="AC1" s="13"/>
     </row>
     <row r="2" spans="1:29" s="16" customFormat="1" ht="23">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="83" t="s">
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83" t="s">
+      <c r="F2" s="72"/>
+      <c r="G2" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83" t="s">
+      <c r="H2" s="72"/>
+      <c r="I2" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="83"/>
-      <c r="K2" s="85" t="s">
+      <c r="J2" s="72"/>
+      <c r="K2" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85" t="s">
+      <c r="L2" s="74"/>
+      <c r="M2" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85" t="s">
+      <c r="N2" s="74"/>
+      <c r="O2" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="79" t="s">
+      <c r="P2" s="74"/>
+      <c r="Q2" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79" t="s">
+      <c r="R2" s="76"/>
+      <c r="S2" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="79"/>
-      <c r="U2" s="79" t="s">
+      <c r="T2" s="76"/>
+      <c r="U2" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="79"/>
-      <c r="W2" s="81" t="s">
+      <c r="V2" s="76"/>
+      <c r="W2" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="81"/>
-      <c r="Y2" s="81" t="s">
+      <c r="X2" s="78"/>
+      <c r="Y2" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="Z2" s="81"/>
-      <c r="AA2" s="81" t="s">
+      <c r="Z2" s="78"/>
+      <c r="AA2" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="81"/>
+      <c r="AB2" s="78"/>
       <c r="AC2" s="14"/>
     </row>
     <row r="3" spans="1:29" s="22" customFormat="1" ht="20">
@@ -1639,13 +1805,13 @@
       <c r="AC3" s="21"/>
     </row>
     <row r="4" spans="1:29">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="81" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="23">
@@ -1701,9 +1867,9 @@
       <c r="AB4" s="24"/>
     </row>
     <row r="5" spans="1:29">
-      <c r="A5" s="73"/>
-      <c r="B5" s="73"/>
-      <c r="C5" s="72"/>
+      <c r="A5" s="79"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="81"/>
       <c r="D5" s="23">
         <v>183</v>
       </c>
@@ -1733,8 +1899,8 @@
       <c r="AB5" s="24"/>
     </row>
     <row r="6" spans="1:29">
-      <c r="A6" s="73"/>
-      <c r="B6" s="73"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="25" t="s">
         <v>3</v>
       </c>
@@ -1791,8 +1957,8 @@
       <c r="AB6" s="26"/>
     </row>
     <row r="7" spans="1:29">
-      <c r="A7" s="73"/>
-      <c r="B7" s="73" t="s">
+      <c r="A7" s="79"/>
+      <c r="B7" s="79" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="23" t="s">
@@ -1827,9 +1993,9 @@
       <c r="AB7" s="24"/>
     </row>
     <row r="8" spans="1:29">
-      <c r="A8" s="73"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73" t="s">
+      <c r="A8" s="79"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="79" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="25">
@@ -1885,9 +2051,9 @@
       </c>
     </row>
     <row r="9" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A9" s="74"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="74"/>
+      <c r="A9" s="80"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="29">
         <v>171</v>
       </c>
@@ -1918,13 +2084,13 @@
       <c r="AC9" s="31"/>
     </row>
     <row r="10" spans="1:29" ht="16" thickTop="1">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="84" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="27">
@@ -1956,9 +2122,9 @@
       <c r="AB10" s="28"/>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="73"/>
-      <c r="B11" s="73"/>
-      <c r="C11" s="72"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="81"/>
       <c r="D11" s="23">
         <v>139</v>
       </c>
@@ -1988,9 +2154,9 @@
       <c r="AB11" s="24"/>
     </row>
     <row r="12" spans="1:29">
-      <c r="A12" s="73"/>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73" t="s">
+      <c r="A12" s="79"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="79" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="25">
@@ -2022,9 +2188,9 @@
       <c r="AB12" s="26"/>
     </row>
     <row r="13" spans="1:29">
-      <c r="A13" s="73"/>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
+      <c r="A13" s="79"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
       <c r="D13" s="25">
         <v>156</v>
       </c>
@@ -2054,11 +2220,11 @@
       <c r="AB13" s="26"/>
     </row>
     <row r="14" spans="1:29">
-      <c r="A14" s="73"/>
-      <c r="B14" s="73" t="s">
+      <c r="A14" s="79"/>
+      <c r="B14" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="72" t="s">
+      <c r="C14" s="81" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="23">
@@ -2090,9 +2256,9 @@
       <c r="AB14" s="24"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="A15" s="73"/>
-      <c r="B15" s="73"/>
-      <c r="C15" s="72"/>
+      <c r="A15" s="79"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="81"/>
       <c r="D15" s="23">
         <v>132</v>
       </c>
@@ -2122,8 +2288,8 @@
       <c r="AB15" s="24"/>
     </row>
     <row r="16" spans="1:29">
-      <c r="A16" s="73"/>
-      <c r="B16" s="73"/>
+      <c r="A16" s="79"/>
+      <c r="B16" s="79"/>
       <c r="C16" s="25" t="s">
         <v>3</v>
       </c>
@@ -2180,8 +2346,8 @@
       <c r="AB16" s="26"/>
     </row>
     <row r="17" spans="1:29">
-      <c r="A17" s="73"/>
-      <c r="B17" s="73" t="s">
+      <c r="A17" s="79"/>
+      <c r="B17" s="79" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="23" t="s">
@@ -2228,8 +2394,8 @@
       <c r="AB17" s="24"/>
     </row>
     <row r="18" spans="1:29">
-      <c r="A18" s="73"/>
-      <c r="B18" s="73"/>
+      <c r="A18" s="79"/>
+      <c r="B18" s="79"/>
       <c r="C18" s="25" t="s">
         <v>3</v>
       </c>
@@ -2286,11 +2452,11 @@
       <c r="AB18" s="26"/>
     </row>
     <row r="19" spans="1:29">
-      <c r="A19" s="73"/>
-      <c r="B19" s="73" t="s">
+      <c r="A19" s="79"/>
+      <c r="B19" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="72" t="s">
+      <c r="C19" s="81" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="23">
@@ -2334,9 +2500,9 @@
       <c r="AB19" s="24"/>
     </row>
     <row r="20" spans="1:29">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
-      <c r="C20" s="72"/>
+      <c r="A20" s="79"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="81"/>
       <c r="D20" s="23">
         <v>112</v>
       </c>
@@ -2366,9 +2532,9 @@
       <c r="AB20" s="24"/>
     </row>
     <row r="21" spans="1:29">
-      <c r="A21" s="73"/>
-      <c r="B21" s="73"/>
-      <c r="C21" s="73" t="s">
+      <c r="A21" s="79"/>
+      <c r="B21" s="79"/>
+      <c r="C21" s="79" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="25">
@@ -2412,9 +2578,9 @@
       <c r="AB21" s="26"/>
     </row>
     <row r="22" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A22" s="74"/>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
+      <c r="A22" s="80"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
       <c r="D22" s="29">
         <v>117</v>
       </c>
@@ -2469,10 +2635,10 @@
       <c r="AC22" s="31"/>
     </row>
     <row r="23" spans="1:29" ht="16" thickTop="1">
-      <c r="A23" s="75" t="s">
+      <c r="A23" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="75" t="s">
+      <c r="B23" s="82" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="35" t="s">
@@ -2555,8 +2721,8 @@
       </c>
     </row>
     <row r="24" spans="1:29">
-      <c r="A24" s="73"/>
-      <c r="B24" s="73"/>
+      <c r="A24" s="79"/>
+      <c r="B24" s="79"/>
       <c r="C24" s="25" t="s">
         <v>3</v>
       </c>
@@ -2613,8 +2779,8 @@
       <c r="AB24" s="26"/>
     </row>
     <row r="25" spans="1:29">
-      <c r="A25" s="73"/>
-      <c r="B25" s="73" t="s">
+      <c r="A25" s="79"/>
+      <c r="B25" s="79" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="23" t="s">
@@ -2649,8 +2815,8 @@
       <c r="AB25" s="24"/>
     </row>
     <row r="26" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A26" s="74"/>
-      <c r="B26" s="74"/>
+      <c r="A26" s="80"/>
+      <c r="B26" s="80"/>
       <c r="C26" s="29" t="s">
         <v>3</v>
       </c>
@@ -2720,10 +2886,10 @@
       <c r="AC26" s="31"/>
     </row>
     <row r="27" spans="1:29" ht="16" thickTop="1">
-      <c r="A27" s="76" t="s">
+      <c r="A27" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="76" t="s">
+      <c r="B27" s="83" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="27" t="s">
@@ -2794,8 +2960,8 @@
       <c r="AB27" s="28"/>
     </row>
     <row r="28" spans="1:29">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
+      <c r="A28" s="79"/>
+      <c r="B28" s="79"/>
       <c r="C28" s="25" t="s">
         <v>3</v>
       </c>
@@ -2864,11 +3030,11 @@
       <c r="AB28" s="26"/>
     </row>
     <row r="29" spans="1:29">
-      <c r="A29" s="73"/>
-      <c r="B29" s="73" t="s">
+      <c r="A29" s="79"/>
+      <c r="B29" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="72" t="s">
+      <c r="C29" s="81" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="23">
@@ -2924,9 +3090,9 @@
       <c r="AB29" s="24"/>
     </row>
     <row r="30" spans="1:29">
-      <c r="A30" s="73"/>
-      <c r="B30" s="73"/>
-      <c r="C30" s="72"/>
+      <c r="A30" s="79"/>
+      <c r="B30" s="79"/>
+      <c r="C30" s="81"/>
       <c r="D30" s="23">
         <v>412</v>
       </c>
@@ -2956,9 +3122,9 @@
       <c r="AB30" s="24"/>
     </row>
     <row r="31" spans="1:29">
-      <c r="A31" s="73"/>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73" t="s">
+      <c r="A31" s="79"/>
+      <c r="B31" s="79"/>
+      <c r="C31" s="79" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="25">
@@ -3002,9 +3168,9 @@
       <c r="AB31" s="26"/>
     </row>
     <row r="32" spans="1:29">
-      <c r="A32" s="73"/>
-      <c r="B32" s="73"/>
-      <c r="C32" s="73"/>
+      <c r="A32" s="79"/>
+      <c r="B32" s="79"/>
+      <c r="C32" s="79"/>
       <c r="D32" s="25">
         <v>414</v>
       </c>
@@ -3046,11 +3212,11 @@
       <c r="AB32" s="26"/>
     </row>
     <row r="33" spans="1:29">
-      <c r="A33" s="73"/>
-      <c r="B33" s="73" t="s">
+      <c r="A33" s="79"/>
+      <c r="B33" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="72" t="s">
+      <c r="C33" s="81" t="s">
         <v>2</v>
       </c>
       <c r="D33" s="23">
@@ -3082,9 +3248,9 @@
       <c r="AB33" s="24"/>
     </row>
     <row r="34" spans="1:29">
-      <c r="A34" s="73"/>
-      <c r="B34" s="73"/>
-      <c r="C34" s="72"/>
+      <c r="A34" s="79"/>
+      <c r="B34" s="79"/>
+      <c r="C34" s="81"/>
       <c r="D34" s="23">
         <v>482</v>
       </c>
@@ -3138,8 +3304,8 @@
       <c r="AB34" s="24"/>
     </row>
     <row r="35" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A35" s="74"/>
-      <c r="B35" s="74"/>
+      <c r="A35" s="80"/>
+      <c r="B35" s="80"/>
       <c r="C35" s="29" t="s">
         <v>3</v>
       </c>
@@ -3199,27 +3365,12 @@
     <row r="36" spans="1:29" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K1:P1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W1:AB1"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B33:B35"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A27:A35"/>
     <mergeCell ref="C21:C22"/>
@@ -3235,12 +3386,27 @@
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W1:AB1"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3256,11 +3422,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O22" sqref="O22"/>
+      <selection pane="bottomRight" sqref="A1:O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3351,10 +3517,10 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="81" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="23">
@@ -3410,8 +3576,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A5" s="73"/>
-      <c r="B5" s="72"/>
+      <c r="A5" s="79"/>
+      <c r="B5" s="81"/>
       <c r="C5" s="42">
         <v>183</v>
       </c>
@@ -3465,7 +3631,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A6" s="73"/>
+      <c r="A6" s="79"/>
       <c r="B6" s="44" t="s">
         <v>3</v>
       </c>
@@ -3522,7 +3688,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="79" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="45" t="s">
@@ -3581,8 +3747,8 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="16" thickTop="1">
-      <c r="A8" s="73"/>
-      <c r="B8" s="73" t="s">
+      <c r="A8" s="79"/>
+      <c r="B8" s="79" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="33">
@@ -3638,8 +3804,8 @@
       </c>
     </row>
     <row r="9" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A9" s="73"/>
-      <c r="B9" s="73"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="79"/>
       <c r="C9" s="34">
         <v>171</v>
       </c>
@@ -3693,10 +3859,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="16" thickTop="1">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="81" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="27">
@@ -3752,8 +3918,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A11" s="73"/>
-      <c r="B11" s="72"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="42">
         <v>139</v>
       </c>
@@ -3807,8 +3973,8 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="16" thickTop="1">
-      <c r="A12" s="73"/>
-      <c r="B12" s="73" t="s">
+      <c r="A12" s="79"/>
+      <c r="B12" s="79" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="33">
@@ -3864,8 +4030,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A13" s="73"/>
-      <c r="B13" s="73"/>
+      <c r="A13" s="79"/>
+      <c r="B13" s="79"/>
       <c r="C13" s="34">
         <v>156</v>
       </c>
@@ -3919,10 +4085,10 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" thickTop="1">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="81" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="27">
@@ -3978,8 +4144,8 @@
       </c>
     </row>
     <row r="15" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A15" s="73"/>
-      <c r="B15" s="72"/>
+      <c r="A15" s="79"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="42">
         <v>132</v>
       </c>
@@ -4033,7 +4199,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A16" s="73"/>
+      <c r="A16" s="79"/>
       <c r="B16" s="44" t="s">
         <v>3</v>
       </c>
@@ -4090,7 +4256,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A17" s="73" t="s">
+      <c r="A17" s="79" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="45" t="s">
@@ -4149,7 +4315,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A18" s="73"/>
+      <c r="A18" s="79"/>
       <c r="B18" s="44" t="s">
         <v>3</v>
       </c>
@@ -4206,10 +4372,10 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="16" thickTop="1">
-      <c r="A19" s="73" t="s">
+      <c r="A19" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="81" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="27">
@@ -4265,8 +4431,8 @@
       </c>
     </row>
     <row r="20" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A20" s="73"/>
-      <c r="B20" s="72"/>
+      <c r="A20" s="79"/>
+      <c r="B20" s="81"/>
       <c r="C20" s="42">
         <v>112</v>
       </c>
@@ -4320,8 +4486,8 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="16" thickTop="1">
-      <c r="A21" s="73"/>
-      <c r="B21" s="73" t="s">
+      <c r="A21" s="79"/>
+      <c r="B21" s="79" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="33">
@@ -4377,8 +4543,8 @@
       </c>
     </row>
     <row r="22" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A22" s="73"/>
-      <c r="B22" s="73"/>
+      <c r="A22" s="79"/>
+      <c r="B22" s="79"/>
       <c r="C22" s="34">
         <v>117</v>
       </c>
@@ -4432,7 +4598,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="79" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="45" t="s">
@@ -4491,7 +4657,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A24" s="73"/>
+      <c r="A24" s="79"/>
       <c r="B24" s="44" t="s">
         <v>3</v>
       </c>
@@ -4548,7 +4714,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A25" s="73" t="s">
+      <c r="A25" s="79" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="45" t="s">
@@ -4607,7 +4773,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A26" s="73"/>
+      <c r="A26" s="79"/>
       <c r="B26" s="44" t="s">
         <v>3</v>
       </c>
@@ -4664,7 +4830,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A27" s="73" t="s">
+      <c r="A27" s="79" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="45" t="s">
@@ -4723,7 +4889,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A28" s="73"/>
+      <c r="A28" s="79"/>
       <c r="B28" s="44" t="s">
         <v>3</v>
       </c>
@@ -4780,10 +4946,10 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="16" thickTop="1">
-      <c r="A29" s="73" t="s">
+      <c r="A29" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="72" t="s">
+      <c r="B29" s="81" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="27">
@@ -4839,8 +5005,8 @@
       </c>
     </row>
     <row r="30" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A30" s="73"/>
-      <c r="B30" s="72"/>
+      <c r="A30" s="79"/>
+      <c r="B30" s="81"/>
       <c r="C30" s="42">
         <v>412</v>
       </c>
@@ -4894,8 +5060,8 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="16" thickTop="1">
-      <c r="A31" s="73"/>
-      <c r="B31" s="73" t="s">
+      <c r="A31" s="79"/>
+      <c r="B31" s="79" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="33">
@@ -4951,8 +5117,8 @@
       </c>
     </row>
     <row r="32" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A32" s="73"/>
-      <c r="B32" s="73"/>
+      <c r="A32" s="79"/>
+      <c r="B32" s="79"/>
       <c r="C32" s="34">
         <v>414</v>
       </c>
@@ -5006,10 +5172,10 @@
       </c>
     </row>
     <row r="33" spans="1:15" ht="16" thickTop="1">
-      <c r="A33" s="73" t="s">
+      <c r="A33" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="72" t="s">
+      <c r="B33" s="81" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="27">
@@ -5065,8 +5231,8 @@
       </c>
     </row>
     <row r="34" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A34" s="73"/>
-      <c r="B34" s="72"/>
+      <c r="A34" s="79"/>
+      <c r="B34" s="81"/>
       <c r="C34" s="42">
         <v>482</v>
       </c>
@@ -5120,7 +5286,7 @@
       </c>
     </row>
     <row r="35" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A35" s="73"/>
+      <c r="A35" s="79"/>
       <c r="B35" s="44" t="s">
         <v>3</v>
       </c>
@@ -5179,16 +5345,6 @@
     <row r="36" spans="1:15" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="A4:A6"/>
@@ -5205,6 +5361,16 @@
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5214,4 +5380,1042 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="14" max="14" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="71" customHeight="1">
+      <c r="A1" s="90" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+    </row>
+    <row r="2" spans="1:23" ht="25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="86">
+        <v>2015</v>
+      </c>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="87">
+        <v>2016</v>
+      </c>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="88">
+        <v>2017</v>
+      </c>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="89">
+        <v>2018</v>
+      </c>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+    </row>
+    <row r="3" spans="1:23" ht="23">
+      <c r="A3" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="92" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="92" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="92" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="93" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="93" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="94" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="94" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="94" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="102" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" s="96" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="98" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="98">
+        <f>SUM(Individuals!E4:F5,Individuals!E7:F7)</f>
+        <v>134</v>
+      </c>
+      <c r="D4" s="98">
+        <f>SUM(Individuals!G4:H5,Individuals!G7:H7)</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="98">
+        <f>SUM(Individuals!I4:J5,Individuals!I7:J7)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="98">
+        <f>SUM(Individuals!K4:L5,Individuals!K7:L7)</f>
+        <v>2</v>
+      </c>
+      <c r="G4" s="98">
+        <f>SUM(Individuals!M4:N5,Individuals!M7:N7)</f>
+        <v>42</v>
+      </c>
+      <c r="H4" s="98">
+        <f>SUM(Individuals!O4:P5,Individuals!O7:P7)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="98">
+        <f>SUM(Individuals!Q4:R5,Individuals!Q7:R7)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="98">
+        <f>SUM(Individuals!S4:T5,Individuals!S7:T7)</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="98">
+        <f>SUM(Individuals!U4:V5,Individuals!U7:V7)</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="98">
+        <f>SUM(Individuals!W4:X5,Individuals!W7:X7)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="98">
+        <f>SUM(Individuals!Y4:Z5,Individuals!Y7:Z7)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="98">
+        <f>SUM(Individuals!AA4:BB5,Individuals!AA7:BB7)</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" s="97"/>
+      <c r="B5" s="100" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="100">
+        <f>SUM(Individuals!E6:F6,Individuals!E8:F9)</f>
+        <v>310</v>
+      </c>
+      <c r="D5" s="100">
+        <f>SUM(Individuals!G6:H6,Individuals!G8:H9)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="100">
+        <f>SUM(Individuals!I6:J6,Individuals!I8:J9)</f>
+        <v>51</v>
+      </c>
+      <c r="F5" s="100">
+        <f>SUM(Individuals!K6:L6,Individuals!K8:L9)</f>
+        <v>298</v>
+      </c>
+      <c r="G5" s="100">
+        <f>SUM(Individuals!M6:N6,Individuals!M8:N9)</f>
+        <v>87</v>
+      </c>
+      <c r="H5" s="100">
+        <f>SUM(Individuals!O6:P6,Individuals!O8:P9)</f>
+        <v>39</v>
+      </c>
+      <c r="I5" s="100">
+        <f>SUM(Individuals!Q6:R6,Individuals!Q8:R9)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="100">
+        <f>SUM(Individuals!S6:T6,Individuals!S8:T9)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="100">
+        <f>SUM(Individuals!U6:V6,Individuals!U8:V9)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="100">
+        <f>SUM(Individuals!W6:X6,Individuals!W8:X9)</f>
+        <v>95</v>
+      </c>
+      <c r="M5" s="100">
+        <f>SUM(Individuals!Y6:Z6,Individuals!Y8:Z9)</f>
+        <v>2</v>
+      </c>
+      <c r="N5" s="100">
+        <f>SUM(Individuals!AA6:BB6,Individuals!AA8:BB9)</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6" s="97" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="98" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="98">
+        <f>SUM(Individuals!E10:F11,Individuals!E14:F15,Individuals!E17:F17,Individuals!E19:F20)</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="98">
+        <f>SUM(Individuals!G10:H11,Individuals!G14:H15,Individuals!G17:H17,Individuals!G19:H20)</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="98">
+        <f>SUM(Individuals!I10:J11,Individuals!I14:J15,Individuals!I17:J17,Individuals!I19:J20)</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="98">
+        <f>SUM(Individuals!K10:L11,Individuals!K14:L15,Individuals!K17:L17,Individuals!K19:L20)</f>
+        <v>246</v>
+      </c>
+      <c r="G6" s="98">
+        <f>SUM(Individuals!M10:N11,Individuals!M14:N15,Individuals!M17:N17,Individuals!M19:N20)</f>
+        <v>134</v>
+      </c>
+      <c r="H6" s="98">
+        <f>SUM(Individuals!O10:P11,Individuals!O14:P15,Individuals!O17:P17,Individuals!O19:P20)</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="98">
+        <f>SUM(Individuals!Q10:R11,Individuals!Q14:R15,Individuals!Q17:R17,Individuals!Q19:R20)</f>
+        <v>83</v>
+      </c>
+      <c r="J6" s="98">
+        <f>SUM(Individuals!S10:T11,Individuals!S14:T15,Individuals!S17:T17,Individuals!S19:T20)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="98">
+        <f>SUM(Individuals!U10:V11,Individuals!U14:V15,Individuals!U17:V17,Individuals!U19:V20)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="98">
+        <f>SUM(Individuals!W10:X11,Individuals!W14:X15,Individuals!W17:X17,Individuals!W19:X20)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="98">
+        <f>SUM(Individuals!Y10:Z11,Individuals!Y14:Z15,Individuals!Y17:Z17,Individuals!Y19:Z20)</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="98">
+        <f>SUM(Individuals!AA10:AB11,Individuals!AA14:AB15,Individuals!AA17:AB17,Individuals!AA19:AB20)</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="100"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="100"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" s="97"/>
+      <c r="B7" s="100" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="100">
+        <f>SUM(Individuals!E12:F13,Individuals!E16:F16,Individuals!E18:F18,Individuals!E21:F22)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="100">
+        <f>SUM(Individuals!G12:H13,Individuals!G16:H16,Individuals!G18:H18,Individuals!G21:H22)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="100">
+        <f>SUM(Individuals!I12:J13,Individuals!I16:J16,Individuals!I18:J18,Individuals!I21:J22)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="100">
+        <f>SUM(Individuals!K12:L13,Individuals!K16:L16,Individuals!K18:L18,Individuals!K21:L22)</f>
+        <v>415</v>
+      </c>
+      <c r="G7" s="100">
+        <f>SUM(Individuals!M12:N13,Individuals!M16:N16,Individuals!M18:N18,Individuals!M21:N22)</f>
+        <v>116</v>
+      </c>
+      <c r="H7" s="100">
+        <f>SUM(Individuals!O12:P13,Individuals!O16:P16,Individuals!O18:P18,Individuals!O21:P22)</f>
+        <v>181</v>
+      </c>
+      <c r="I7" s="100">
+        <f>SUM(Individuals!Q12:R13,Individuals!Q16:R16,Individuals!Q18:R18,Individuals!Q21:R22)</f>
+        <v>322</v>
+      </c>
+      <c r="J7" s="100">
+        <f>SUM(Individuals!S12:T13,Individuals!S16:T16,Individuals!S18:T18,Individuals!S21:T22)</f>
+        <v>6</v>
+      </c>
+      <c r="K7" s="100">
+        <f>SUM(Individuals!U12:V13,Individuals!U16:V16,Individuals!U18:V18,Individuals!U21:V22)</f>
+        <v>153</v>
+      </c>
+      <c r="L7" s="100">
+        <f>SUM(Individuals!W12:X13,Individuals!W16:X16,Individuals!W18:X18,Individuals!W21:X22)</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="100">
+        <f>SUM(Individuals!Y12:Z13,Individuals!Y16:Z16,Individuals!Y18:Z18,Individuals!Y21:Z22)</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="100">
+        <f>SUM(Individuals!AA12:AB13,Individuals!AA16:AB16,Individuals!AA18:AB18,Individuals!AA21:AB22)</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="100"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="100"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="98" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="98">
+        <f>SUM(Individuals!E23:F23,Individuals!E25:F25)</f>
+        <v>41</v>
+      </c>
+      <c r="D8" s="98">
+        <f>SUM(Individuals!G23:H23,Individuals!G25:H25)</f>
+        <v>56</v>
+      </c>
+      <c r="E8" s="98">
+        <f>SUM(Individuals!I23:J23,Individuals!I25:J25)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="98">
+        <f>SUM(Individuals!K23:L23,Individuals!K25:L25)</f>
+        <v>402</v>
+      </c>
+      <c r="G8" s="98">
+        <f>SUM(Individuals!M23:N23,Individuals!M25:N25)</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="98">
+        <f>SUM(Individuals!O23:P23,Individuals!O25:P25)</f>
+        <v>8</v>
+      </c>
+      <c r="I8" s="98">
+        <f>SUM(Individuals!Q23:R23,Individuals!Q25:R25)</f>
+        <v>129</v>
+      </c>
+      <c r="J8" s="98">
+        <f>SUM(Individuals!S23:T23,Individuals!S25:T25)</f>
+        <v>54</v>
+      </c>
+      <c r="K8" s="98">
+        <f>SUM(Individuals!U23:V23,Individuals!U25:V25)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="98">
+        <f>SUM(Individuals!W23:X23,Individuals!W25:X25)</f>
+        <v>60</v>
+      </c>
+      <c r="M8" s="98">
+        <f>SUM(Individuals!Y23:Z23,Individuals!Y25:Z25)</f>
+        <v>43</v>
+      </c>
+      <c r="N8" s="98">
+        <f>SUM(Individuals!AA23:AB23,Individuals!AA25:AB25)</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="100"/>
+      <c r="Q8" s="100"/>
+      <c r="R8" s="100"/>
+      <c r="S8" s="100"/>
+      <c r="T8" s="100"/>
+      <c r="U8" s="100"/>
+      <c r="V8" s="100"/>
+      <c r="W8" s="100"/>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" s="97"/>
+      <c r="B9" s="100" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="100">
+        <f>SUM(Individuals!E24:F24,Individuals!E26:F26)</f>
+        <v>145</v>
+      </c>
+      <c r="D9" s="100">
+        <f>SUM(Individuals!G24:H24,Individuals!G26:H26)</f>
+        <v>6</v>
+      </c>
+      <c r="E9" s="100">
+        <f>SUM(Individuals!I24:J24,Individuals!I26:J26)</f>
+        <v>12</v>
+      </c>
+      <c r="F9" s="100">
+        <f>SUM(Individuals!K24:L24,Individuals!K26:L26)</f>
+        <v>3</v>
+      </c>
+      <c r="G9" s="100">
+        <f>SUM(Individuals!M24:N24,Individuals!M26:N26)</f>
+        <v>3</v>
+      </c>
+      <c r="H9" s="100">
+        <f>SUM(Individuals!O24:P24,Individuals!O26:P26)</f>
+        <v>84</v>
+      </c>
+      <c r="I9" s="100">
+        <f>SUM(Individuals!Q24:R24,Individuals!Q26:R26)</f>
+        <v>121</v>
+      </c>
+      <c r="J9" s="100">
+        <f>SUM(Individuals!S24:T24,Individuals!S26:T26)</f>
+        <v>28</v>
+      </c>
+      <c r="K9" s="100">
+        <f>SUM(Individuals!U24:V24,Individuals!U26:V26)</f>
+        <v>13</v>
+      </c>
+      <c r="L9" s="100">
+        <f>SUM(Individuals!W24:X24,Individuals!W26:X26)</f>
+        <v>108</v>
+      </c>
+      <c r="M9" s="100">
+        <f>SUM(Individuals!Y24:Z24,Individuals!Y26:Z26)</f>
+        <v>3</v>
+      </c>
+      <c r="N9" s="100">
+        <f>SUM(Individuals!AA24:AB24,Individuals!AA26:AB26)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="1"/>
+      <c r="P9" s="100"/>
+      <c r="Q9" s="100"/>
+      <c r="R9" s="100"/>
+      <c r="S9" s="100"/>
+      <c r="T9" s="100"/>
+      <c r="U9" s="100"/>
+      <c r="V9" s="100"/>
+      <c r="W9" s="100"/>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" s="97" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="98" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="98">
+        <f>SUM(Individuals!E27:F27,Individuals!E29:F30,Individuals!E33:F34)</f>
+        <v>161</v>
+      </c>
+      <c r="D10" s="98">
+        <f>SUM(Individuals!G27:H27,Individuals!G29:H30,Individuals!G33:H34)</f>
+        <v>81</v>
+      </c>
+      <c r="E10" s="98">
+        <f>SUM(Individuals!I27:J27,Individuals!I29:J30,Individuals!I33:J34)</f>
+        <v>137</v>
+      </c>
+      <c r="F10" s="98">
+        <f>SUM(Individuals!K27:L27,Individuals!K29:L30,Individuals!K33:L34)</f>
+        <v>29</v>
+      </c>
+      <c r="G10" s="98">
+        <f>SUM(Individuals!M27:N27,Individuals!M29:N30,Individuals!M33:N34)</f>
+        <v>6</v>
+      </c>
+      <c r="H10" s="98">
+        <f>SUM(Individuals!O27:P27,Individuals!O29:P30,Individuals!O33:P34)</f>
+        <v>44</v>
+      </c>
+      <c r="I10" s="98">
+        <f>SUM(Individuals!Q27:R27,Individuals!Q29:R30,Individuals!Q33:R34)</f>
+        <v>151</v>
+      </c>
+      <c r="J10" s="98">
+        <f>SUM(Individuals!S27:T27,Individuals!S29:T30,Individuals!S33:T34)</f>
+        <v>87</v>
+      </c>
+      <c r="K10" s="98">
+        <f>SUM(Individuals!U27:V27,Individuals!U29:V30,Individuals!U33:V34)</f>
+        <v>89</v>
+      </c>
+      <c r="L10" s="98">
+        <f>SUM(Individuals!W27:X27,Individuals!W29:X30,Individuals!W33:X34)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="98">
+        <f>SUM(Individuals!Y27:Z27,Individuals!Y29:Z30,Individuals!Y33:Z34)</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="98">
+        <f>SUM(Individuals!AA27:AB27,Individuals!AA29:AB30,Individuals!AA33:AB34)</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="1"/>
+      <c r="P10" s="100"/>
+      <c r="Q10" s="100"/>
+      <c r="R10" s="100"/>
+      <c r="S10" s="100"/>
+      <c r="T10" s="100"/>
+      <c r="U10" s="100"/>
+      <c r="V10" s="100"/>
+      <c r="W10" s="100"/>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11" s="97"/>
+      <c r="B11" s="100" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="100">
+        <f>SUM(Individuals!E28:F28,Individuals!E31:F32,Individuals!E35:F35)</f>
+        <v>155</v>
+      </c>
+      <c r="D11" s="100">
+        <f>SUM(Individuals!G28:H28,Individuals!G31:H32,Individuals!G35:H35)</f>
+        <v>103</v>
+      </c>
+      <c r="E11" s="100">
+        <f>SUM(Individuals!I28:J28,Individuals!I31:J32,Individuals!I35:J35)</f>
+        <v>206</v>
+      </c>
+      <c r="F11" s="100">
+        <f>SUM(Individuals!K28:L28,Individuals!K31:L32,Individuals!K35:L35)</f>
+        <v>125</v>
+      </c>
+      <c r="G11" s="100">
+        <f>SUM(Individuals!M28:N28,Individuals!M31:N32,Individuals!M35:N35)</f>
+        <v>8</v>
+      </c>
+      <c r="H11" s="100">
+        <f>SUM(Individuals!O28:P28,Individuals!O31:P32,Individuals!O35:P35)</f>
+        <v>131</v>
+      </c>
+      <c r="I11" s="100">
+        <f>SUM(Individuals!Q28:R28,Individuals!Q31:R32,Individuals!Q35:R35)</f>
+        <v>33</v>
+      </c>
+      <c r="J11" s="100">
+        <f>SUM(Individuals!S28:T28,Individuals!S31:T32,Individuals!S35:T35)</f>
+        <v>6</v>
+      </c>
+      <c r="K11" s="100">
+        <f>SUM(Individuals!U28:V28,Individuals!U31:V32,Individuals!U35:V35)</f>
+        <v>88</v>
+      </c>
+      <c r="L11" s="100">
+        <f>SUM(Individuals!W28:X28,Individuals!W31:X32,Individuals!W35:X35)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="100">
+        <f>SUM(Individuals!Y28:Z28,Individuals!Y31:Z32,Individuals!Y35:Z35)</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="100">
+        <f>SUM(Individuals!AA28:AB28,Individuals!AA31:AB32,Individuals!AA35:AB35)</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" s="100"/>
+      <c r="Q11" s="100"/>
+      <c r="R11" s="100"/>
+      <c r="S11" s="100"/>
+      <c r="T11" s="100"/>
+      <c r="U11" s="100"/>
+      <c r="V11" s="100"/>
+      <c r="W11" s="100"/>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="A12" s="99"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="100"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="100"/>
+      <c r="F12" s="100"/>
+      <c r="G12" s="100"/>
+      <c r="H12" s="100"/>
+      <c r="I12" s="100"/>
+      <c r="J12" s="100"/>
+      <c r="K12" s="100"/>
+      <c r="L12" s="100"/>
+      <c r="M12" s="100"/>
+      <c r="N12" s="100"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13" s="99"/>
+      <c r="B13" s="100"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="100"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="100"/>
+      <c r="I13" s="100"/>
+      <c r="J13" s="100"/>
+      <c r="K13" s="100"/>
+      <c r="L13" s="100"/>
+      <c r="M13" s="100"/>
+      <c r="N13" s="100"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14" s="99"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="100"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="100"/>
+      <c r="G14" s="100"/>
+      <c r="H14" s="100"/>
+      <c r="I14" s="100"/>
+      <c r="J14" s="100"/>
+      <c r="K14" s="100"/>
+      <c r="L14" s="100"/>
+      <c r="M14" s="100"/>
+      <c r="N14" s="100"/>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15" s="99"/>
+      <c r="B15" s="100"/>
+      <c r="C15" s="100"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="100"/>
+      <c r="F15" s="100"/>
+      <c r="G15" s="100"/>
+      <c r="H15" s="100"/>
+      <c r="I15" s="100"/>
+      <c r="J15" s="100"/>
+      <c r="K15" s="100"/>
+      <c r="L15" s="100"/>
+      <c r="M15" s="100"/>
+      <c r="N15" s="100"/>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16" s="99"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="100"/>
+      <c r="E16" s="100"/>
+      <c r="F16" s="100"/>
+      <c r="G16" s="100"/>
+      <c r="H16" s="100"/>
+      <c r="I16" s="100"/>
+      <c r="J16" s="100"/>
+      <c r="K16" s="100"/>
+      <c r="L16" s="100"/>
+      <c r="M16" s="100"/>
+      <c r="N16" s="100"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="99"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="100"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="100"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="100"/>
+      <c r="H17" s="100"/>
+      <c r="I17" s="100"/>
+      <c r="J17" s="100"/>
+      <c r="K17" s="100"/>
+      <c r="L17" s="100"/>
+      <c r="M17" s="100"/>
+      <c r="N17" s="100"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="99"/>
+      <c r="B18" s="100"/>
+      <c r="C18" s="100"/>
+      <c r="D18" s="100"/>
+      <c r="E18" s="100"/>
+      <c r="F18" s="100"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="100"/>
+      <c r="I18" s="100"/>
+      <c r="J18" s="100"/>
+      <c r="K18" s="100"/>
+      <c r="L18" s="100"/>
+      <c r="M18" s="100"/>
+      <c r="N18" s="100"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="99"/>
+      <c r="B19" s="100"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="100"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="100"/>
+      <c r="H19" s="100"/>
+      <c r="I19" s="100"/>
+      <c r="J19" s="100"/>
+      <c r="K19" s="100"/>
+      <c r="L19" s="100"/>
+      <c r="M19" s="100"/>
+      <c r="N19" s="100"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="99"/>
+      <c r="B20" s="100"/>
+      <c r="C20" s="100"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="100"/>
+      <c r="F20" s="100"/>
+      <c r="G20" s="100"/>
+      <c r="H20" s="100"/>
+      <c r="I20" s="100"/>
+      <c r="J20" s="100"/>
+      <c r="K20" s="100"/>
+      <c r="L20" s="100"/>
+      <c r="M20" s="100"/>
+      <c r="N20" s="100"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="99"/>
+      <c r="B21" s="100"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="100"/>
+      <c r="F21" s="100"/>
+      <c r="G21" s="100"/>
+      <c r="H21" s="100"/>
+      <c r="I21" s="100"/>
+      <c r="J21" s="100"/>
+      <c r="K21" s="100"/>
+      <c r="L21" s="100"/>
+      <c r="M21" s="100"/>
+      <c r="N21" s="100"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="99"/>
+      <c r="B22" s="100"/>
+      <c r="C22" s="100"/>
+      <c r="D22" s="100"/>
+      <c r="E22" s="100"/>
+      <c r="F22" s="100"/>
+      <c r="G22" s="100"/>
+      <c r="H22" s="100"/>
+      <c r="I22" s="100"/>
+      <c r="J22" s="100"/>
+      <c r="K22" s="100"/>
+      <c r="L22" s="100"/>
+      <c r="M22" s="100"/>
+      <c r="N22" s="100"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="99"/>
+      <c r="B23" s="100"/>
+      <c r="C23" s="100"/>
+      <c r="D23" s="100"/>
+      <c r="E23" s="100"/>
+      <c r="F23" s="100"/>
+      <c r="G23" s="100"/>
+      <c r="H23" s="100"/>
+      <c r="I23" s="100"/>
+      <c r="J23" s="100"/>
+      <c r="K23" s="100"/>
+      <c r="L23" s="100"/>
+      <c r="M23" s="100"/>
+      <c r="N23" s="100"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="99"/>
+      <c r="B24" s="100"/>
+      <c r="C24" s="100"/>
+      <c r="D24" s="100"/>
+      <c r="E24" s="100"/>
+      <c r="F24" s="100"/>
+      <c r="G24" s="100"/>
+      <c r="H24" s="100"/>
+      <c r="I24" s="100"/>
+      <c r="J24" s="100"/>
+      <c r="K24" s="100"/>
+      <c r="L24" s="100"/>
+      <c r="M24" s="100"/>
+      <c r="N24" s="100"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="99"/>
+      <c r="B25" s="100"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="100"/>
+      <c r="E25" s="100"/>
+      <c r="F25" s="100"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="100"/>
+      <c r="K25" s="100"/>
+      <c r="L25" s="100"/>
+      <c r="M25" s="100"/>
+      <c r="N25" s="100"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="99"/>
+      <c r="B26" s="100"/>
+      <c r="C26" s="100"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="100"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="100"/>
+      <c r="I26" s="100"/>
+      <c r="J26" s="100"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="100"/>
+      <c r="M26" s="100"/>
+      <c r="N26" s="100"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="99"/>
+      <c r="B27" s="100"/>
+      <c r="C27" s="100"/>
+      <c r="D27" s="100"/>
+      <c r="E27" s="100"/>
+      <c r="F27" s="100"/>
+      <c r="G27" s="100"/>
+      <c r="H27" s="100"/>
+      <c r="I27" s="100"/>
+      <c r="J27" s="100"/>
+      <c r="K27" s="100"/>
+      <c r="L27" s="100"/>
+      <c r="M27" s="100"/>
+      <c r="N27" s="100"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="99"/>
+      <c r="B28" s="100"/>
+      <c r="C28" s="100"/>
+      <c r="D28" s="100"/>
+      <c r="E28" s="100"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="100"/>
+      <c r="I28" s="100"/>
+      <c r="J28" s="100"/>
+      <c r="K28" s="100"/>
+      <c r="L28" s="100"/>
+      <c r="M28" s="100"/>
+      <c r="N28" s="100"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="99"/>
+      <c r="B29" s="100"/>
+      <c r="C29" s="100"/>
+      <c r="D29" s="100"/>
+      <c r="E29" s="100"/>
+      <c r="F29" s="100"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="100"/>
+      <c r="I29" s="100"/>
+      <c r="J29" s="100"/>
+      <c r="K29" s="100"/>
+      <c r="L29" s="100"/>
+      <c r="M29" s="100"/>
+      <c r="N29" s="100"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="99"/>
+      <c r="B30" s="100"/>
+      <c r="C30" s="100"/>
+      <c r="D30" s="100"/>
+      <c r="E30" s="100"/>
+      <c r="F30" s="100"/>
+      <c r="G30" s="100"/>
+      <c r="H30" s="100"/>
+      <c r="I30" s="100"/>
+      <c r="J30" s="100"/>
+      <c r="K30" s="100"/>
+      <c r="L30" s="100"/>
+      <c r="M30" s="100"/>
+      <c r="N30" s="100"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="99"/>
+      <c r="B31" s="100"/>
+      <c r="C31" s="100"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="100"/>
+      <c r="F31" s="100"/>
+      <c r="G31" s="100"/>
+      <c r="H31" s="100"/>
+      <c r="I31" s="100"/>
+      <c r="J31" s="100"/>
+      <c r="K31" s="100"/>
+      <c r="L31" s="100"/>
+      <c r="M31" s="100"/>
+      <c r="N31" s="100"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="99"/>
+      <c r="B32" s="100"/>
+      <c r="C32" s="100"/>
+      <c r="D32" s="100"/>
+      <c r="E32" s="100"/>
+      <c r="F32" s="100"/>
+      <c r="G32" s="100"/>
+      <c r="H32" s="100"/>
+      <c r="I32" s="100"/>
+      <c r="J32" s="100"/>
+      <c r="K32" s="100"/>
+      <c r="L32" s="100"/>
+      <c r="M32" s="100"/>
+      <c r="N32" s="100"/>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="99"/>
+      <c r="B33" s="100"/>
+      <c r="C33" s="100"/>
+      <c r="D33" s="100"/>
+      <c r="E33" s="100"/>
+      <c r="F33" s="100"/>
+      <c r="G33" s="100"/>
+      <c r="H33" s="100"/>
+      <c r="I33" s="100"/>
+      <c r="J33" s="100"/>
+      <c r="K33" s="100"/>
+      <c r="L33" s="100"/>
+      <c r="M33" s="100"/>
+      <c r="N33" s="100"/>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="99"/>
+      <c r="B34" s="100"/>
+      <c r="C34" s="100"/>
+      <c r="D34" s="100"/>
+      <c r="E34" s="100"/>
+      <c r="F34" s="100"/>
+      <c r="G34" s="100"/>
+      <c r="H34" s="100"/>
+      <c r="I34" s="100"/>
+      <c r="J34" s="100"/>
+      <c r="K34" s="100"/>
+      <c r="L34" s="100"/>
+      <c r="M34" s="100"/>
+      <c r="N34" s="100"/>
+    </row>
+    <row r="35" spans="1:14" s="1" customFormat="1">
+      <c r="A35" s="100"/>
+      <c r="B35" s="100"/>
+      <c r="C35" s="100"/>
+      <c r="D35" s="100"/>
+      <c r="E35" s="100"/>
+      <c r="F35" s="100"/>
+      <c r="G35" s="100"/>
+      <c r="H35" s="100"/>
+      <c r="I35" s="100"/>
+      <c r="J35" s="100"/>
+      <c r="K35" s="100"/>
+      <c r="L35" s="100"/>
+      <c r="M35" s="100"/>
+      <c r="N35" s="100"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C4:N11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to sample table.
</commit_message>
<xml_diff>
--- a/data/sampleTable.xlsx
+++ b/data/sampleTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37620" windowHeight="21140" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17480" windowHeight="21140" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -242,7 +242,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,6 +338,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -748,8 +754,6 @@
     <xf numFmtId="0" fontId="14" fillId="13" borderId="10" xfId="23" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="15" borderId="14" xfId="24" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="15" xfId="22" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="10" xfId="22" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="11" xfId="22" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="15" xfId="22" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="15" xfId="22" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="10" xfId="22" applyFill="1" applyBorder="1"/>
@@ -856,6 +860,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="91">
     <cellStyle name="Bad" xfId="22" builtinId="27"/>
@@ -1294,34 +1304,34 @@
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66">
+      <c r="B1" s="64">
         <v>2015</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="68">
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="66">
         <v>2016</v>
       </c>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="69">
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="67">
         <v>2017</v>
       </c>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="70">
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="68">
         <v>2018</v>
       </c>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
     </row>
     <row r="2" spans="1:21" s="2" customFormat="1" ht="36">
       <c r="A2" s="6" t="s">
@@ -1609,7 +1619,7 @@
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="E9" activeCellId="2" sqref="E6 F6 E8:F9"/>
+      <selection pane="bottomRight" activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1624,97 +1634,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="15" customFormat="1" ht="25">
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="71">
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="69">
         <v>2015</v>
       </c>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="73">
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="71">
         <v>2016</v>
       </c>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="75">
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="73">
         <v>2017</v>
       </c>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="75"/>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="77">
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="75">
         <v>2018</v>
       </c>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="75"/>
+      <c r="AB1" s="75"/>
       <c r="AC1" s="13"/>
     </row>
     <row r="2" spans="1:29" s="16" customFormat="1" ht="23">
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="72" t="s">
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72" t="s">
+      <c r="F2" s="70"/>
+      <c r="G2" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72" t="s">
+      <c r="H2" s="70"/>
+      <c r="I2" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="72"/>
-      <c r="K2" s="74" t="s">
+      <c r="J2" s="70"/>
+      <c r="K2" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74" t="s">
+      <c r="L2" s="72"/>
+      <c r="M2" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74" t="s">
+      <c r="N2" s="72"/>
+      <c r="O2" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="76" t="s">
+      <c r="P2" s="72"/>
+      <c r="Q2" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="76"/>
-      <c r="S2" s="76" t="s">
+      <c r="R2" s="74"/>
+      <c r="S2" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="76"/>
-      <c r="U2" s="76" t="s">
+      <c r="T2" s="74"/>
+      <c r="U2" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="76"/>
-      <c r="W2" s="78" t="s">
+      <c r="V2" s="74"/>
+      <c r="W2" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="78"/>
-      <c r="Y2" s="78" t="s">
+      <c r="X2" s="76"/>
+      <c r="Y2" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="Z2" s="78"/>
-      <c r="AA2" s="78" t="s">
+      <c r="Z2" s="76"/>
+      <c r="AA2" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="78"/>
+      <c r="AB2" s="76"/>
       <c r="AC2" s="14"/>
     </row>
     <row r="3" spans="1:29" s="22" customFormat="1" ht="20">
@@ -1805,13 +1815,13 @@
       <c r="AC3" s="21"/>
     </row>
     <row r="4" spans="1:29">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="79" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="23">
@@ -1867,9 +1877,9 @@
       <c r="AB4" s="24"/>
     </row>
     <row r="5" spans="1:29">
-      <c r="A5" s="79"/>
-      <c r="B5" s="79"/>
-      <c r="C5" s="81"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="23">
         <v>183</v>
       </c>
@@ -1899,8 +1909,8 @@
       <c r="AB5" s="24"/>
     </row>
     <row r="6" spans="1:29">
-      <c r="A6" s="79"/>
-      <c r="B6" s="79"/>
+      <c r="A6" s="77"/>
+      <c r="B6" s="77"/>
       <c r="C6" s="25" t="s">
         <v>3</v>
       </c>
@@ -1957,8 +1967,8 @@
       <c r="AB6" s="26"/>
     </row>
     <row r="7" spans="1:29">
-      <c r="A7" s="79"/>
-      <c r="B7" s="79" t="s">
+      <c r="A7" s="77"/>
+      <c r="B7" s="77" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="23" t="s">
@@ -1993,9 +2003,9 @@
       <c r="AB7" s="24"/>
     </row>
     <row r="8" spans="1:29">
-      <c r="A8" s="79"/>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79" t="s">
+      <c r="A8" s="77"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="77" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="25">
@@ -2051,9 +2061,9 @@
       </c>
     </row>
     <row r="9" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A9" s="80"/>
-      <c r="B9" s="80"/>
-      <c r="C9" s="80"/>
+      <c r="A9" s="78"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
       <c r="D9" s="29">
         <v>171</v>
       </c>
@@ -2084,13 +2094,13 @@
       <c r="AC9" s="31"/>
     </row>
     <row r="10" spans="1:29" ht="16" thickTop="1">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="82" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="27">
@@ -2122,9 +2132,9 @@
       <c r="AB10" s="28"/>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="79"/>
-      <c r="B11" s="79"/>
-      <c r="C11" s="81"/>
+      <c r="A11" s="77"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="79"/>
       <c r="D11" s="23">
         <v>139</v>
       </c>
@@ -2154,9 +2164,9 @@
       <c r="AB11" s="24"/>
     </row>
     <row r="12" spans="1:29">
-      <c r="A12" s="79"/>
-      <c r="B12" s="79"/>
-      <c r="C12" s="79" t="s">
+      <c r="A12" s="77"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="25">
@@ -2188,9 +2198,9 @@
       <c r="AB12" s="26"/>
     </row>
     <row r="13" spans="1:29">
-      <c r="A13" s="79"/>
-      <c r="B13" s="79"/>
-      <c r="C13" s="79"/>
+      <c r="A13" s="77"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="77"/>
       <c r="D13" s="25">
         <v>156</v>
       </c>
@@ -2220,11 +2230,11 @@
       <c r="AB13" s="26"/>
     </row>
     <row r="14" spans="1:29">
-      <c r="A14" s="79"/>
-      <c r="B14" s="79" t="s">
+      <c r="A14" s="77"/>
+      <c r="B14" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="81" t="s">
+      <c r="C14" s="79" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="23">
@@ -2256,9 +2266,9 @@
       <c r="AB14" s="24"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="A15" s="79"/>
-      <c r="B15" s="79"/>
-      <c r="C15" s="81"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="79"/>
       <c r="D15" s="23">
         <v>132</v>
       </c>
@@ -2288,8 +2298,8 @@
       <c r="AB15" s="24"/>
     </row>
     <row r="16" spans="1:29">
-      <c r="A16" s="79"/>
-      <c r="B16" s="79"/>
+      <c r="A16" s="77"/>
+      <c r="B16" s="77"/>
       <c r="C16" s="25" t="s">
         <v>3</v>
       </c>
@@ -2346,8 +2356,8 @@
       <c r="AB16" s="26"/>
     </row>
     <row r="17" spans="1:29">
-      <c r="A17" s="79"/>
-      <c r="B17" s="79" t="s">
+      <c r="A17" s="77"/>
+      <c r="B17" s="77" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="23" t="s">
@@ -2394,8 +2404,8 @@
       <c r="AB17" s="24"/>
     </row>
     <row r="18" spans="1:29">
-      <c r="A18" s="79"/>
-      <c r="B18" s="79"/>
+      <c r="A18" s="77"/>
+      <c r="B18" s="77"/>
       <c r="C18" s="25" t="s">
         <v>3</v>
       </c>
@@ -2452,11 +2462,11 @@
       <c r="AB18" s="26"/>
     </row>
     <row r="19" spans="1:29">
-      <c r="A19" s="79"/>
-      <c r="B19" s="79" t="s">
+      <c r="A19" s="77"/>
+      <c r="B19" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="81" t="s">
+      <c r="C19" s="79" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="23">
@@ -2500,9 +2510,9 @@
       <c r="AB19" s="24"/>
     </row>
     <row r="20" spans="1:29">
-      <c r="A20" s="79"/>
-      <c r="B20" s="79"/>
-      <c r="C20" s="81"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="77"/>
+      <c r="C20" s="79"/>
       <c r="D20" s="23">
         <v>112</v>
       </c>
@@ -2518,12 +2528,24 @@
       <c r="N20" s="24"/>
       <c r="O20" s="24"/>
       <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24"/>
-      <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
+      <c r="Q20" s="24">
+        <v>34</v>
+      </c>
+      <c r="R20" s="24">
+        <v>10</v>
+      </c>
+      <c r="S20" s="24">
+        <v>110</v>
+      </c>
+      <c r="T20" s="24">
+        <v>0</v>
+      </c>
+      <c r="U20" s="24">
+        <v>0</v>
+      </c>
+      <c r="V20" s="24">
+        <v>0</v>
+      </c>
       <c r="W20" s="24"/>
       <c r="X20" s="24"/>
       <c r="Y20" s="24"/>
@@ -2532,9 +2554,9 @@
       <c r="AB20" s="24"/>
     </row>
     <row r="21" spans="1:29">
-      <c r="A21" s="79"/>
-      <c r="B21" s="79"/>
-      <c r="C21" s="79" t="s">
+      <c r="A21" s="77"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="25">
@@ -2578,9 +2600,9 @@
       <c r="AB21" s="26"/>
     </row>
     <row r="22" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A22" s="80"/>
-      <c r="B22" s="80"/>
-      <c r="C22" s="80"/>
+      <c r="A22" s="78"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="78"/>
       <c r="D22" s="29">
         <v>117</v>
       </c>
@@ -2635,10 +2657,10 @@
       <c r="AC22" s="31"/>
     </row>
     <row r="23" spans="1:29" ht="16" thickTop="1">
-      <c r="A23" s="82" t="s">
+      <c r="A23" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="82" t="s">
+      <c r="B23" s="80" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="35" t="s">
@@ -2721,8 +2743,8 @@
       </c>
     </row>
     <row r="24" spans="1:29">
-      <c r="A24" s="79"/>
-      <c r="B24" s="79"/>
+      <c r="A24" s="77"/>
+      <c r="B24" s="77"/>
       <c r="C24" s="25" t="s">
         <v>3</v>
       </c>
@@ -2779,8 +2801,8 @@
       <c r="AB24" s="26"/>
     </row>
     <row r="25" spans="1:29">
-      <c r="A25" s="79"/>
-      <c r="B25" s="79" t="s">
+      <c r="A25" s="77"/>
+      <c r="B25" s="77" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="23" t="s">
@@ -2801,12 +2823,24 @@
       <c r="N25" s="24"/>
       <c r="O25" s="24"/>
       <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="24"/>
-      <c r="U25" s="24"/>
-      <c r="V25" s="24"/>
+      <c r="Q25" s="24">
+        <v>1</v>
+      </c>
+      <c r="R25" s="24">
+        <v>0</v>
+      </c>
+      <c r="S25" s="24">
+        <v>8</v>
+      </c>
+      <c r="T25" s="24">
+        <v>13</v>
+      </c>
+      <c r="U25" s="24">
+        <v>0</v>
+      </c>
+      <c r="V25" s="24">
+        <v>0</v>
+      </c>
       <c r="W25" s="24"/>
       <c r="X25" s="24"/>
       <c r="Y25" s="24"/>
@@ -2815,8 +2849,8 @@
       <c r="AB25" s="24"/>
     </row>
     <row r="26" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A26" s="80"/>
-      <c r="B26" s="80"/>
+      <c r="A26" s="78"/>
+      <c r="B26" s="78"/>
       <c r="C26" s="29" t="s">
         <v>3</v>
       </c>
@@ -2841,14 +2875,26 @@
       <c r="J26" s="30">
         <v>5</v>
       </c>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
+      <c r="K26" s="30">
+        <v>51</v>
+      </c>
+      <c r="L26" s="30">
+        <v>0</v>
+      </c>
+      <c r="M26" s="30">
+        <v>0</v>
+      </c>
+      <c r="N26" s="30">
+        <v>0</v>
+      </c>
+      <c r="O26" s="30">
+        <v>0</v>
+      </c>
+      <c r="P26" s="30">
+        <v>0</v>
+      </c>
       <c r="Q26" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R26" s="30">
         <v>0</v>
@@ -2857,7 +2903,7 @@
         <v>5</v>
       </c>
       <c r="T26" s="30">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="U26" s="30">
         <v>10</v>
@@ -2886,10 +2932,10 @@
       <c r="AC26" s="31"/>
     </row>
     <row r="27" spans="1:29" ht="16" thickTop="1">
-      <c r="A27" s="83" t="s">
+      <c r="A27" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="83" t="s">
+      <c r="B27" s="81" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="27" t="s">
@@ -2960,8 +3006,8 @@
       <c r="AB27" s="28"/>
     </row>
     <row r="28" spans="1:29">
-      <c r="A28" s="79"/>
-      <c r="B28" s="79"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="25" t="s">
         <v>3</v>
       </c>
@@ -3005,16 +3051,16 @@
         <v>15</v>
       </c>
       <c r="Q28" s="26">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="R28" s="26">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="S28" s="26">
         <v>6</v>
       </c>
       <c r="T28" s="26">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="U28" s="26">
         <v>8</v>
@@ -3030,11 +3076,11 @@
       <c r="AB28" s="26"/>
     </row>
     <row r="29" spans="1:29">
-      <c r="A29" s="79"/>
-      <c r="B29" s="79" t="s">
+      <c r="A29" s="77"/>
+      <c r="B29" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="81" t="s">
+      <c r="C29" s="79" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="23">
@@ -3090,9 +3136,9 @@
       <c r="AB29" s="24"/>
     </row>
     <row r="30" spans="1:29">
-      <c r="A30" s="79"/>
-      <c r="B30" s="79"/>
-      <c r="C30" s="81"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="79"/>
       <c r="D30" s="23">
         <v>412</v>
       </c>
@@ -3122,9 +3168,9 @@
       <c r="AB30" s="24"/>
     </row>
     <row r="31" spans="1:29">
-      <c r="A31" s="79"/>
-      <c r="B31" s="79"/>
-      <c r="C31" s="79" t="s">
+      <c r="A31" s="77"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="77" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="25">
@@ -3168,9 +3214,9 @@
       <c r="AB31" s="26"/>
     </row>
     <row r="32" spans="1:29">
-      <c r="A32" s="79"/>
-      <c r="B32" s="79"/>
-      <c r="C32" s="79"/>
+      <c r="A32" s="77"/>
+      <c r="B32" s="77"/>
+      <c r="C32" s="77"/>
       <c r="D32" s="25">
         <v>414</v>
       </c>
@@ -3212,22 +3258,34 @@
       <c r="AB32" s="26"/>
     </row>
     <row r="33" spans="1:29">
-      <c r="A33" s="79"/>
-      <c r="B33" s="79" t="s">
+      <c r="A33" s="77"/>
+      <c r="B33" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="81" t="s">
+      <c r="C33" s="79" t="s">
         <v>2</v>
       </c>
       <c r="D33" s="23">
         <v>481</v>
       </c>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
+      <c r="E33" s="24">
+        <v>85</v>
+      </c>
+      <c r="F33" s="24">
+        <v>52</v>
+      </c>
+      <c r="G33" s="24">
+        <v>0</v>
+      </c>
+      <c r="H33" s="24">
+        <v>0</v>
+      </c>
+      <c r="I33" s="24">
+        <v>37</v>
+      </c>
+      <c r="J33" s="24">
+        <v>4</v>
+      </c>
       <c r="K33" s="24"/>
       <c r="L33" s="24"/>
       <c r="M33" s="24"/>
@@ -3248,9 +3306,9 @@
       <c r="AB33" s="24"/>
     </row>
     <row r="34" spans="1:29">
-      <c r="A34" s="79"/>
-      <c r="B34" s="79"/>
-      <c r="C34" s="81"/>
+      <c r="A34" s="77"/>
+      <c r="B34" s="77"/>
+      <c r="C34" s="79"/>
       <c r="D34" s="23">
         <v>482</v>
       </c>
@@ -3304,8 +3362,8 @@
       <c r="AB34" s="24"/>
     </row>
     <row r="35" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A35" s="80"/>
-      <c r="B35" s="80"/>
+      <c r="A35" s="78"/>
+      <c r="B35" s="78"/>
       <c r="C35" s="29" t="s">
         <v>3</v>
       </c>
@@ -3422,11 +3480,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:O35"/>
+      <selection pane="bottomRight" activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3435,39 +3493,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="48" customHeight="1">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
     </row>
     <row r="2" spans="1:15" ht="25">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
-      <c r="D2" s="86">
+      <c r="D2" s="84">
         <v>2015</v>
       </c>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="87">
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="85">
         <v>2016</v>
       </c>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="88">
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="86">
         <v>2017</v>
       </c>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="89">
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="87">
         <v>2018</v>
       </c>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="87"/>
     </row>
     <row r="3" spans="1:15" ht="23">
       <c r="A3" s="36" t="s">
@@ -3517,10 +3575,10 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="79" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="23">
@@ -3550,34 +3608,34 @@
         <f>SUM(Individuals!O4:P4)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="63">
+      <c r="J4" s="61">
         <f>SUM(Individuals!Q4:R4)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="63">
+      <c r="K4" s="61">
         <f>SUM(Individuals!S4:T4)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="63">
+      <c r="L4" s="61">
         <f>SUM(Individuals!U4:V4)</f>
         <v>0</v>
       </c>
-      <c r="M4" s="63">
+      <c r="M4" s="61">
         <f>SUM(Individuals!W4:X4)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="63">
+      <c r="N4" s="61">
         <f>SUM(Individuals!Y4:Z4)</f>
         <v>0</v>
       </c>
-      <c r="O4" s="63">
+      <c r="O4" s="61">
         <f>SUM(Individuals!AA4:BB4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A5" s="79"/>
-      <c r="B5" s="81"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="79"/>
       <c r="C5" s="42">
         <v>183</v>
       </c>
@@ -3605,33 +3663,33 @@
         <f>SUM(Individuals!O5:P5)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="62">
+      <c r="J5" s="60">
         <f>SUM(Individuals!Q5:R5)</f>
         <v>0</v>
       </c>
-      <c r="K5" s="62">
+      <c r="K5" s="60">
         <f>SUM(Individuals!S5:T5)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="62">
+      <c r="L5" s="60">
         <f>SUM(Individuals!U5:V5)</f>
         <v>0</v>
       </c>
-      <c r="M5" s="62">
+      <c r="M5" s="60">
         <f>SUM(Individuals!W5:X5)</f>
         <v>0</v>
       </c>
-      <c r="N5" s="62">
+      <c r="N5" s="60">
         <f>SUM(Individuals!Y5:Z5)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="62">
+      <c r="O5" s="60">
         <f>SUM(Individuals!AA5:BB5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A6" s="79"/>
+      <c r="A6" s="77"/>
       <c r="B6" s="44" t="s">
         <v>3</v>
       </c>
@@ -3688,7 +3746,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="77" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="45" t="s">
@@ -3709,46 +3767,46 @@
         <f>SUM(Individuals!I7:J7)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="60">
+      <c r="G7" s="58">
         <f>SUM(Individuals!K7:L7)</f>
         <v>0</v>
       </c>
-      <c r="H7" s="60">
+      <c r="H7" s="58">
         <f>SUM(Individuals!M7:N7)</f>
         <v>0</v>
       </c>
-      <c r="I7" s="60">
+      <c r="I7" s="58">
         <f>SUM(Individuals!O7:P7)</f>
         <v>0</v>
       </c>
-      <c r="J7" s="60">
+      <c r="J7" s="58">
         <f>SUM(Individuals!Q7:R7)</f>
         <v>0</v>
       </c>
-      <c r="K7" s="60">
+      <c r="K7" s="58">
         <f>SUM(Individuals!S7:T7)</f>
         <v>0</v>
       </c>
-      <c r="L7" s="60">
+      <c r="L7" s="58">
         <f>SUM(Individuals!U7:V7)</f>
         <v>0</v>
       </c>
-      <c r="M7" s="60">
+      <c r="M7" s="58">
         <f>SUM(Individuals!W7:X7)</f>
         <v>0</v>
       </c>
-      <c r="N7" s="60">
+      <c r="N7" s="58">
         <f>SUM(Individuals!Y7:Z7)</f>
         <v>0</v>
       </c>
-      <c r="O7" s="60">
+      <c r="O7" s="58">
         <f>SUM(Individuals!AA7:BB7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="16" thickTop="1">
-      <c r="A8" s="79"/>
-      <c r="B8" s="79" t="s">
+      <c r="A8" s="77"/>
+      <c r="B8" s="77" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="33">
@@ -3778,15 +3836,15 @@
         <f>SUM(Individuals!O8:P8)</f>
         <v>4</v>
       </c>
-      <c r="J8" s="61">
+      <c r="J8" s="59">
         <f>SUM(Individuals!Q8:R8)</f>
         <v>0</v>
       </c>
-      <c r="K8" s="61">
+      <c r="K8" s="59">
         <f>SUM(Individuals!S8:T8)</f>
         <v>0</v>
       </c>
-      <c r="L8" s="61">
+      <c r="L8" s="59">
         <f>SUM(Individuals!U8:V8)</f>
         <v>0</v>
       </c>
@@ -3804,8 +3862,8 @@
       </c>
     </row>
     <row r="9" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A9" s="79"/>
-      <c r="B9" s="79"/>
+      <c r="A9" s="77"/>
+      <c r="B9" s="77"/>
       <c r="C9" s="34">
         <v>171</v>
       </c>
@@ -3833,15 +3891,15 @@
         <f>SUM(Individuals!O9:P9)</f>
         <v>0</v>
       </c>
-      <c r="J9" s="62">
+      <c r="J9" s="60">
         <f>SUM(Individuals!Q9:R9)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="62">
+      <c r="K9" s="60">
         <f>SUM(Individuals!S9:T9)</f>
         <v>0</v>
       </c>
-      <c r="L9" s="62">
+      <c r="L9" s="60">
         <f>SUM(Individuals!U9:V9)</f>
         <v>0</v>
       </c>
@@ -3859,10 +3917,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="16" thickTop="1">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="79" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="27">
@@ -3880,27 +3938,27 @@
         <f>SUM(Individuals!I10:J10)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="61">
+      <c r="G10" s="59">
         <f>SUM(Individuals!K10:L10)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="61">
+      <c r="H10" s="59">
         <f>SUM(Individuals!M10:N10)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="61">
+      <c r="I10" s="59">
         <f>SUM(Individuals!O10:P10)</f>
         <v>0</v>
       </c>
-      <c r="J10" s="61">
+      <c r="J10" s="59">
         <f>SUM(Individuals!Q10:R10)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="61">
+      <c r="K10" s="59">
         <f>SUM(Individuals!S10:T10)</f>
         <v>0</v>
       </c>
-      <c r="L10" s="61">
+      <c r="L10" s="59">
         <f>SUM(Individuals!U10:V10)</f>
         <v>0</v>
       </c>
@@ -3918,8 +3976,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A11" s="79"/>
-      <c r="B11" s="81"/>
+      <c r="A11" s="77"/>
+      <c r="B11" s="79"/>
       <c r="C11" s="42">
         <v>139</v>
       </c>
@@ -3935,27 +3993,27 @@
         <f>SUM(Individuals!I11:J11)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="62">
+      <c r="G11" s="60">
         <f>SUM(Individuals!K11:L11)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="62">
+      <c r="H11" s="60">
         <f>SUM(Individuals!M11:N11)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="62">
+      <c r="I11" s="60">
         <f>SUM(Individuals!O11:P11)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="62">
+      <c r="J11" s="60">
         <f>SUM(Individuals!Q11:R11)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="62">
+      <c r="K11" s="60">
         <f>SUM(Individuals!S11:T11)</f>
         <v>0</v>
       </c>
-      <c r="L11" s="62">
+      <c r="L11" s="60">
         <f>SUM(Individuals!U11:V11)</f>
         <v>0</v>
       </c>
@@ -3973,8 +4031,8 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="16" thickTop="1">
-      <c r="A12" s="79"/>
-      <c r="B12" s="79" t="s">
+      <c r="A12" s="77"/>
+      <c r="B12" s="77" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="33">
@@ -3992,27 +4050,27 @@
         <f>SUM(Individuals!I12:J12)</f>
         <v>0</v>
       </c>
-      <c r="G12" s="61">
+      <c r="G12" s="59">
         <f>SUM(Individuals!K12:L12)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="61">
+      <c r="H12" s="59">
         <f>SUM(Individuals!M12:N12)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="61">
+      <c r="I12" s="59">
         <f>SUM(Individuals!O12:P12)</f>
         <v>0</v>
       </c>
-      <c r="J12" s="61">
+      <c r="J12" s="59">
         <f>SUM(Individuals!Q12:R12)</f>
         <v>0</v>
       </c>
-      <c r="K12" s="61">
+      <c r="K12" s="59">
         <f>SUM(Individuals!S12:T12)</f>
         <v>0</v>
       </c>
-      <c r="L12" s="61">
+      <c r="L12" s="59">
         <f>SUM(Individuals!U12:V12)</f>
         <v>0</v>
       </c>
@@ -4030,8 +4088,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A13" s="79"/>
-      <c r="B13" s="79"/>
+      <c r="A13" s="77"/>
+      <c r="B13" s="77"/>
       <c r="C13" s="34">
         <v>156</v>
       </c>
@@ -4047,27 +4105,27 @@
         <f>SUM(Individuals!I13:J13)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="62">
+      <c r="G13" s="60">
         <f>SUM(Individuals!K13:L13)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="62">
+      <c r="H13" s="60">
         <f>SUM(Individuals!M13:N13)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="62">
+      <c r="I13" s="60">
         <f>SUM(Individuals!O13:P13)</f>
         <v>0</v>
       </c>
-      <c r="J13" s="62">
+      <c r="J13" s="60">
         <f>SUM(Individuals!Q13:R13)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="62">
+      <c r="K13" s="60">
         <f>SUM(Individuals!S13:T13)</f>
         <v>0</v>
       </c>
-      <c r="L13" s="62">
+      <c r="L13" s="60">
         <f>SUM(Individuals!U13:V13)</f>
         <v>0</v>
       </c>
@@ -4085,10 +4143,10 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" thickTop="1">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="79" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="27">
@@ -4106,15 +4164,15 @@
         <f>SUM(Individuals!I14:J14)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="61">
+      <c r="G14" s="59">
         <f>SUM(Individuals!K14:L14)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="61">
+      <c r="H14" s="59">
         <f>SUM(Individuals!M14:N14)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="61">
+      <c r="I14" s="59">
         <f>SUM(Individuals!O14:P14)</f>
         <v>0</v>
       </c>
@@ -4144,8 +4202,8 @@
       </c>
     </row>
     <row r="15" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A15" s="79"/>
-      <c r="B15" s="81"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="79"/>
       <c r="C15" s="42">
         <v>132</v>
       </c>
@@ -4161,15 +4219,15 @@
         <f>SUM(Individuals!I15:J15)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="62">
+      <c r="G15" s="60">
         <f>SUM(Individuals!K15:L15)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="62">
+      <c r="H15" s="60">
         <f>SUM(Individuals!M15:N15)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="62">
+      <c r="I15" s="60">
         <f>SUM(Individuals!O15:P15)</f>
         <v>0</v>
       </c>
@@ -4199,7 +4257,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A16" s="79"/>
+      <c r="A16" s="77"/>
       <c r="B16" s="44" t="s">
         <v>3</v>
       </c>
@@ -4256,7 +4314,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A17" s="79" t="s">
+      <c r="A17" s="77" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="45" t="s">
@@ -4315,7 +4373,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A18" s="79"/>
+      <c r="A18" s="77"/>
       <c r="B18" s="44" t="s">
         <v>3</v>
       </c>
@@ -4372,10 +4430,10 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="16" thickTop="1">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="79" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="27">
@@ -4405,15 +4463,15 @@
         <f>SUM(Individuals!O19:P19)</f>
         <v>2</v>
       </c>
-      <c r="J19" s="61">
+      <c r="J19" s="53">
         <f>SUM(Individuals!Q19:R19)</f>
         <v>0</v>
       </c>
-      <c r="K19" s="61">
+      <c r="K19" s="53">
         <f>SUM(Individuals!S19:T19)</f>
         <v>0</v>
       </c>
-      <c r="L19" s="61">
+      <c r="L19" s="54">
         <f>SUM(Individuals!U19:V19)</f>
         <v>0</v>
       </c>
@@ -4431,8 +4489,8 @@
       </c>
     </row>
     <row r="20" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A20" s="79"/>
-      <c r="B20" s="81"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="79"/>
       <c r="C20" s="42">
         <v>112</v>
       </c>
@@ -4448,7 +4506,7 @@
         <f>SUM(Individuals!I20:J20)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="47">
+      <c r="G20" s="43">
         <f>SUM(Individuals!K20:L20)</f>
         <v>0</v>
       </c>
@@ -4460,15 +4518,15 @@
         <f>SUM(Individuals!O20:P20)</f>
         <v>0</v>
       </c>
-      <c r="J20" s="62">
+      <c r="J20" s="43">
         <f>SUM(Individuals!Q20:R20)</f>
-        <v>0</v>
-      </c>
-      <c r="K20" s="62">
+        <v>44</v>
+      </c>
+      <c r="K20" s="43">
         <f>SUM(Individuals!S20:T20)</f>
-        <v>0</v>
-      </c>
-      <c r="L20" s="62">
+        <v>110</v>
+      </c>
+      <c r="L20" s="47">
         <f>SUM(Individuals!U20:V20)</f>
         <v>0</v>
       </c>
@@ -4486,8 +4544,8 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="16" thickTop="1">
-      <c r="A21" s="79"/>
-      <c r="B21" s="79" t="s">
+      <c r="A21" s="77"/>
+      <c r="B21" s="77" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="33">
@@ -4543,8 +4601,8 @@
       </c>
     </row>
     <row r="22" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A22" s="79"/>
-      <c r="B22" s="79"/>
+      <c r="A22" s="77"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="34">
         <v>117</v>
       </c>
@@ -4598,7 +4656,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A23" s="79" t="s">
+      <c r="A23" s="77" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="45" t="s">
@@ -4657,7 +4715,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A24" s="79"/>
+      <c r="A24" s="77"/>
       <c r="B24" s="44" t="s">
         <v>3</v>
       </c>
@@ -4714,7 +4772,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A25" s="79" t="s">
+      <c r="A25" s="77" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="45" t="s">
@@ -4747,15 +4805,15 @@
         <f>SUM(Individuals!O25:P25)</f>
         <v>0</v>
       </c>
-      <c r="J25" s="60">
+      <c r="J25" s="50">
         <f>SUM(Individuals!Q25:R25)</f>
-        <v>0</v>
-      </c>
-      <c r="K25" s="60">
+        <v>1</v>
+      </c>
+      <c r="K25" s="50">
         <f>SUM(Individuals!S25:T25)</f>
-        <v>0</v>
-      </c>
-      <c r="L25" s="60">
+        <v>21</v>
+      </c>
+      <c r="L25" s="50">
         <f>SUM(Individuals!U25:V25)</f>
         <v>0</v>
       </c>
@@ -4773,7 +4831,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A26" s="79"/>
+      <c r="A26" s="77"/>
       <c r="B26" s="44" t="s">
         <v>3</v>
       </c>
@@ -4794,7 +4852,7 @@
       </c>
       <c r="G26" s="49">
         <f>SUM(Individuals!K26:L26)</f>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="H26" s="50">
         <f>SUM(Individuals!M26:N26)</f>
@@ -4806,11 +4864,11 @@
       </c>
       <c r="J26" s="50">
         <f>SUM(Individuals!Q26:R26)</f>
-        <v>0</v>
-      </c>
-      <c r="K26" s="50">
+        <v>10</v>
+      </c>
+      <c r="K26" s="49">
         <f>SUM(Individuals!S26:T26)</f>
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="L26" s="50">
         <f>SUM(Individuals!U26:V26)</f>
@@ -4830,7 +4888,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A27" s="79" t="s">
+      <c r="A27" s="77" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="45" t="s">
@@ -4889,7 +4947,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A28" s="79"/>
+      <c r="A28" s="77"/>
       <c r="B28" s="44" t="s">
         <v>3</v>
       </c>
@@ -4922,11 +4980,11 @@
       </c>
       <c r="J28" s="49">
         <f>SUM(Individuals!Q28:R28)</f>
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="K28" s="50">
         <f>SUM(Individuals!S28:T28)</f>
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="L28" s="50">
         <f>SUM(Individuals!U28:V28)</f>
@@ -4946,10 +5004,10 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="16" thickTop="1">
-      <c r="A29" s="79" t="s">
+      <c r="A29" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="81" t="s">
+      <c r="B29" s="79" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="27">
@@ -5005,8 +5063,8 @@
       </c>
     </row>
     <row r="30" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A30" s="79"/>
-      <c r="B30" s="81"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="79"/>
       <c r="C30" s="42">
         <v>412</v>
       </c>
@@ -5034,15 +5092,15 @@
         <f>SUM(Individuals!O30:P30)</f>
         <v>0</v>
       </c>
-      <c r="J30" s="62">
+      <c r="J30" s="60">
         <f>SUM(Individuals!Q30:R30)</f>
         <v>0</v>
       </c>
-      <c r="K30" s="62">
+      <c r="K30" s="60">
         <f>SUM(Individuals!S30:T30)</f>
         <v>0</v>
       </c>
-      <c r="L30" s="62">
+      <c r="L30" s="60">
         <f>SUM(Individuals!U30:V30)</f>
         <v>0</v>
       </c>
@@ -5060,8 +5118,8 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="16" thickTop="1">
-      <c r="A31" s="79"/>
-      <c r="B31" s="79" t="s">
+      <c r="A31" s="77"/>
+      <c r="B31" s="77" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="33">
@@ -5091,34 +5149,34 @@
         <f>SUM(Individuals!O31:P31)</f>
         <v>0</v>
       </c>
-      <c r="J31" s="64">
+      <c r="J31" s="62">
         <f>SUM(Individuals!Q31:R31)</f>
         <v>0</v>
       </c>
-      <c r="K31" s="64">
+      <c r="K31" s="62">
         <f>SUM(Individuals!S31:T31)</f>
         <v>0</v>
       </c>
-      <c r="L31" s="64">
+      <c r="L31" s="62">
         <f>SUM(Individuals!U31:V31)</f>
         <v>0</v>
       </c>
-      <c r="M31" s="61">
+      <c r="M31" s="59">
         <f>SUM(Individuals!W31:X31)</f>
         <v>0</v>
       </c>
-      <c r="N31" s="61">
+      <c r="N31" s="59">
         <f>SUM(Individuals!Y31:Z31)</f>
         <v>0</v>
       </c>
-      <c r="O31" s="61">
+      <c r="O31" s="59">
         <f>SUM(Individuals!AA31:BB31)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A32" s="79"/>
-      <c r="B32" s="79"/>
+      <c r="A32" s="77"/>
+      <c r="B32" s="77"/>
       <c r="C32" s="34">
         <v>414</v>
       </c>
@@ -5146,52 +5204,52 @@
         <f>SUM(Individuals!O32:P32)</f>
         <v>1</v>
       </c>
-      <c r="J32" s="65">
+      <c r="J32" s="63">
         <f>SUM(Individuals!Q32:R32)</f>
         <v>0</v>
       </c>
-      <c r="K32" s="65">
+      <c r="K32" s="63">
         <f>SUM(Individuals!S32:T32)</f>
         <v>0</v>
       </c>
-      <c r="L32" s="65">
+      <c r="L32" s="63">
         <f>SUM(Individuals!U32:V32)</f>
         <v>0</v>
       </c>
-      <c r="M32" s="62">
+      <c r="M32" s="60">
         <f>SUM(Individuals!W32:X32)</f>
         <v>0</v>
       </c>
-      <c r="N32" s="62">
+      <c r="N32" s="60">
         <f>SUM(Individuals!Y32:Z32)</f>
         <v>0</v>
       </c>
-      <c r="O32" s="62">
+      <c r="O32" s="60">
         <f>SUM(Individuals!AA32:BB32)</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="16" thickTop="1">
-      <c r="A33" s="79" t="s">
+      <c r="A33" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="81" t="s">
+      <c r="B33" s="79" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="27">
         <v>481</v>
       </c>
-      <c r="D33" s="57">
+      <c r="D33" s="53">
         <f>SUM(Individuals!E33:F33)</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="57">
+        <v>137</v>
+      </c>
+      <c r="E33" s="54">
         <f>SUM(Individuals!G33:H33)</f>
         <v>0</v>
       </c>
-      <c r="F33" s="57">
+      <c r="F33" s="53">
         <f>SUM(Individuals!I33:J33)</f>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="G33" s="54">
         <f>SUM(Individuals!K33:L33)</f>
@@ -5217,34 +5275,34 @@
         <f>SUM(Individuals!U33:V33)</f>
         <v>0</v>
       </c>
-      <c r="M33" s="61">
+      <c r="M33" s="59">
         <f>SUM(Individuals!W33:X33)</f>
         <v>0</v>
       </c>
-      <c r="N33" s="61">
+      <c r="N33" s="59">
         <f>SUM(Individuals!Y33:Z33)</f>
         <v>0</v>
       </c>
-      <c r="O33" s="61">
+      <c r="O33" s="59">
         <f>SUM(Individuals!AA33:BB33)</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A34" s="79"/>
-      <c r="B34" s="81"/>
+      <c r="A34" s="77"/>
+      <c r="B34" s="79"/>
       <c r="C34" s="42">
         <v>482</v>
       </c>
-      <c r="D34" s="58">
+      <c r="D34" s="43">
         <f>SUM(Individuals!E34:F34)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="58">
+      <c r="E34" s="47">
         <f>SUM(Individuals!G34:H34)</f>
         <v>0</v>
       </c>
-      <c r="F34" s="58">
+      <c r="F34" s="43">
         <f>SUM(Individuals!I34:J34)</f>
         <v>0</v>
       </c>
@@ -5272,36 +5330,36 @@
         <f>SUM(Individuals!U34:V34)</f>
         <v>86</v>
       </c>
-      <c r="M34" s="62">
+      <c r="M34" s="60">
         <f>SUM(Individuals!W34:X34)</f>
         <v>0</v>
       </c>
-      <c r="N34" s="62">
+      <c r="N34" s="60">
         <f>SUM(Individuals!Y34:Z34)</f>
         <v>0</v>
       </c>
-      <c r="O34" s="62">
+      <c r="O34" s="60">
         <f>SUM(Individuals!AA34:BB34)</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A35" s="79"/>
+      <c r="A35" s="77"/>
       <c r="B35" s="44" t="s">
         <v>3</v>
       </c>
       <c r="C35" s="44">
         <v>402</v>
       </c>
-      <c r="D35" s="59">
+      <c r="D35" s="57">
         <f>SUM(Individuals!E35:F35)</f>
         <v>0</v>
       </c>
-      <c r="E35" s="59">
+      <c r="E35" s="57">
         <f>SUM(Individuals!G35:H35)</f>
         <v>0</v>
       </c>
-      <c r="F35" s="59">
+      <c r="F35" s="57">
         <f>SUM(Individuals!I35:J35)</f>
         <v>0</v>
       </c>
@@ -5386,8 +5444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5396,134 +5454,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="71" customHeight="1">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
     </row>
     <row r="2" spans="1:23" ht="25">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
-      <c r="C2" s="86">
+      <c r="C2" s="84">
         <v>2015</v>
       </c>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="87">
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="85">
         <v>2016</v>
       </c>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="88">
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="86">
         <v>2017</v>
       </c>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="89">
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="87">
         <v>2018</v>
       </c>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="M2" s="87"/>
+      <c r="N2" s="87"/>
     </row>
     <row r="3" spans="1:23" ht="23">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="92" t="s">
+      <c r="D3" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="93" t="s">
+      <c r="F3" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="93" t="s">
+      <c r="G3" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="93" t="s">
+      <c r="H3" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="94" t="s">
+      <c r="I3" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="94" t="s">
+      <c r="J3" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="94" t="s">
+      <c r="K3" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="95" t="s">
+      <c r="L3" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="101" t="s">
+      <c r="M3" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="102" t="s">
+      <c r="N3" s="100" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:23">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="98">
+      <c r="C4" s="96">
         <f>SUM(Individuals!E4:F5,Individuals!E7:F7)</f>
         <v>134</v>
       </c>
-      <c r="D4" s="98">
+      <c r="D4" s="96">
         <f>SUM(Individuals!G4:H5,Individuals!G7:H7)</f>
         <v>1</v>
       </c>
-      <c r="E4" s="98">
+      <c r="E4" s="96">
         <f>SUM(Individuals!I4:J5,Individuals!I7:J7)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="98">
+      <c r="F4" s="96">
         <f>SUM(Individuals!K4:L5,Individuals!K7:L7)</f>
         <v>2</v>
       </c>
-      <c r="G4" s="98">
+      <c r="G4" s="96">
         <f>SUM(Individuals!M4:N5,Individuals!M7:N7)</f>
         <v>42</v>
       </c>
-      <c r="H4" s="98">
+      <c r="H4" s="96">
         <f>SUM(Individuals!O4:P5,Individuals!O7:P7)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="98">
+      <c r="I4" s="96">
         <f>SUM(Individuals!Q4:R5,Individuals!Q7:R7)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="98">
+      <c r="J4" s="96">
         <f>SUM(Individuals!S4:T5,Individuals!S7:T7)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="98">
+      <c r="K4" s="96">
         <f>SUM(Individuals!U4:V5,Individuals!U7:V7)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="98">
+      <c r="L4" s="96">
         <f>SUM(Individuals!W4:X5,Individuals!W7:X7)</f>
         <v>0</v>
       </c>
-      <c r="M4" s="98">
+      <c r="M4" s="96">
         <f>SUM(Individuals!Y4:Z5,Individuals!Y7:Z7)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="98">
+      <c r="N4" s="96">
         <f>SUM(Individuals!AA4:BB5,Individuals!AA7:BB7)</f>
         <v>0</v>
       </c>
@@ -5538,55 +5596,55 @@
       <c r="W4" s="1"/>
     </row>
     <row r="5" spans="1:23">
-      <c r="A5" s="97"/>
-      <c r="B5" s="100" t="s">
+      <c r="A5" s="95"/>
+      <c r="B5" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="100">
+      <c r="C5" s="98">
         <f>SUM(Individuals!E6:F6,Individuals!E8:F9)</f>
         <v>310</v>
       </c>
-      <c r="D5" s="100">
+      <c r="D5" s="98">
         <f>SUM(Individuals!G6:H6,Individuals!G8:H9)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="100">
+      <c r="E5" s="98">
         <f>SUM(Individuals!I6:J6,Individuals!I8:J9)</f>
         <v>51</v>
       </c>
-      <c r="F5" s="100">
+      <c r="F5" s="98">
         <f>SUM(Individuals!K6:L6,Individuals!K8:L9)</f>
         <v>298</v>
       </c>
-      <c r="G5" s="100">
+      <c r="G5" s="98">
         <f>SUM(Individuals!M6:N6,Individuals!M8:N9)</f>
         <v>87</v>
       </c>
-      <c r="H5" s="100">
+      <c r="H5" s="98">
         <f>SUM(Individuals!O6:P6,Individuals!O8:P9)</f>
         <v>39</v>
       </c>
-      <c r="I5" s="100">
+      <c r="I5" s="98">
         <f>SUM(Individuals!Q6:R6,Individuals!Q8:R9)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="100">
+      <c r="J5" s="98">
         <f>SUM(Individuals!S6:T6,Individuals!S8:T9)</f>
         <v>0</v>
       </c>
-      <c r="K5" s="100">
+      <c r="K5" s="98">
         <f>SUM(Individuals!U6:V6,Individuals!U8:V9)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="100">
+      <c r="L5" s="98">
         <f>SUM(Individuals!W6:X6,Individuals!W8:X9)</f>
         <v>95</v>
       </c>
-      <c r="M5" s="100">
+      <c r="M5" s="98">
         <f>SUM(Individuals!Y6:Z6,Individuals!Y8:Z9)</f>
         <v>2</v>
       </c>
-      <c r="N5" s="100">
+      <c r="N5" s="98">
         <f>SUM(Individuals!AA6:BB6,Individuals!AA8:BB9)</f>
         <v>0</v>
       </c>
@@ -5601,64 +5659,64 @@
       <c r="W5" s="1"/>
     </row>
     <row r="6" spans="1:23">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="98">
+      <c r="C6" s="101">
         <f>SUM(Individuals!E10:F11,Individuals!E14:F15,Individuals!E17:F17,Individuals!E19:F20)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="98">
+      <c r="D6" s="101">
         <f>SUM(Individuals!G10:H11,Individuals!G14:H15,Individuals!G17:H17,Individuals!G19:H20)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="98">
+      <c r="E6" s="101">
         <f>SUM(Individuals!I10:J11,Individuals!I14:J15,Individuals!I17:J17,Individuals!I19:J20)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="98">
+      <c r="F6" s="96">
         <f>SUM(Individuals!K10:L11,Individuals!K14:L15,Individuals!K17:L17,Individuals!K19:L20)</f>
         <v>246</v>
       </c>
-      <c r="G6" s="98">
+      <c r="G6" s="96">
         <f>SUM(Individuals!M10:N11,Individuals!M14:N15,Individuals!M17:N17,Individuals!M19:N20)</f>
         <v>134</v>
       </c>
-      <c r="H6" s="98">
+      <c r="H6" s="96">
         <f>SUM(Individuals!O10:P11,Individuals!O14:P15,Individuals!O17:P17,Individuals!O19:P20)</f>
         <v>2</v>
       </c>
-      <c r="I6" s="98">
+      <c r="I6" s="96">
         <f>SUM(Individuals!Q10:R11,Individuals!Q14:R15,Individuals!Q17:R17,Individuals!Q19:R20)</f>
-        <v>83</v>
-      </c>
-      <c r="J6" s="98">
+        <v>127</v>
+      </c>
+      <c r="J6" s="96">
         <f>SUM(Individuals!S10:T11,Individuals!S14:T15,Individuals!S17:T17,Individuals!S19:T20)</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="98">
+        <v>110</v>
+      </c>
+      <c r="K6" s="96">
         <f>SUM(Individuals!U10:V11,Individuals!U14:V15,Individuals!U17:V17,Individuals!U19:V20)</f>
         <v>0</v>
       </c>
-      <c r="L6" s="98">
+      <c r="L6" s="96">
         <f>SUM(Individuals!W10:X11,Individuals!W14:X15,Individuals!W17:X17,Individuals!W19:X20)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="98">
+      <c r="M6" s="96">
         <f>SUM(Individuals!Y10:Z11,Individuals!Y14:Z15,Individuals!Y17:Z17,Individuals!Y19:Z20)</f>
         <v>0</v>
       </c>
-      <c r="N6" s="98">
+      <c r="N6" s="96">
         <f>SUM(Individuals!AA10:AB11,Individuals!AA14:AB15,Individuals!AA17:AB17,Individuals!AA19:AB20)</f>
         <v>0</v>
       </c>
       <c r="O6" s="1"/>
-      <c r="P6" s="100"/>
+      <c r="P6" s="98"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="100"/>
+      <c r="R6" s="98"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -5666,62 +5724,62 @@
       <c r="W6" s="1"/>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="97"/>
-      <c r="B7" s="100" t="s">
+      <c r="A7" s="95"/>
+      <c r="B7" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="100">
+      <c r="C7" s="102">
         <f>SUM(Individuals!E12:F13,Individuals!E16:F16,Individuals!E18:F18,Individuals!E21:F22)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="100">
+      <c r="D7" s="102">
         <f>SUM(Individuals!G12:H13,Individuals!G16:H16,Individuals!G18:H18,Individuals!G21:H22)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="100">
+      <c r="E7" s="102">
         <f>SUM(Individuals!I12:J13,Individuals!I16:J16,Individuals!I18:J18,Individuals!I21:J22)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="100">
+      <c r="F7" s="98">
         <f>SUM(Individuals!K12:L13,Individuals!K16:L16,Individuals!K18:L18,Individuals!K21:L22)</f>
         <v>415</v>
       </c>
-      <c r="G7" s="100">
+      <c r="G7" s="98">
         <f>SUM(Individuals!M12:N13,Individuals!M16:N16,Individuals!M18:N18,Individuals!M21:N22)</f>
         <v>116</v>
       </c>
-      <c r="H7" s="100">
+      <c r="H7" s="98">
         <f>SUM(Individuals!O12:P13,Individuals!O16:P16,Individuals!O18:P18,Individuals!O21:P22)</f>
         <v>181</v>
       </c>
-      <c r="I7" s="100">
+      <c r="I7" s="98">
         <f>SUM(Individuals!Q12:R13,Individuals!Q16:R16,Individuals!Q18:R18,Individuals!Q21:R22)</f>
         <v>322</v>
       </c>
-      <c r="J7" s="100">
+      <c r="J7" s="98">
         <f>SUM(Individuals!S12:T13,Individuals!S16:T16,Individuals!S18:T18,Individuals!S21:T22)</f>
         <v>6</v>
       </c>
-      <c r="K7" s="100">
+      <c r="K7" s="98">
         <f>SUM(Individuals!U12:V13,Individuals!U16:V16,Individuals!U18:V18,Individuals!U21:V22)</f>
         <v>153</v>
       </c>
-      <c r="L7" s="100">
+      <c r="L7" s="98">
         <f>SUM(Individuals!W12:X13,Individuals!W16:X16,Individuals!W18:X18,Individuals!W21:X22)</f>
         <v>0</v>
       </c>
-      <c r="M7" s="100">
+      <c r="M7" s="98">
         <f>SUM(Individuals!Y12:Z13,Individuals!Y16:Z16,Individuals!Y18:Z18,Individuals!Y21:Z22)</f>
         <v>0</v>
       </c>
-      <c r="N7" s="100">
+      <c r="N7" s="98">
         <f>SUM(Individuals!AA12:AB13,Individuals!AA16:AB16,Individuals!AA18:AB18,Individuals!AA21:AB22)</f>
         <v>0</v>
       </c>
       <c r="O7" s="1"/>
-      <c r="P7" s="100"/>
+      <c r="P7" s="98"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="100"/>
+      <c r="R7" s="98"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
@@ -5729,276 +5787,276 @@
       <c r="W7" s="1"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="97" t="s">
+      <c r="A8" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="98">
+      <c r="C8" s="96">
         <f>SUM(Individuals!E23:F23,Individuals!E25:F25)</f>
         <v>41</v>
       </c>
-      <c r="D8" s="98">
+      <c r="D8" s="96">
         <f>SUM(Individuals!G23:H23,Individuals!G25:H25)</f>
         <v>56</v>
       </c>
-      <c r="E8" s="98">
+      <c r="E8" s="96">
         <f>SUM(Individuals!I23:J23,Individuals!I25:J25)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="98">
+      <c r="F8" s="96">
         <f>SUM(Individuals!K23:L23,Individuals!K25:L25)</f>
         <v>402</v>
       </c>
-      <c r="G8" s="98">
+      <c r="G8" s="96">
         <f>SUM(Individuals!M23:N23,Individuals!M25:N25)</f>
         <v>1</v>
       </c>
-      <c r="H8" s="98">
+      <c r="H8" s="96">
         <f>SUM(Individuals!O23:P23,Individuals!O25:P25)</f>
         <v>8</v>
       </c>
-      <c r="I8" s="98">
+      <c r="I8" s="96">
         <f>SUM(Individuals!Q23:R23,Individuals!Q25:R25)</f>
-        <v>129</v>
-      </c>
-      <c r="J8" s="98">
+        <v>130</v>
+      </c>
+      <c r="J8" s="96">
         <f>SUM(Individuals!S23:T23,Individuals!S25:T25)</f>
-        <v>54</v>
-      </c>
-      <c r="K8" s="98">
+        <v>75</v>
+      </c>
+      <c r="K8" s="96">
         <f>SUM(Individuals!U23:V23,Individuals!U25:V25)</f>
         <v>0</v>
       </c>
-      <c r="L8" s="98">
+      <c r="L8" s="96">
         <f>SUM(Individuals!W23:X23,Individuals!W25:X25)</f>
         <v>60</v>
       </c>
-      <c r="M8" s="98">
+      <c r="M8" s="96">
         <f>SUM(Individuals!Y23:Z23,Individuals!Y25:Z25)</f>
         <v>43</v>
       </c>
-      <c r="N8" s="98">
+      <c r="N8" s="96">
         <f>SUM(Individuals!AA23:AB23,Individuals!AA25:AB25)</f>
         <v>0</v>
       </c>
       <c r="O8" s="1"/>
-      <c r="P8" s="100"/>
-      <c r="Q8" s="100"/>
-      <c r="R8" s="100"/>
-      <c r="S8" s="100"/>
-      <c r="T8" s="100"/>
-      <c r="U8" s="100"/>
-      <c r="V8" s="100"/>
-      <c r="W8" s="100"/>
+      <c r="P8" s="98"/>
+      <c r="Q8" s="98"/>
+      <c r="R8" s="98"/>
+      <c r="S8" s="98"/>
+      <c r="T8" s="98"/>
+      <c r="U8" s="98"/>
+      <c r="V8" s="98"/>
+      <c r="W8" s="98"/>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="97"/>
-      <c r="B9" s="100" t="s">
+      <c r="A9" s="95"/>
+      <c r="B9" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="100">
+      <c r="C9" s="98">
         <f>SUM(Individuals!E24:F24,Individuals!E26:F26)</f>
         <v>145</v>
       </c>
-      <c r="D9" s="100">
+      <c r="D9" s="98">
         <f>SUM(Individuals!G24:H24,Individuals!G26:H26)</f>
         <v>6</v>
       </c>
-      <c r="E9" s="100">
+      <c r="E9" s="98">
         <f>SUM(Individuals!I24:J24,Individuals!I26:J26)</f>
         <v>12</v>
       </c>
-      <c r="F9" s="100">
+      <c r="F9" s="98">
         <f>SUM(Individuals!K24:L24,Individuals!K26:L26)</f>
-        <v>3</v>
-      </c>
-      <c r="G9" s="100">
+        <v>54</v>
+      </c>
+      <c r="G9" s="98">
         <f>SUM(Individuals!M24:N24,Individuals!M26:N26)</f>
         <v>3</v>
       </c>
-      <c r="H9" s="100">
+      <c r="H9" s="98">
         <f>SUM(Individuals!O24:P24,Individuals!O26:P26)</f>
         <v>84</v>
       </c>
-      <c r="I9" s="100">
+      <c r="I9" s="98">
         <f>SUM(Individuals!Q24:R24,Individuals!Q26:R26)</f>
-        <v>121</v>
-      </c>
-      <c r="J9" s="100">
+        <v>131</v>
+      </c>
+      <c r="J9" s="98">
         <f>SUM(Individuals!S24:T24,Individuals!S26:T26)</f>
-        <v>28</v>
-      </c>
-      <c r="K9" s="100">
+        <v>38</v>
+      </c>
+      <c r="K9" s="98">
         <f>SUM(Individuals!U24:V24,Individuals!U26:V26)</f>
         <v>13</v>
       </c>
-      <c r="L9" s="100">
+      <c r="L9" s="98">
         <f>SUM(Individuals!W24:X24,Individuals!W26:X26)</f>
         <v>108</v>
       </c>
-      <c r="M9" s="100">
+      <c r="M9" s="98">
         <f>SUM(Individuals!Y24:Z24,Individuals!Y26:Z26)</f>
         <v>3</v>
       </c>
-      <c r="N9" s="100">
+      <c r="N9" s="98">
         <f>SUM(Individuals!AA24:AB24,Individuals!AA26:AB26)</f>
         <v>0</v>
       </c>
       <c r="O9" s="1"/>
-      <c r="P9" s="100"/>
-      <c r="Q9" s="100"/>
-      <c r="R9" s="100"/>
-      <c r="S9" s="100"/>
-      <c r="T9" s="100"/>
-      <c r="U9" s="100"/>
-      <c r="V9" s="100"/>
-      <c r="W9" s="100"/>
+      <c r="P9" s="98"/>
+      <c r="Q9" s="98"/>
+      <c r="R9" s="98"/>
+      <c r="S9" s="98"/>
+      <c r="T9" s="98"/>
+      <c r="U9" s="98"/>
+      <c r="V9" s="98"/>
+      <c r="W9" s="98"/>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="97" t="s">
+      <c r="A10" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="98" t="s">
+      <c r="B10" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="98">
+      <c r="C10" s="96">
         <f>SUM(Individuals!E27:F27,Individuals!E29:F30,Individuals!E33:F34)</f>
-        <v>161</v>
-      </c>
-      <c r="D10" s="98">
+        <v>298</v>
+      </c>
+      <c r="D10" s="96">
         <f>SUM(Individuals!G27:H27,Individuals!G29:H30,Individuals!G33:H34)</f>
         <v>81</v>
       </c>
-      <c r="E10" s="98">
+      <c r="E10" s="96">
         <f>SUM(Individuals!I27:J27,Individuals!I29:J30,Individuals!I33:J34)</f>
-        <v>137</v>
-      </c>
-      <c r="F10" s="98">
+        <v>178</v>
+      </c>
+      <c r="F10" s="96">
         <f>SUM(Individuals!K27:L27,Individuals!K29:L30,Individuals!K33:L34)</f>
         <v>29</v>
       </c>
-      <c r="G10" s="98">
+      <c r="G10" s="96">
         <f>SUM(Individuals!M27:N27,Individuals!M29:N30,Individuals!M33:N34)</f>
         <v>6</v>
       </c>
-      <c r="H10" s="98">
+      <c r="H10" s="96">
         <f>SUM(Individuals!O27:P27,Individuals!O29:P30,Individuals!O33:P34)</f>
         <v>44</v>
       </c>
-      <c r="I10" s="98">
+      <c r="I10" s="96">
         <f>SUM(Individuals!Q27:R27,Individuals!Q29:R30,Individuals!Q33:R34)</f>
         <v>151</v>
       </c>
-      <c r="J10" s="98">
+      <c r="J10" s="96">
         <f>SUM(Individuals!S27:T27,Individuals!S29:T30,Individuals!S33:T34)</f>
         <v>87</v>
       </c>
-      <c r="K10" s="98">
+      <c r="K10" s="96">
         <f>SUM(Individuals!U27:V27,Individuals!U29:V30,Individuals!U33:V34)</f>
         <v>89</v>
       </c>
-      <c r="L10" s="98">
+      <c r="L10" s="96">
         <f>SUM(Individuals!W27:X27,Individuals!W29:X30,Individuals!W33:X34)</f>
         <v>0</v>
       </c>
-      <c r="M10" s="98">
+      <c r="M10" s="96">
         <f>SUM(Individuals!Y27:Z27,Individuals!Y29:Z30,Individuals!Y33:Z34)</f>
         <v>0</v>
       </c>
-      <c r="N10" s="98">
+      <c r="N10" s="96">
         <f>SUM(Individuals!AA27:AB27,Individuals!AA29:AB30,Individuals!AA33:AB34)</f>
         <v>0</v>
       </c>
       <c r="O10" s="1"/>
-      <c r="P10" s="100"/>
-      <c r="Q10" s="100"/>
-      <c r="R10" s="100"/>
-      <c r="S10" s="100"/>
-      <c r="T10" s="100"/>
-      <c r="U10" s="100"/>
-      <c r="V10" s="100"/>
-      <c r="W10" s="100"/>
+      <c r="P10" s="98"/>
+      <c r="Q10" s="98"/>
+      <c r="R10" s="98"/>
+      <c r="S10" s="98"/>
+      <c r="T10" s="98"/>
+      <c r="U10" s="98"/>
+      <c r="V10" s="98"/>
+      <c r="W10" s="98"/>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="97"/>
-      <c r="B11" s="100" t="s">
+      <c r="A11" s="95"/>
+      <c r="B11" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="100">
+      <c r="C11" s="98">
         <f>SUM(Individuals!E28:F28,Individuals!E31:F32,Individuals!E35:F35)</f>
         <v>155</v>
       </c>
-      <c r="D11" s="100">
+      <c r="D11" s="98">
         <f>SUM(Individuals!G28:H28,Individuals!G31:H32,Individuals!G35:H35)</f>
         <v>103</v>
       </c>
-      <c r="E11" s="100">
+      <c r="E11" s="98">
         <f>SUM(Individuals!I28:J28,Individuals!I31:J32,Individuals!I35:J35)</f>
         <v>206</v>
       </c>
-      <c r="F11" s="100">
+      <c r="F11" s="98">
         <f>SUM(Individuals!K28:L28,Individuals!K31:L32,Individuals!K35:L35)</f>
         <v>125</v>
       </c>
-      <c r="G11" s="100">
+      <c r="G11" s="98">
         <f>SUM(Individuals!M28:N28,Individuals!M31:N32,Individuals!M35:N35)</f>
         <v>8</v>
       </c>
-      <c r="H11" s="100">
+      <c r="H11" s="98">
         <f>SUM(Individuals!O28:P28,Individuals!O31:P32,Individuals!O35:P35)</f>
         <v>131</v>
       </c>
-      <c r="I11" s="100">
+      <c r="I11" s="98">
         <f>SUM(Individuals!Q28:R28,Individuals!Q31:R32,Individuals!Q35:R35)</f>
-        <v>33</v>
-      </c>
-      <c r="J11" s="100">
+        <v>96</v>
+      </c>
+      <c r="J11" s="98">
         <f>SUM(Individuals!S28:T28,Individuals!S31:T32,Individuals!S35:T35)</f>
-        <v>6</v>
-      </c>
-      <c r="K11" s="100">
+        <v>28</v>
+      </c>
+      <c r="K11" s="98">
         <f>SUM(Individuals!U28:V28,Individuals!U31:V32,Individuals!U35:V35)</f>
         <v>88</v>
       </c>
-      <c r="L11" s="100">
+      <c r="L11" s="98">
         <f>SUM(Individuals!W28:X28,Individuals!W31:X32,Individuals!W35:X35)</f>
         <v>0</v>
       </c>
-      <c r="M11" s="100">
+      <c r="M11" s="98">
         <f>SUM(Individuals!Y28:Z28,Individuals!Y31:Z32,Individuals!Y35:Z35)</f>
         <v>0</v>
       </c>
-      <c r="N11" s="100">
+      <c r="N11" s="98">
         <f>SUM(Individuals!AA28:AB28,Individuals!AA31:AB32,Individuals!AA35:AB35)</f>
         <v>0</v>
       </c>
       <c r="O11" s="1"/>
-      <c r="P11" s="100"/>
-      <c r="Q11" s="100"/>
-      <c r="R11" s="100"/>
-      <c r="S11" s="100"/>
-      <c r="T11" s="100"/>
-      <c r="U11" s="100"/>
-      <c r="V11" s="100"/>
-      <c r="W11" s="100"/>
+      <c r="P11" s="98"/>
+      <c r="Q11" s="98"/>
+      <c r="R11" s="98"/>
+      <c r="S11" s="98"/>
+      <c r="T11" s="98"/>
+      <c r="U11" s="98"/>
+      <c r="V11" s="98"/>
+      <c r="W11" s="98"/>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="99"/>
-      <c r="B12" s="100"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="100"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="100"/>
-      <c r="H12" s="100"/>
-      <c r="I12" s="100"/>
-      <c r="J12" s="100"/>
-      <c r="K12" s="100"/>
-      <c r="L12" s="100"/>
-      <c r="M12" s="100"/>
-      <c r="N12" s="100"/>
+      <c r="A12" s="97"/>
+      <c r="B12" s="98"/>
+      <c r="C12" s="98"/>
+      <c r="D12" s="98"/>
+      <c r="E12" s="98"/>
+      <c r="F12" s="98"/>
+      <c r="G12" s="98"/>
+      <c r="H12" s="98"/>
+      <c r="I12" s="98"/>
+      <c r="J12" s="98"/>
+      <c r="K12" s="98"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
+      <c r="N12" s="98"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -6010,20 +6068,20 @@
       <c r="W12" s="1"/>
     </row>
     <row r="13" spans="1:23">
-      <c r="A13" s="99"/>
-      <c r="B13" s="100"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="100"/>
-      <c r="H13" s="100"/>
-      <c r="I13" s="100"/>
-      <c r="J13" s="100"/>
-      <c r="K13" s="100"/>
-      <c r="L13" s="100"/>
-      <c r="M13" s="100"/>
-      <c r="N13" s="100"/>
+      <c r="A13" s="97"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="98"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="98"/>
+      <c r="H13" s="98"/>
+      <c r="I13" s="98"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -6035,356 +6093,356 @@
       <c r="W13" s="1"/>
     </row>
     <row r="14" spans="1:23">
-      <c r="A14" s="99"/>
-      <c r="B14" s="100"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="100"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="100"/>
-      <c r="H14" s="100"/>
-      <c r="I14" s="100"/>
-      <c r="J14" s="100"/>
-      <c r="K14" s="100"/>
-      <c r="L14" s="100"/>
-      <c r="M14" s="100"/>
-      <c r="N14" s="100"/>
+      <c r="A14" s="97"/>
+      <c r="B14" s="98"/>
+      <c r="C14" s="98"/>
+      <c r="D14" s="98"/>
+      <c r="E14" s="98"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="98"/>
+      <c r="H14" s="98"/>
+      <c r="I14" s="98"/>
+      <c r="J14" s="98"/>
+      <c r="K14" s="98"/>
+      <c r="L14" s="98"/>
+      <c r="M14" s="98"/>
+      <c r="N14" s="98"/>
     </row>
     <row r="15" spans="1:23">
-      <c r="A15" s="99"/>
-      <c r="B15" s="100"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="100"/>
-      <c r="F15" s="100"/>
-      <c r="G15" s="100"/>
-      <c r="H15" s="100"/>
-      <c r="I15" s="100"/>
-      <c r="J15" s="100"/>
-      <c r="K15" s="100"/>
-      <c r="L15" s="100"/>
-      <c r="M15" s="100"/>
-      <c r="N15" s="100"/>
+      <c r="A15" s="97"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="98"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="99"/>
-      <c r="B16" s="100"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="100"/>
-      <c r="E16" s="100"/>
-      <c r="F16" s="100"/>
-      <c r="G16" s="100"/>
-      <c r="H16" s="100"/>
-      <c r="I16" s="100"/>
-      <c r="J16" s="100"/>
-      <c r="K16" s="100"/>
-      <c r="L16" s="100"/>
-      <c r="M16" s="100"/>
-      <c r="N16" s="100"/>
+      <c r="A16" s="97"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="98"/>
+      <c r="J16" s="98"/>
+      <c r="K16" s="98"/>
+      <c r="L16" s="98"/>
+      <c r="M16" s="98"/>
+      <c r="N16" s="98"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="99"/>
-      <c r="B17" s="100"/>
-      <c r="C17" s="100"/>
-      <c r="D17" s="100"/>
-      <c r="E17" s="100"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="100"/>
-      <c r="H17" s="100"/>
-      <c r="I17" s="100"/>
-      <c r="J17" s="100"/>
-      <c r="K17" s="100"/>
-      <c r="L17" s="100"/>
-      <c r="M17" s="100"/>
-      <c r="N17" s="100"/>
+      <c r="A17" s="97"/>
+      <c r="B17" s="98"/>
+      <c r="C17" s="98"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="98"/>
+      <c r="F17" s="98"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="98"/>
+      <c r="I17" s="98"/>
+      <c r="J17" s="98"/>
+      <c r="K17" s="98"/>
+      <c r="L17" s="98"/>
+      <c r="M17" s="98"/>
+      <c r="N17" s="98"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="99"/>
-      <c r="B18" s="100"/>
-      <c r="C18" s="100"/>
-      <c r="D18" s="100"/>
-      <c r="E18" s="100"/>
-      <c r="F18" s="100"/>
-      <c r="G18" s="100"/>
-      <c r="H18" s="100"/>
-      <c r="I18" s="100"/>
-      <c r="J18" s="100"/>
-      <c r="K18" s="100"/>
-      <c r="L18" s="100"/>
-      <c r="M18" s="100"/>
-      <c r="N18" s="100"/>
+      <c r="A18" s="97"/>
+      <c r="B18" s="98"/>
+      <c r="C18" s="98"/>
+      <c r="D18" s="98"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="98"/>
+      <c r="J18" s="98"/>
+      <c r="K18" s="98"/>
+      <c r="L18" s="98"/>
+      <c r="M18" s="98"/>
+      <c r="N18" s="98"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="99"/>
-      <c r="B19" s="100"/>
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="100"/>
-      <c r="H19" s="100"/>
-      <c r="I19" s="100"/>
-      <c r="J19" s="100"/>
-      <c r="K19" s="100"/>
-      <c r="L19" s="100"/>
-      <c r="M19" s="100"/>
-      <c r="N19" s="100"/>
+      <c r="A19" s="97"/>
+      <c r="B19" s="98"/>
+      <c r="C19" s="98"/>
+      <c r="D19" s="98"/>
+      <c r="E19" s="98"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="98"/>
+      <c r="H19" s="98"/>
+      <c r="I19" s="98"/>
+      <c r="J19" s="98"/>
+      <c r="K19" s="98"/>
+      <c r="L19" s="98"/>
+      <c r="M19" s="98"/>
+      <c r="N19" s="98"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="99"/>
-      <c r="B20" s="100"/>
-      <c r="C20" s="100"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="100"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="100"/>
-      <c r="H20" s="100"/>
-      <c r="I20" s="100"/>
-      <c r="J20" s="100"/>
-      <c r="K20" s="100"/>
-      <c r="L20" s="100"/>
-      <c r="M20" s="100"/>
-      <c r="N20" s="100"/>
+      <c r="A20" s="97"/>
+      <c r="B20" s="98"/>
+      <c r="C20" s="98"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="98"/>
+      <c r="F20" s="98"/>
+      <c r="G20" s="98"/>
+      <c r="H20" s="98"/>
+      <c r="I20" s="98"/>
+      <c r="J20" s="98"/>
+      <c r="K20" s="98"/>
+      <c r="L20" s="98"/>
+      <c r="M20" s="98"/>
+      <c r="N20" s="98"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="99"/>
-      <c r="B21" s="100"/>
-      <c r="C21" s="100"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="100"/>
-      <c r="H21" s="100"/>
-      <c r="I21" s="100"/>
-      <c r="J21" s="100"/>
-      <c r="K21" s="100"/>
-      <c r="L21" s="100"/>
-      <c r="M21" s="100"/>
-      <c r="N21" s="100"/>
+      <c r="A21" s="97"/>
+      <c r="B21" s="98"/>
+      <c r="C21" s="98"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="98"/>
+      <c r="G21" s="98"/>
+      <c r="H21" s="98"/>
+      <c r="I21" s="98"/>
+      <c r="J21" s="98"/>
+      <c r="K21" s="98"/>
+      <c r="L21" s="98"/>
+      <c r="M21" s="98"/>
+      <c r="N21" s="98"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="99"/>
-      <c r="B22" s="100"/>
-      <c r="C22" s="100"/>
-      <c r="D22" s="100"/>
-      <c r="E22" s="100"/>
-      <c r="F22" s="100"/>
-      <c r="G22" s="100"/>
-      <c r="H22" s="100"/>
-      <c r="I22" s="100"/>
-      <c r="J22" s="100"/>
-      <c r="K22" s="100"/>
-      <c r="L22" s="100"/>
-      <c r="M22" s="100"/>
-      <c r="N22" s="100"/>
+      <c r="A22" s="97"/>
+      <c r="B22" s="98"/>
+      <c r="C22" s="98"/>
+      <c r="D22" s="98"/>
+      <c r="E22" s="98"/>
+      <c r="F22" s="98"/>
+      <c r="G22" s="98"/>
+      <c r="H22" s="98"/>
+      <c r="I22" s="98"/>
+      <c r="J22" s="98"/>
+      <c r="K22" s="98"/>
+      <c r="L22" s="98"/>
+      <c r="M22" s="98"/>
+      <c r="N22" s="98"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="99"/>
-      <c r="B23" s="100"/>
-      <c r="C23" s="100"/>
-      <c r="D23" s="100"/>
-      <c r="E23" s="100"/>
-      <c r="F23" s="100"/>
-      <c r="G23" s="100"/>
-      <c r="H23" s="100"/>
-      <c r="I23" s="100"/>
-      <c r="J23" s="100"/>
-      <c r="K23" s="100"/>
-      <c r="L23" s="100"/>
-      <c r="M23" s="100"/>
-      <c r="N23" s="100"/>
+      <c r="A23" s="97"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="98"/>
+      <c r="D23" s="98"/>
+      <c r="E23" s="98"/>
+      <c r="F23" s="98"/>
+      <c r="G23" s="98"/>
+      <c r="H23" s="98"/>
+      <c r="I23" s="98"/>
+      <c r="J23" s="98"/>
+      <c r="K23" s="98"/>
+      <c r="L23" s="98"/>
+      <c r="M23" s="98"/>
+      <c r="N23" s="98"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="99"/>
-      <c r="B24" s="100"/>
-      <c r="C24" s="100"/>
-      <c r="D24" s="100"/>
-      <c r="E24" s="100"/>
-      <c r="F24" s="100"/>
-      <c r="G24" s="100"/>
-      <c r="H24" s="100"/>
-      <c r="I24" s="100"/>
-      <c r="J24" s="100"/>
-      <c r="K24" s="100"/>
-      <c r="L24" s="100"/>
-      <c r="M24" s="100"/>
-      <c r="N24" s="100"/>
+      <c r="A24" s="97"/>
+      <c r="B24" s="98"/>
+      <c r="C24" s="98"/>
+      <c r="D24" s="98"/>
+      <c r="E24" s="98"/>
+      <c r="F24" s="98"/>
+      <c r="G24" s="98"/>
+      <c r="H24" s="98"/>
+      <c r="I24" s="98"/>
+      <c r="J24" s="98"/>
+      <c r="K24" s="98"/>
+      <c r="L24" s="98"/>
+      <c r="M24" s="98"/>
+      <c r="N24" s="98"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="99"/>
-      <c r="B25" s="100"/>
-      <c r="C25" s="100"/>
-      <c r="D25" s="100"/>
-      <c r="E25" s="100"/>
-      <c r="F25" s="100"/>
-      <c r="G25" s="100"/>
-      <c r="H25" s="100"/>
-      <c r="I25" s="100"/>
-      <c r="J25" s="100"/>
-      <c r="K25" s="100"/>
-      <c r="L25" s="100"/>
-      <c r="M25" s="100"/>
-      <c r="N25" s="100"/>
+      <c r="A25" s="97"/>
+      <c r="B25" s="98"/>
+      <c r="C25" s="98"/>
+      <c r="D25" s="98"/>
+      <c r="E25" s="98"/>
+      <c r="F25" s="98"/>
+      <c r="G25" s="98"/>
+      <c r="H25" s="98"/>
+      <c r="I25" s="98"/>
+      <c r="J25" s="98"/>
+      <c r="K25" s="98"/>
+      <c r="L25" s="98"/>
+      <c r="M25" s="98"/>
+      <c r="N25" s="98"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="99"/>
-      <c r="B26" s="100"/>
-      <c r="C26" s="100"/>
-      <c r="D26" s="100"/>
-      <c r="E26" s="100"/>
-      <c r="F26" s="100"/>
-      <c r="G26" s="100"/>
-      <c r="H26" s="100"/>
-      <c r="I26" s="100"/>
-      <c r="J26" s="100"/>
-      <c r="K26" s="100"/>
-      <c r="L26" s="100"/>
-      <c r="M26" s="100"/>
-      <c r="N26" s="100"/>
+      <c r="A26" s="97"/>
+      <c r="B26" s="98"/>
+      <c r="C26" s="98"/>
+      <c r="D26" s="98"/>
+      <c r="E26" s="98"/>
+      <c r="F26" s="98"/>
+      <c r="G26" s="98"/>
+      <c r="H26" s="98"/>
+      <c r="I26" s="98"/>
+      <c r="J26" s="98"/>
+      <c r="K26" s="98"/>
+      <c r="L26" s="98"/>
+      <c r="M26" s="98"/>
+      <c r="N26" s="98"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="99"/>
-      <c r="B27" s="100"/>
-      <c r="C27" s="100"/>
-      <c r="D27" s="100"/>
-      <c r="E27" s="100"/>
-      <c r="F27" s="100"/>
-      <c r="G27" s="100"/>
-      <c r="H27" s="100"/>
-      <c r="I27" s="100"/>
-      <c r="J27" s="100"/>
-      <c r="K27" s="100"/>
-      <c r="L27" s="100"/>
-      <c r="M27" s="100"/>
-      <c r="N27" s="100"/>
+      <c r="A27" s="97"/>
+      <c r="B27" s="98"/>
+      <c r="C27" s="98"/>
+      <c r="D27" s="98"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="98"/>
+      <c r="H27" s="98"/>
+      <c r="I27" s="98"/>
+      <c r="J27" s="98"/>
+      <c r="K27" s="98"/>
+      <c r="L27" s="98"/>
+      <c r="M27" s="98"/>
+      <c r="N27" s="98"/>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="99"/>
-      <c r="B28" s="100"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="100"/>
-      <c r="E28" s="100"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="100"/>
-      <c r="H28" s="100"/>
-      <c r="I28" s="100"/>
-      <c r="J28" s="100"/>
-      <c r="K28" s="100"/>
-      <c r="L28" s="100"/>
-      <c r="M28" s="100"/>
-      <c r="N28" s="100"/>
+      <c r="A28" s="97"/>
+      <c r="B28" s="98"/>
+      <c r="C28" s="98"/>
+      <c r="D28" s="98"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="98"/>
+      <c r="H28" s="98"/>
+      <c r="I28" s="98"/>
+      <c r="J28" s="98"/>
+      <c r="K28" s="98"/>
+      <c r="L28" s="98"/>
+      <c r="M28" s="98"/>
+      <c r="N28" s="98"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="99"/>
-      <c r="B29" s="100"/>
-      <c r="C29" s="100"/>
-      <c r="D29" s="100"/>
-      <c r="E29" s="100"/>
-      <c r="F29" s="100"/>
-      <c r="G29" s="100"/>
-      <c r="H29" s="100"/>
-      <c r="I29" s="100"/>
-      <c r="J29" s="100"/>
-      <c r="K29" s="100"/>
-      <c r="L29" s="100"/>
-      <c r="M29" s="100"/>
-      <c r="N29" s="100"/>
+      <c r="A29" s="97"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="98"/>
+      <c r="D29" s="98"/>
+      <c r="E29" s="98"/>
+      <c r="F29" s="98"/>
+      <c r="G29" s="98"/>
+      <c r="H29" s="98"/>
+      <c r="I29" s="98"/>
+      <c r="J29" s="98"/>
+      <c r="K29" s="98"/>
+      <c r="L29" s="98"/>
+      <c r="M29" s="98"/>
+      <c r="N29" s="98"/>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="99"/>
-      <c r="B30" s="100"/>
-      <c r="C30" s="100"/>
-      <c r="D30" s="100"/>
-      <c r="E30" s="100"/>
-      <c r="F30" s="100"/>
-      <c r="G30" s="100"/>
-      <c r="H30" s="100"/>
-      <c r="I30" s="100"/>
-      <c r="J30" s="100"/>
-      <c r="K30" s="100"/>
-      <c r="L30" s="100"/>
-      <c r="M30" s="100"/>
-      <c r="N30" s="100"/>
+      <c r="A30" s="97"/>
+      <c r="B30" s="98"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="98"/>
+      <c r="F30" s="98"/>
+      <c r="G30" s="98"/>
+      <c r="H30" s="98"/>
+      <c r="I30" s="98"/>
+      <c r="J30" s="98"/>
+      <c r="K30" s="98"/>
+      <c r="L30" s="98"/>
+      <c r="M30" s="98"/>
+      <c r="N30" s="98"/>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="99"/>
-      <c r="B31" s="100"/>
-      <c r="C31" s="100"/>
-      <c r="D31" s="100"/>
-      <c r="E31" s="100"/>
-      <c r="F31" s="100"/>
-      <c r="G31" s="100"/>
-      <c r="H31" s="100"/>
-      <c r="I31" s="100"/>
-      <c r="J31" s="100"/>
-      <c r="K31" s="100"/>
-      <c r="L31" s="100"/>
-      <c r="M31" s="100"/>
-      <c r="N31" s="100"/>
+      <c r="A31" s="97"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="98"/>
+      <c r="D31" s="98"/>
+      <c r="E31" s="98"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="98"/>
+      <c r="I31" s="98"/>
+      <c r="J31" s="98"/>
+      <c r="K31" s="98"/>
+      <c r="L31" s="98"/>
+      <c r="M31" s="98"/>
+      <c r="N31" s="98"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="99"/>
-      <c r="B32" s="100"/>
-      <c r="C32" s="100"/>
-      <c r="D32" s="100"/>
-      <c r="E32" s="100"/>
-      <c r="F32" s="100"/>
-      <c r="G32" s="100"/>
-      <c r="H32" s="100"/>
-      <c r="I32" s="100"/>
-      <c r="J32" s="100"/>
-      <c r="K32" s="100"/>
-      <c r="L32" s="100"/>
-      <c r="M32" s="100"/>
-      <c r="N32" s="100"/>
+      <c r="A32" s="97"/>
+      <c r="B32" s="98"/>
+      <c r="C32" s="98"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="98"/>
+      <c r="G32" s="98"/>
+      <c r="H32" s="98"/>
+      <c r="I32" s="98"/>
+      <c r="J32" s="98"/>
+      <c r="K32" s="98"/>
+      <c r="L32" s="98"/>
+      <c r="M32" s="98"/>
+      <c r="N32" s="98"/>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="99"/>
-      <c r="B33" s="100"/>
-      <c r="C33" s="100"/>
-      <c r="D33" s="100"/>
-      <c r="E33" s="100"/>
-      <c r="F33" s="100"/>
-      <c r="G33" s="100"/>
-      <c r="H33" s="100"/>
-      <c r="I33" s="100"/>
-      <c r="J33" s="100"/>
-      <c r="K33" s="100"/>
-      <c r="L33" s="100"/>
-      <c r="M33" s="100"/>
-      <c r="N33" s="100"/>
+      <c r="A33" s="97"/>
+      <c r="B33" s="98"/>
+      <c r="C33" s="98"/>
+      <c r="D33" s="98"/>
+      <c r="E33" s="98"/>
+      <c r="F33" s="98"/>
+      <c r="G33" s="98"/>
+      <c r="H33" s="98"/>
+      <c r="I33" s="98"/>
+      <c r="J33" s="98"/>
+      <c r="K33" s="98"/>
+      <c r="L33" s="98"/>
+      <c r="M33" s="98"/>
+      <c r="N33" s="98"/>
     </row>
     <row r="34" spans="1:14">
-      <c r="A34" s="99"/>
-      <c r="B34" s="100"/>
-      <c r="C34" s="100"/>
-      <c r="D34" s="100"/>
-      <c r="E34" s="100"/>
-      <c r="F34" s="100"/>
-      <c r="G34" s="100"/>
-      <c r="H34" s="100"/>
-      <c r="I34" s="100"/>
-      <c r="J34" s="100"/>
-      <c r="K34" s="100"/>
-      <c r="L34" s="100"/>
-      <c r="M34" s="100"/>
-      <c r="N34" s="100"/>
+      <c r="A34" s="97"/>
+      <c r="B34" s="98"/>
+      <c r="C34" s="98"/>
+      <c r="D34" s="98"/>
+      <c r="E34" s="98"/>
+      <c r="F34" s="98"/>
+      <c r="G34" s="98"/>
+      <c r="H34" s="98"/>
+      <c r="I34" s="98"/>
+      <c r="J34" s="98"/>
+      <c r="K34" s="98"/>
+      <c r="L34" s="98"/>
+      <c r="M34" s="98"/>
+      <c r="N34" s="98"/>
     </row>
     <row r="35" spans="1:14" s="1" customFormat="1">
-      <c r="A35" s="100"/>
-      <c r="B35" s="100"/>
-      <c r="C35" s="100"/>
-      <c r="D35" s="100"/>
-      <c r="E35" s="100"/>
-      <c r="F35" s="100"/>
-      <c r="G35" s="100"/>
-      <c r="H35" s="100"/>
-      <c r="I35" s="100"/>
-      <c r="J35" s="100"/>
-      <c r="K35" s="100"/>
-      <c r="L35" s="100"/>
-      <c r="M35" s="100"/>
-      <c r="N35" s="100"/>
+      <c r="A35" s="98"/>
+      <c r="B35" s="98"/>
+      <c r="C35" s="98"/>
+      <c r="D35" s="98"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="98"/>
+      <c r="H35" s="98"/>
+      <c r="I35" s="98"/>
+      <c r="J35" s="98"/>
+      <c r="K35" s="98"/>
+      <c r="L35" s="98"/>
+      <c r="M35" s="98"/>
+      <c r="N35" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
Save sample table with new regional summary lumping onshore and offshore.
</commit_message>
<xml_diff>
--- a/data/sampleTable.xlsx
+++ b/data/sampleTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17480" windowHeight="21140" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20560" windowHeight="21140" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="31">
   <si>
     <t>Year</t>
   </si>
@@ -348,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -570,8 +570,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -663,8 +674,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -761,81 +780,6 @@
     <xf numFmtId="0" fontId="13" fillId="17" borderId="8" xfId="22" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="10" xfId="22" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="11" xfId="22" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -843,12 +787,6 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -866,8 +804,98 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="99">
     <cellStyle name="Bad" xfId="22" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -912,6 +940,10 @@
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="21" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -956,6 +988,10 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="23" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="24" builtinId="21"/>
@@ -1304,34 +1340,34 @@
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64">
+      <c r="B1" s="76">
         <v>2015</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="66">
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="78">
         <v>2016</v>
       </c>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="67">
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="79">
         <v>2017</v>
       </c>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="68">
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="80">
         <v>2018</v>
       </c>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
     </row>
     <row r="2" spans="1:21" s="2" customFormat="1" ht="36">
       <c r="A2" s="6" t="s">
@@ -1634,97 +1670,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="15" customFormat="1" ht="25">
-      <c r="B1" s="83" t="s">
+      <c r="B1" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="69">
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="92">
         <v>2015</v>
       </c>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="71">
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="94">
         <v>2016</v>
       </c>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="73">
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="88">
         <v>2017</v>
       </c>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="75">
+      <c r="R1" s="88"/>
+      <c r="S1" s="88"/>
+      <c r="T1" s="88"/>
+      <c r="U1" s="88"/>
+      <c r="V1" s="88"/>
+      <c r="W1" s="90">
         <v>2018</v>
       </c>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="75"/>
-      <c r="AA1" s="75"/>
-      <c r="AB1" s="75"/>
+      <c r="X1" s="90"/>
+      <c r="Y1" s="90"/>
+      <c r="Z1" s="90"/>
+      <c r="AA1" s="90"/>
+      <c r="AB1" s="90"/>
       <c r="AC1" s="13"/>
     </row>
     <row r="2" spans="1:29" s="16" customFormat="1" ht="23">
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="70" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70" t="s">
+      <c r="F2" s="93"/>
+      <c r="G2" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70" t="s">
+      <c r="H2" s="93"/>
+      <c r="I2" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="70"/>
-      <c r="K2" s="72" t="s">
+      <c r="J2" s="93"/>
+      <c r="K2" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72" t="s">
+      <c r="L2" s="95"/>
+      <c r="M2" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72" t="s">
+      <c r="N2" s="95"/>
+      <c r="O2" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="74" t="s">
+      <c r="P2" s="95"/>
+      <c r="Q2" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="74"/>
-      <c r="S2" s="74" t="s">
+      <c r="R2" s="89"/>
+      <c r="S2" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="74"/>
-      <c r="U2" s="74" t="s">
+      <c r="T2" s="89"/>
+      <c r="U2" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="74"/>
-      <c r="W2" s="76" t="s">
+      <c r="V2" s="89"/>
+      <c r="W2" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="76"/>
-      <c r="Y2" s="76" t="s">
+      <c r="X2" s="91"/>
+      <c r="Y2" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="Z2" s="76"/>
-      <c r="AA2" s="76" t="s">
+      <c r="Z2" s="91"/>
+      <c r="AA2" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="76"/>
+      <c r="AB2" s="91"/>
       <c r="AC2" s="14"/>
     </row>
     <row r="3" spans="1:29" s="22" customFormat="1" ht="20">
@@ -1815,13 +1851,13 @@
       <c r="AC3" s="21"/>
     </row>
     <row r="4" spans="1:29">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="79" t="s">
+      <c r="C4" s="82" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="23">
@@ -1877,9 +1913,9 @@
       <c r="AB4" s="24"/>
     </row>
     <row r="5" spans="1:29">
-      <c r="A5" s="77"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="79"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="82"/>
       <c r="D5" s="23">
         <v>183</v>
       </c>
@@ -1909,8 +1945,8 @@
       <c r="AB5" s="24"/>
     </row>
     <row r="6" spans="1:29">
-      <c r="A6" s="77"/>
-      <c r="B6" s="77"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="83"/>
       <c r="C6" s="25" t="s">
         <v>3</v>
       </c>
@@ -1967,8 +2003,8 @@
       <c r="AB6" s="26"/>
     </row>
     <row r="7" spans="1:29">
-      <c r="A7" s="77"/>
-      <c r="B7" s="77" t="s">
+      <c r="A7" s="83"/>
+      <c r="B7" s="83" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="23" t="s">
@@ -2003,9 +2039,9 @@
       <c r="AB7" s="24"/>
     </row>
     <row r="8" spans="1:29">
-      <c r="A8" s="77"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77" t="s">
+      <c r="A8" s="83"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="25">
@@ -2061,9 +2097,9 @@
       </c>
     </row>
     <row r="9" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="84"/>
+      <c r="C9" s="84"/>
       <c r="D9" s="29">
         <v>171</v>
       </c>
@@ -2094,13 +2130,13 @@
       <c r="AC9" s="31"/>
     </row>
     <row r="10" spans="1:29" ht="16" thickTop="1">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="82" t="s">
+      <c r="C10" s="87" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="27">
@@ -2132,9 +2168,9 @@
       <c r="AB10" s="28"/>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="77"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="23">
         <v>139</v>
       </c>
@@ -2164,9 +2200,9 @@
       <c r="AB11" s="24"/>
     </row>
     <row r="12" spans="1:29">
-      <c r="A12" s="77"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="77" t="s">
+      <c r="A12" s="83"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="25">
@@ -2198,9 +2234,9 @@
       <c r="AB12" s="26"/>
     </row>
     <row r="13" spans="1:29">
-      <c r="A13" s="77"/>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="83"/>
       <c r="D13" s="25">
         <v>156</v>
       </c>
@@ -2230,11 +2266,11 @@
       <c r="AB13" s="26"/>
     </row>
     <row r="14" spans="1:29">
-      <c r="A14" s="77"/>
-      <c r="B14" s="77" t="s">
+      <c r="A14" s="83"/>
+      <c r="B14" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="82" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="23">
@@ -2266,9 +2302,9 @@
       <c r="AB14" s="24"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="A15" s="77"/>
-      <c r="B15" s="77"/>
-      <c r="C15" s="79"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="82"/>
       <c r="D15" s="23">
         <v>132</v>
       </c>
@@ -2298,8 +2334,8 @@
       <c r="AB15" s="24"/>
     </row>
     <row r="16" spans="1:29">
-      <c r="A16" s="77"/>
-      <c r="B16" s="77"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="25" t="s">
         <v>3</v>
       </c>
@@ -2356,8 +2392,8 @@
       <c r="AB16" s="26"/>
     </row>
     <row r="17" spans="1:29">
-      <c r="A17" s="77"/>
-      <c r="B17" s="77" t="s">
+      <c r="A17" s="83"/>
+      <c r="B17" s="83" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="23" t="s">
@@ -2404,8 +2440,8 @@
       <c r="AB17" s="24"/>
     </row>
     <row r="18" spans="1:29">
-      <c r="A18" s="77"/>
-      <c r="B18" s="77"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="83"/>
       <c r="C18" s="25" t="s">
         <v>3</v>
       </c>
@@ -2462,11 +2498,11 @@
       <c r="AB18" s="26"/>
     </row>
     <row r="19" spans="1:29">
-      <c r="A19" s="77"/>
-      <c r="B19" s="77" t="s">
+      <c r="A19" s="83"/>
+      <c r="B19" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="79" t="s">
+      <c r="C19" s="82" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="23">
@@ -2510,9 +2546,9 @@
       <c r="AB19" s="24"/>
     </row>
     <row r="20" spans="1:29">
-      <c r="A20" s="77"/>
-      <c r="B20" s="77"/>
-      <c r="C20" s="79"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="82"/>
       <c r="D20" s="23">
         <v>112</v>
       </c>
@@ -2554,9 +2590,9 @@
       <c r="AB20" s="24"/>
     </row>
     <row r="21" spans="1:29">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77" t="s">
+      <c r="A21" s="83"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="83" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="25">
@@ -2600,9 +2636,9 @@
       <c r="AB21" s="26"/>
     </row>
     <row r="22" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A22" s="78"/>
-      <c r="B22" s="78"/>
-      <c r="C22" s="78"/>
+      <c r="A22" s="84"/>
+      <c r="B22" s="84"/>
+      <c r="C22" s="84"/>
       <c r="D22" s="29">
         <v>117</v>
       </c>
@@ -2657,10 +2693,10 @@
       <c r="AC22" s="31"/>
     </row>
     <row r="23" spans="1:29" ht="16" thickTop="1">
-      <c r="A23" s="80" t="s">
+      <c r="A23" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="80" t="s">
+      <c r="B23" s="85" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="35" t="s">
@@ -2743,8 +2779,8 @@
       </c>
     </row>
     <row r="24" spans="1:29">
-      <c r="A24" s="77"/>
-      <c r="B24" s="77"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="83"/>
       <c r="C24" s="25" t="s">
         <v>3</v>
       </c>
@@ -2801,8 +2837,8 @@
       <c r="AB24" s="26"/>
     </row>
     <row r="25" spans="1:29">
-      <c r="A25" s="77"/>
-      <c r="B25" s="77" t="s">
+      <c r="A25" s="83"/>
+      <c r="B25" s="83" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="23" t="s">
@@ -2849,8 +2885,8 @@
       <c r="AB25" s="24"/>
     </row>
     <row r="26" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A26" s="78"/>
-      <c r="B26" s="78"/>
+      <c r="A26" s="84"/>
+      <c r="B26" s="84"/>
       <c r="C26" s="29" t="s">
         <v>3</v>
       </c>
@@ -2932,10 +2968,10 @@
       <c r="AC26" s="31"/>
     </row>
     <row r="27" spans="1:29" ht="16" thickTop="1">
-      <c r="A27" s="81" t="s">
+      <c r="A27" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="81" t="s">
+      <c r="B27" s="86" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="27" t="s">
@@ -3006,8 +3042,8 @@
       <c r="AB27" s="28"/>
     </row>
     <row r="28" spans="1:29">
-      <c r="A28" s="77"/>
-      <c r="B28" s="77"/>
+      <c r="A28" s="83"/>
+      <c r="B28" s="83"/>
       <c r="C28" s="25" t="s">
         <v>3</v>
       </c>
@@ -3076,11 +3112,11 @@
       <c r="AB28" s="26"/>
     </row>
     <row r="29" spans="1:29">
-      <c r="A29" s="77"/>
-      <c r="B29" s="77" t="s">
+      <c r="A29" s="83"/>
+      <c r="B29" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="79" t="s">
+      <c r="C29" s="82" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="23">
@@ -3136,9 +3172,9 @@
       <c r="AB29" s="24"/>
     </row>
     <row r="30" spans="1:29">
-      <c r="A30" s="77"/>
-      <c r="B30" s="77"/>
-      <c r="C30" s="79"/>
+      <c r="A30" s="83"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="82"/>
       <c r="D30" s="23">
         <v>412</v>
       </c>
@@ -3168,9 +3204,9 @@
       <c r="AB30" s="24"/>
     </row>
     <row r="31" spans="1:29">
-      <c r="A31" s="77"/>
-      <c r="B31" s="77"/>
-      <c r="C31" s="77" t="s">
+      <c r="A31" s="83"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="83" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="25">
@@ -3214,9 +3250,9 @@
       <c r="AB31" s="26"/>
     </row>
     <row r="32" spans="1:29">
-      <c r="A32" s="77"/>
-      <c r="B32" s="77"/>
-      <c r="C32" s="77"/>
+      <c r="A32" s="83"/>
+      <c r="B32" s="83"/>
+      <c r="C32" s="83"/>
       <c r="D32" s="25">
         <v>414</v>
       </c>
@@ -3258,11 +3294,11 @@
       <c r="AB32" s="26"/>
     </row>
     <row r="33" spans="1:29">
-      <c r="A33" s="77"/>
-      <c r="B33" s="77" t="s">
+      <c r="A33" s="83"/>
+      <c r="B33" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="79" t="s">
+      <c r="C33" s="82" t="s">
         <v>2</v>
       </c>
       <c r="D33" s="23">
@@ -3306,9 +3342,9 @@
       <c r="AB33" s="24"/>
     </row>
     <row r="34" spans="1:29">
-      <c r="A34" s="77"/>
-      <c r="B34" s="77"/>
-      <c r="C34" s="79"/>
+      <c r="A34" s="83"/>
+      <c r="B34" s="83"/>
+      <c r="C34" s="82"/>
       <c r="D34" s="23">
         <v>482</v>
       </c>
@@ -3362,8 +3398,8 @@
       <c r="AB34" s="24"/>
     </row>
     <row r="35" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A35" s="78"/>
-      <c r="B35" s="78"/>
+      <c r="A35" s="84"/>
+      <c r="B35" s="84"/>
       <c r="C35" s="29" t="s">
         <v>3</v>
       </c>
@@ -3423,12 +3459,27 @@
     <row r="36" spans="1:29" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W1:AB1"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B7:B9"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A27:A35"/>
     <mergeCell ref="C21:C22"/>
@@ -3444,27 +3495,12 @@
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W1:AB1"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K1:P1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B33:B35"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3480,11 +3516,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L43" sqref="L43"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3493,39 +3529,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="48" customHeight="1">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
     </row>
     <row r="2" spans="1:15" ht="25">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
-      <c r="D2" s="84">
+      <c r="D2" s="96">
         <v>2015</v>
       </c>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="85">
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="97">
         <v>2016</v>
       </c>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="86">
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="98">
         <v>2017</v>
       </c>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="87">
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="99">
         <v>2018</v>
       </c>
-      <c r="N2" s="87"/>
-      <c r="O2" s="87"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
     </row>
     <row r="3" spans="1:15" ht="23">
       <c r="A3" s="36" t="s">
@@ -3575,10 +3611,10 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="82" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="23">
@@ -3634,8 +3670,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A5" s="77"/>
-      <c r="B5" s="79"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="82"/>
       <c r="C5" s="42">
         <v>183</v>
       </c>
@@ -3689,7 +3725,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A6" s="77"/>
+      <c r="A6" s="83"/>
       <c r="B6" s="44" t="s">
         <v>3</v>
       </c>
@@ -3746,7 +3782,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="83" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="45" t="s">
@@ -3805,8 +3841,8 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="16" thickTop="1">
-      <c r="A8" s="77"/>
-      <c r="B8" s="77" t="s">
+      <c r="A8" s="83"/>
+      <c r="B8" s="83" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="33">
@@ -3862,8 +3898,8 @@
       </c>
     </row>
     <row r="9" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A9" s="77"/>
-      <c r="B9" s="77"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="34">
         <v>171</v>
       </c>
@@ -3917,10 +3953,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="16" thickTop="1">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="79" t="s">
+      <c r="B10" s="82" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="27">
@@ -3976,8 +4012,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A11" s="77"/>
-      <c r="B11" s="79"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="42">
         <v>139</v>
       </c>
@@ -4031,8 +4067,8 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="16" thickTop="1">
-      <c r="A12" s="77"/>
-      <c r="B12" s="77" t="s">
+      <c r="A12" s="83"/>
+      <c r="B12" s="83" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="33">
@@ -4088,8 +4124,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A13" s="77"/>
-      <c r="B13" s="77"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="34">
         <v>156</v>
       </c>
@@ -4143,10 +4179,10 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" thickTop="1">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="82" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="27">
@@ -4202,8 +4238,8 @@
       </c>
     </row>
     <row r="15" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A15" s="77"/>
-      <c r="B15" s="79"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="82"/>
       <c r="C15" s="42">
         <v>132</v>
       </c>
@@ -4257,7 +4293,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A16" s="77"/>
+      <c r="A16" s="83"/>
       <c r="B16" s="44" t="s">
         <v>3</v>
       </c>
@@ -4314,7 +4350,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="83" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="45" t="s">
@@ -4373,7 +4409,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A18" s="77"/>
+      <c r="A18" s="83"/>
       <c r="B18" s="44" t="s">
         <v>3</v>
       </c>
@@ -4430,10 +4466,10 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="16" thickTop="1">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="79" t="s">
+      <c r="B19" s="82" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="27">
@@ -4489,8 +4525,8 @@
       </c>
     </row>
     <row r="20" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A20" s="77"/>
-      <c r="B20" s="79"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="82"/>
       <c r="C20" s="42">
         <v>112</v>
       </c>
@@ -4544,8 +4580,8 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="16" thickTop="1">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77" t="s">
+      <c r="A21" s="83"/>
+      <c r="B21" s="83" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="33">
@@ -4601,8 +4637,8 @@
       </c>
     </row>
     <row r="22" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A22" s="77"/>
-      <c r="B22" s="77"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="83"/>
       <c r="C22" s="34">
         <v>117</v>
       </c>
@@ -4656,7 +4692,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="83" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="45" t="s">
@@ -4715,7 +4751,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A24" s="77"/>
+      <c r="A24" s="83"/>
       <c r="B24" s="44" t="s">
         <v>3</v>
       </c>
@@ -4772,7 +4808,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="83" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="45" t="s">
@@ -4831,7 +4867,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A26" s="77"/>
+      <c r="A26" s="83"/>
       <c r="B26" s="44" t="s">
         <v>3</v>
       </c>
@@ -4888,7 +4924,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="83" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="45" t="s">
@@ -4947,7 +4983,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A28" s="77"/>
+      <c r="A28" s="83"/>
       <c r="B28" s="44" t="s">
         <v>3</v>
       </c>
@@ -5004,10 +5040,10 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="16" thickTop="1">
-      <c r="A29" s="77" t="s">
+      <c r="A29" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="79" t="s">
+      <c r="B29" s="82" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="27">
@@ -5063,8 +5099,8 @@
       </c>
     </row>
     <row r="30" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A30" s="77"/>
-      <c r="B30" s="79"/>
+      <c r="A30" s="83"/>
+      <c r="B30" s="82"/>
       <c r="C30" s="42">
         <v>412</v>
       </c>
@@ -5118,8 +5154,8 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="16" thickTop="1">
-      <c r="A31" s="77"/>
-      <c r="B31" s="77" t="s">
+      <c r="A31" s="83"/>
+      <c r="B31" s="83" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="33">
@@ -5175,8 +5211,8 @@
       </c>
     </row>
     <row r="32" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A32" s="77"/>
-      <c r="B32" s="77"/>
+      <c r="A32" s="83"/>
+      <c r="B32" s="83"/>
       <c r="C32" s="34">
         <v>414</v>
       </c>
@@ -5230,10 +5266,10 @@
       </c>
     </row>
     <row r="33" spans="1:15" ht="16" thickTop="1">
-      <c r="A33" s="77" t="s">
+      <c r="A33" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="79" t="s">
+      <c r="B33" s="82" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="27">
@@ -5289,8 +5325,8 @@
       </c>
     </row>
     <row r="34" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A34" s="77"/>
-      <c r="B34" s="79"/>
+      <c r="A34" s="83"/>
+      <c r="B34" s="82"/>
       <c r="C34" s="42">
         <v>482</v>
       </c>
@@ -5344,7 +5380,7 @@
       </c>
     </row>
     <row r="35" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A35" s="77"/>
+      <c r="A35" s="83"/>
       <c r="B35" s="44" t="s">
         <v>3</v>
       </c>
@@ -5403,6 +5439,16 @@
     <row r="36" spans="1:15" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="A4:A6"/>
@@ -5419,16 +5465,6 @@
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5442,10 +5478,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W35"/>
+  <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5454,134 +5490,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="71" customHeight="1">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
     </row>
     <row r="2" spans="1:23" ht="25">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
-      <c r="C2" s="84">
+      <c r="C2" s="96">
         <v>2015</v>
       </c>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="85">
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="97">
         <v>2016</v>
       </c>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="86">
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="98">
         <v>2017</v>
       </c>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="87">
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="99">
         <v>2018</v>
       </c>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
     </row>
     <row r="3" spans="1:23" ht="23">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="90" t="s">
+      <c r="D3" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="90" t="s">
+      <c r="E3" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="91" t="s">
+      <c r="G3" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="91" t="s">
+      <c r="H3" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="92" t="s">
+      <c r="I3" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="92" t="s">
+      <c r="J3" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="92" t="s">
+      <c r="K3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="93" t="s">
+      <c r="L3" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="99" t="s">
+      <c r="M3" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="100" t="s">
+      <c r="N3" s="73" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:23">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="96">
+      <c r="C4" s="69">
         <f>SUM(Individuals!E4:F5,Individuals!E7:F7)</f>
         <v>134</v>
       </c>
-      <c r="D4" s="96">
+      <c r="D4" s="69">
         <f>SUM(Individuals!G4:H5,Individuals!G7:H7)</f>
         <v>1</v>
       </c>
-      <c r="E4" s="96">
+      <c r="E4" s="69">
         <f>SUM(Individuals!I4:J5,Individuals!I7:J7)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="96">
+      <c r="F4" s="69">
         <f>SUM(Individuals!K4:L5,Individuals!K7:L7)</f>
         <v>2</v>
       </c>
-      <c r="G4" s="96">
+      <c r="G4" s="69">
         <f>SUM(Individuals!M4:N5,Individuals!M7:N7)</f>
         <v>42</v>
       </c>
-      <c r="H4" s="96">
+      <c r="H4" s="69">
         <f>SUM(Individuals!O4:P5,Individuals!O7:P7)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="96">
+      <c r="I4" s="69">
         <f>SUM(Individuals!Q4:R5,Individuals!Q7:R7)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="96">
+      <c r="J4" s="69">
         <f>SUM(Individuals!S4:T5,Individuals!S7:T7)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="96">
+      <c r="K4" s="69">
         <f>SUM(Individuals!U4:V5,Individuals!U7:V7)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="96">
+      <c r="L4" s="69">
         <f>SUM(Individuals!W4:X5,Individuals!W7:X7)</f>
         <v>0</v>
       </c>
-      <c r="M4" s="96">
+      <c r="M4" s="69">
         <f>SUM(Individuals!Y4:Z5,Individuals!Y7:Z7)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="96">
+      <c r="N4" s="69">
         <f>SUM(Individuals!AA4:BB5,Individuals!AA7:BB7)</f>
         <v>0</v>
       </c>
@@ -5596,55 +5632,55 @@
       <c r="W4" s="1"/>
     </row>
     <row r="5" spans="1:23">
-      <c r="A5" s="95"/>
-      <c r="B5" s="98" t="s">
+      <c r="A5" s="102"/>
+      <c r="B5" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="98">
+      <c r="C5" s="71">
         <f>SUM(Individuals!E6:F6,Individuals!E8:F9)</f>
         <v>310</v>
       </c>
-      <c r="D5" s="98">
+      <c r="D5" s="71">
         <f>SUM(Individuals!G6:H6,Individuals!G8:H9)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="98">
+      <c r="E5" s="71">
         <f>SUM(Individuals!I6:J6,Individuals!I8:J9)</f>
         <v>51</v>
       </c>
-      <c r="F5" s="98">
+      <c r="F5" s="71">
         <f>SUM(Individuals!K6:L6,Individuals!K8:L9)</f>
         <v>298</v>
       </c>
-      <c r="G5" s="98">
+      <c r="G5" s="71">
         <f>SUM(Individuals!M6:N6,Individuals!M8:N9)</f>
         <v>87</v>
       </c>
-      <c r="H5" s="98">
+      <c r="H5" s="71">
         <f>SUM(Individuals!O6:P6,Individuals!O8:P9)</f>
         <v>39</v>
       </c>
-      <c r="I5" s="98">
+      <c r="I5" s="71">
         <f>SUM(Individuals!Q6:R6,Individuals!Q8:R9)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="98">
+      <c r="J5" s="71">
         <f>SUM(Individuals!S6:T6,Individuals!S8:T9)</f>
         <v>0</v>
       </c>
-      <c r="K5" s="98">
+      <c r="K5" s="71">
         <f>SUM(Individuals!U6:V6,Individuals!U8:V9)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="98">
+      <c r="L5" s="71">
         <f>SUM(Individuals!W6:X6,Individuals!W8:X9)</f>
         <v>95</v>
       </c>
-      <c r="M5" s="98">
+      <c r="M5" s="71">
         <f>SUM(Individuals!Y6:Z6,Individuals!Y8:Z9)</f>
         <v>2</v>
       </c>
-      <c r="N5" s="98">
+      <c r="N5" s="71">
         <f>SUM(Individuals!AA6:BB6,Individuals!AA8:BB9)</f>
         <v>0</v>
       </c>
@@ -5659,64 +5695,64 @@
       <c r="W5" s="1"/>
     </row>
     <row r="6" spans="1:23">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="101">
+      <c r="C6" s="74">
         <f>SUM(Individuals!E10:F11,Individuals!E14:F15,Individuals!E17:F17,Individuals!E19:F20)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="101">
+      <c r="D6" s="74">
         <f>SUM(Individuals!G10:H11,Individuals!G14:H15,Individuals!G17:H17,Individuals!G19:H20)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="101">
+      <c r="E6" s="74">
         <f>SUM(Individuals!I10:J11,Individuals!I14:J15,Individuals!I17:J17,Individuals!I19:J20)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="96">
+      <c r="F6" s="69">
         <f>SUM(Individuals!K10:L11,Individuals!K14:L15,Individuals!K17:L17,Individuals!K19:L20)</f>
         <v>246</v>
       </c>
-      <c r="G6" s="96">
+      <c r="G6" s="69">
         <f>SUM(Individuals!M10:N11,Individuals!M14:N15,Individuals!M17:N17,Individuals!M19:N20)</f>
         <v>134</v>
       </c>
-      <c r="H6" s="96">
+      <c r="H6" s="69">
         <f>SUM(Individuals!O10:P11,Individuals!O14:P15,Individuals!O17:P17,Individuals!O19:P20)</f>
         <v>2</v>
       </c>
-      <c r="I6" s="96">
+      <c r="I6" s="69">
         <f>SUM(Individuals!Q10:R11,Individuals!Q14:R15,Individuals!Q17:R17,Individuals!Q19:R20)</f>
         <v>127</v>
       </c>
-      <c r="J6" s="96">
+      <c r="J6" s="69">
         <f>SUM(Individuals!S10:T11,Individuals!S14:T15,Individuals!S17:T17,Individuals!S19:T20)</f>
         <v>110</v>
       </c>
-      <c r="K6" s="96">
+      <c r="K6" s="69">
         <f>SUM(Individuals!U10:V11,Individuals!U14:V15,Individuals!U17:V17,Individuals!U19:V20)</f>
         <v>0</v>
       </c>
-      <c r="L6" s="96">
+      <c r="L6" s="69">
         <f>SUM(Individuals!W10:X11,Individuals!W14:X15,Individuals!W17:X17,Individuals!W19:X20)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="96">
+      <c r="M6" s="69">
         <f>SUM(Individuals!Y10:Z11,Individuals!Y14:Z15,Individuals!Y17:Z17,Individuals!Y19:Z20)</f>
         <v>0</v>
       </c>
-      <c r="N6" s="96">
+      <c r="N6" s="69">
         <f>SUM(Individuals!AA10:AB11,Individuals!AA14:AB15,Individuals!AA17:AB17,Individuals!AA19:AB20)</f>
         <v>0</v>
       </c>
       <c r="O6" s="1"/>
-      <c r="P6" s="98"/>
+      <c r="P6" s="71"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="98"/>
+      <c r="R6" s="71"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -5724,62 +5760,62 @@
       <c r="W6" s="1"/>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="95"/>
-      <c r="B7" s="98" t="s">
+      <c r="A7" s="102"/>
+      <c r="B7" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="102">
+      <c r="C7" s="75">
         <f>SUM(Individuals!E12:F13,Individuals!E16:F16,Individuals!E18:F18,Individuals!E21:F22)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="102">
+      <c r="D7" s="75">
         <f>SUM(Individuals!G12:H13,Individuals!G16:H16,Individuals!G18:H18,Individuals!G21:H22)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="102">
+      <c r="E7" s="75">
         <f>SUM(Individuals!I12:J13,Individuals!I16:J16,Individuals!I18:J18,Individuals!I21:J22)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="98">
+      <c r="F7" s="71">
         <f>SUM(Individuals!K12:L13,Individuals!K16:L16,Individuals!K18:L18,Individuals!K21:L22)</f>
         <v>415</v>
       </c>
-      <c r="G7" s="98">
+      <c r="G7" s="71">
         <f>SUM(Individuals!M12:N13,Individuals!M16:N16,Individuals!M18:N18,Individuals!M21:N22)</f>
         <v>116</v>
       </c>
-      <c r="H7" s="98">
+      <c r="H7" s="71">
         <f>SUM(Individuals!O12:P13,Individuals!O16:P16,Individuals!O18:P18,Individuals!O21:P22)</f>
         <v>181</v>
       </c>
-      <c r="I7" s="98">
+      <c r="I7" s="71">
         <f>SUM(Individuals!Q12:R13,Individuals!Q16:R16,Individuals!Q18:R18,Individuals!Q21:R22)</f>
         <v>322</v>
       </c>
-      <c r="J7" s="98">
+      <c r="J7" s="71">
         <f>SUM(Individuals!S12:T13,Individuals!S16:T16,Individuals!S18:T18,Individuals!S21:T22)</f>
         <v>6</v>
       </c>
-      <c r="K7" s="98">
+      <c r="K7" s="71">
         <f>SUM(Individuals!U12:V13,Individuals!U16:V16,Individuals!U18:V18,Individuals!U21:V22)</f>
         <v>153</v>
       </c>
-      <c r="L7" s="98">
+      <c r="L7" s="71">
         <f>SUM(Individuals!W12:X13,Individuals!W16:X16,Individuals!W18:X18,Individuals!W21:X22)</f>
         <v>0</v>
       </c>
-      <c r="M7" s="98">
+      <c r="M7" s="71">
         <f>SUM(Individuals!Y12:Z13,Individuals!Y16:Z16,Individuals!Y18:Z18,Individuals!Y21:Z22)</f>
         <v>0</v>
       </c>
-      <c r="N7" s="98">
+      <c r="N7" s="71">
         <f>SUM(Individuals!AA12:AB13,Individuals!AA16:AB16,Individuals!AA18:AB18,Individuals!AA21:AB22)</f>
         <v>0</v>
       </c>
       <c r="O7" s="1"/>
-      <c r="P7" s="98"/>
+      <c r="P7" s="71"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="98"/>
+      <c r="R7" s="71"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
@@ -5787,276 +5823,276 @@
       <c r="W7" s="1"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="95" t="s">
+      <c r="A8" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="96">
+      <c r="C8" s="69">
         <f>SUM(Individuals!E23:F23,Individuals!E25:F25)</f>
         <v>41</v>
       </c>
-      <c r="D8" s="96">
+      <c r="D8" s="69">
         <f>SUM(Individuals!G23:H23,Individuals!G25:H25)</f>
         <v>56</v>
       </c>
-      <c r="E8" s="96">
+      <c r="E8" s="69">
         <f>SUM(Individuals!I23:J23,Individuals!I25:J25)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="96">
+      <c r="F8" s="69">
         <f>SUM(Individuals!K23:L23,Individuals!K25:L25)</f>
         <v>402</v>
       </c>
-      <c r="G8" s="96">
+      <c r="G8" s="69">
         <f>SUM(Individuals!M23:N23,Individuals!M25:N25)</f>
         <v>1</v>
       </c>
-      <c r="H8" s="96">
+      <c r="H8" s="69">
         <f>SUM(Individuals!O23:P23,Individuals!O25:P25)</f>
         <v>8</v>
       </c>
-      <c r="I8" s="96">
+      <c r="I8" s="69">
         <f>SUM(Individuals!Q23:R23,Individuals!Q25:R25)</f>
         <v>130</v>
       </c>
-      <c r="J8" s="96">
+      <c r="J8" s="69">
         <f>SUM(Individuals!S23:T23,Individuals!S25:T25)</f>
         <v>75</v>
       </c>
-      <c r="K8" s="96">
+      <c r="K8" s="69">
         <f>SUM(Individuals!U23:V23,Individuals!U25:V25)</f>
         <v>0</v>
       </c>
-      <c r="L8" s="96">
+      <c r="L8" s="69">
         <f>SUM(Individuals!W23:X23,Individuals!W25:X25)</f>
         <v>60</v>
       </c>
-      <c r="M8" s="96">
+      <c r="M8" s="69">
         <f>SUM(Individuals!Y23:Z23,Individuals!Y25:Z25)</f>
         <v>43</v>
       </c>
-      <c r="N8" s="96">
+      <c r="N8" s="69">
         <f>SUM(Individuals!AA23:AB23,Individuals!AA25:AB25)</f>
         <v>0</v>
       </c>
       <c r="O8" s="1"/>
-      <c r="P8" s="98"/>
-      <c r="Q8" s="98"/>
-      <c r="R8" s="98"/>
-      <c r="S8" s="98"/>
-      <c r="T8" s="98"/>
-      <c r="U8" s="98"/>
-      <c r="V8" s="98"/>
-      <c r="W8" s="98"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="71"/>
+      <c r="T8" s="71"/>
+      <c r="U8" s="71"/>
+      <c r="V8" s="71"/>
+      <c r="W8" s="71"/>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="95"/>
-      <c r="B9" s="98" t="s">
+      <c r="A9" s="102"/>
+      <c r="B9" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="98">
+      <c r="C9" s="71">
         <f>SUM(Individuals!E24:F24,Individuals!E26:F26)</f>
         <v>145</v>
       </c>
-      <c r="D9" s="98">
+      <c r="D9" s="71">
         <f>SUM(Individuals!G24:H24,Individuals!G26:H26)</f>
         <v>6</v>
       </c>
-      <c r="E9" s="98">
+      <c r="E9" s="71">
         <f>SUM(Individuals!I24:J24,Individuals!I26:J26)</f>
         <v>12</v>
       </c>
-      <c r="F9" s="98">
+      <c r="F9" s="71">
         <f>SUM(Individuals!K24:L24,Individuals!K26:L26)</f>
         <v>54</v>
       </c>
-      <c r="G9" s="98">
+      <c r="G9" s="71">
         <f>SUM(Individuals!M24:N24,Individuals!M26:N26)</f>
         <v>3</v>
       </c>
-      <c r="H9" s="98">
+      <c r="H9" s="71">
         <f>SUM(Individuals!O24:P24,Individuals!O26:P26)</f>
         <v>84</v>
       </c>
-      <c r="I9" s="98">
+      <c r="I9" s="71">
         <f>SUM(Individuals!Q24:R24,Individuals!Q26:R26)</f>
         <v>131</v>
       </c>
-      <c r="J9" s="98">
+      <c r="J9" s="71">
         <f>SUM(Individuals!S24:T24,Individuals!S26:T26)</f>
         <v>38</v>
       </c>
-      <c r="K9" s="98">
+      <c r="K9" s="71">
         <f>SUM(Individuals!U24:V24,Individuals!U26:V26)</f>
         <v>13</v>
       </c>
-      <c r="L9" s="98">
+      <c r="L9" s="71">
         <f>SUM(Individuals!W24:X24,Individuals!W26:X26)</f>
         <v>108</v>
       </c>
-      <c r="M9" s="98">
+      <c r="M9" s="71">
         <f>SUM(Individuals!Y24:Z24,Individuals!Y26:Z26)</f>
         <v>3</v>
       </c>
-      <c r="N9" s="98">
+      <c r="N9" s="71">
         <f>SUM(Individuals!AA24:AB24,Individuals!AA26:AB26)</f>
         <v>0</v>
       </c>
       <c r="O9" s="1"/>
-      <c r="P9" s="98"/>
-      <c r="Q9" s="98"/>
-      <c r="R9" s="98"/>
-      <c r="S9" s="98"/>
-      <c r="T9" s="98"/>
-      <c r="U9" s="98"/>
-      <c r="V9" s="98"/>
-      <c r="W9" s="98"/>
+      <c r="P9" s="71"/>
+      <c r="Q9" s="71"/>
+      <c r="R9" s="71"/>
+      <c r="S9" s="71"/>
+      <c r="T9" s="71"/>
+      <c r="U9" s="71"/>
+      <c r="V9" s="71"/>
+      <c r="W9" s="71"/>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="95" t="s">
+      <c r="A10" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="96" t="s">
+      <c r="B10" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="96">
+      <c r="C10" s="69">
         <f>SUM(Individuals!E27:F27,Individuals!E29:F30,Individuals!E33:F34)</f>
         <v>298</v>
       </c>
-      <c r="D10" s="96">
+      <c r="D10" s="69">
         <f>SUM(Individuals!G27:H27,Individuals!G29:H30,Individuals!G33:H34)</f>
         <v>81</v>
       </c>
-      <c r="E10" s="96">
+      <c r="E10" s="69">
         <f>SUM(Individuals!I27:J27,Individuals!I29:J30,Individuals!I33:J34)</f>
         <v>178</v>
       </c>
-      <c r="F10" s="96">
+      <c r="F10" s="69">
         <f>SUM(Individuals!K27:L27,Individuals!K29:L30,Individuals!K33:L34)</f>
         <v>29</v>
       </c>
-      <c r="G10" s="96">
+      <c r="G10" s="69">
         <f>SUM(Individuals!M27:N27,Individuals!M29:N30,Individuals!M33:N34)</f>
         <v>6</v>
       </c>
-      <c r="H10" s="96">
+      <c r="H10" s="69">
         <f>SUM(Individuals!O27:P27,Individuals!O29:P30,Individuals!O33:P34)</f>
         <v>44</v>
       </c>
-      <c r="I10" s="96">
+      <c r="I10" s="69">
         <f>SUM(Individuals!Q27:R27,Individuals!Q29:R30,Individuals!Q33:R34)</f>
         <v>151</v>
       </c>
-      <c r="J10" s="96">
+      <c r="J10" s="69">
         <f>SUM(Individuals!S27:T27,Individuals!S29:T30,Individuals!S33:T34)</f>
         <v>87</v>
       </c>
-      <c r="K10" s="96">
+      <c r="K10" s="69">
         <f>SUM(Individuals!U27:V27,Individuals!U29:V30,Individuals!U33:V34)</f>
         <v>89</v>
       </c>
-      <c r="L10" s="96">
+      <c r="L10" s="69">
         <f>SUM(Individuals!W27:X27,Individuals!W29:X30,Individuals!W33:X34)</f>
         <v>0</v>
       </c>
-      <c r="M10" s="96">
+      <c r="M10" s="69">
         <f>SUM(Individuals!Y27:Z27,Individuals!Y29:Z30,Individuals!Y33:Z34)</f>
         <v>0</v>
       </c>
-      <c r="N10" s="96">
+      <c r="N10" s="69">
         <f>SUM(Individuals!AA27:AB27,Individuals!AA29:AB30,Individuals!AA33:AB34)</f>
         <v>0</v>
       </c>
       <c r="O10" s="1"/>
-      <c r="P10" s="98"/>
-      <c r="Q10" s="98"/>
-      <c r="R10" s="98"/>
-      <c r="S10" s="98"/>
-      <c r="T10" s="98"/>
-      <c r="U10" s="98"/>
-      <c r="V10" s="98"/>
-      <c r="W10" s="98"/>
+      <c r="P10" s="71"/>
+      <c r="Q10" s="71"/>
+      <c r="R10" s="71"/>
+      <c r="S10" s="71"/>
+      <c r="T10" s="71"/>
+      <c r="U10" s="71"/>
+      <c r="V10" s="71"/>
+      <c r="W10" s="71"/>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="95"/>
-      <c r="B11" s="98" t="s">
+      <c r="A11" s="102"/>
+      <c r="B11" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="98">
+      <c r="C11" s="71">
         <f>SUM(Individuals!E28:F28,Individuals!E31:F32,Individuals!E35:F35)</f>
         <v>155</v>
       </c>
-      <c r="D11" s="98">
+      <c r="D11" s="71">
         <f>SUM(Individuals!G28:H28,Individuals!G31:H32,Individuals!G35:H35)</f>
         <v>103</v>
       </c>
-      <c r="E11" s="98">
+      <c r="E11" s="71">
         <f>SUM(Individuals!I28:J28,Individuals!I31:J32,Individuals!I35:J35)</f>
         <v>206</v>
       </c>
-      <c r="F11" s="98">
+      <c r="F11" s="71">
         <f>SUM(Individuals!K28:L28,Individuals!K31:L32,Individuals!K35:L35)</f>
         <v>125</v>
       </c>
-      <c r="G11" s="98">
+      <c r="G11" s="71">
         <f>SUM(Individuals!M28:N28,Individuals!M31:N32,Individuals!M35:N35)</f>
         <v>8</v>
       </c>
-      <c r="H11" s="98">
+      <c r="H11" s="71">
         <f>SUM(Individuals!O28:P28,Individuals!O31:P32,Individuals!O35:P35)</f>
         <v>131</v>
       </c>
-      <c r="I11" s="98">
+      <c r="I11" s="71">
         <f>SUM(Individuals!Q28:R28,Individuals!Q31:R32,Individuals!Q35:R35)</f>
         <v>96</v>
       </c>
-      <c r="J11" s="98">
+      <c r="J11" s="71">
         <f>SUM(Individuals!S28:T28,Individuals!S31:T32,Individuals!S35:T35)</f>
         <v>28</v>
       </c>
-      <c r="K11" s="98">
+      <c r="K11" s="71">
         <f>SUM(Individuals!U28:V28,Individuals!U31:V32,Individuals!U35:V35)</f>
         <v>88</v>
       </c>
-      <c r="L11" s="98">
+      <c r="L11" s="71">
         <f>SUM(Individuals!W28:X28,Individuals!W31:X32,Individuals!W35:X35)</f>
         <v>0</v>
       </c>
-      <c r="M11" s="98">
+      <c r="M11" s="71">
         <f>SUM(Individuals!Y28:Z28,Individuals!Y31:Z32,Individuals!Y35:Z35)</f>
         <v>0</v>
       </c>
-      <c r="N11" s="98">
+      <c r="N11" s="71">
         <f>SUM(Individuals!AA28:AB28,Individuals!AA31:AB32,Individuals!AA35:AB35)</f>
         <v>0</v>
       </c>
       <c r="O11" s="1"/>
-      <c r="P11" s="98"/>
-      <c r="Q11" s="98"/>
-      <c r="R11" s="98"/>
-      <c r="S11" s="98"/>
-      <c r="T11" s="98"/>
-      <c r="U11" s="98"/>
-      <c r="V11" s="98"/>
-      <c r="W11" s="98"/>
+      <c r="P11" s="71"/>
+      <c r="Q11" s="71"/>
+      <c r="R11" s="71"/>
+      <c r="S11" s="71"/>
+      <c r="T11" s="71"/>
+      <c r="U11" s="71"/>
+      <c r="V11" s="71"/>
+      <c r="W11" s="71"/>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="97"/>
-      <c r="B12" s="98"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="98"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="98"/>
-      <c r="J12" s="98"/>
-      <c r="K12" s="98"/>
-      <c r="L12" s="98"/>
-      <c r="M12" s="98"/>
-      <c r="N12" s="98"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -6067,21 +6103,29 @@
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:23">
-      <c r="A13" s="97"/>
-      <c r="B13" s="98"/>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98"/>
-      <c r="H13" s="98"/>
-      <c r="I13" s="98"/>
+    <row r="13" spans="1:23" ht="25">
+      <c r="A13" s="70"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="96">
+        <v>2015</v>
+      </c>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="97">
+        <v>2016</v>
+      </c>
+      <c r="G13" s="97"/>
+      <c r="H13" s="97"/>
+      <c r="I13" s="98">
+        <v>2017</v>
+      </c>
       <c r="J13" s="98"/>
       <c r="K13" s="98"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="98"/>
-      <c r="N13" s="98"/>
+      <c r="L13" s="99">
+        <v>2018</v>
+      </c>
+      <c r="M13" s="99"/>
+      <c r="N13" s="99"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -6092,371 +6136,685 @@
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:23">
-      <c r="A14" s="97"/>
-      <c r="B14" s="98"/>
-      <c r="C14" s="98"/>
-      <c r="D14" s="98"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="98"/>
-      <c r="G14" s="98"/>
-      <c r="H14" s="98"/>
-      <c r="I14" s="98"/>
-      <c r="J14" s="98"/>
-      <c r="K14" s="98"/>
-      <c r="L14" s="98"/>
-      <c r="M14" s="98"/>
-      <c r="N14" s="98"/>
+    <row r="14" spans="1:23" ht="23">
+      <c r="A14" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="66" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="66" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" s="73" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:23">
-      <c r="A15" s="97"/>
-      <c r="B15" s="98"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
-      <c r="G15" s="98"/>
-      <c r="H15" s="98"/>
-      <c r="I15" s="98"/>
-      <c r="J15" s="98"/>
-      <c r="K15" s="98"/>
-      <c r="L15" s="98"/>
-      <c r="M15" s="98"/>
-      <c r="N15" s="98"/>
+      <c r="A15" s="103" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="104" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="104">
+        <f>SUM(Ind_Summary!D4:D6)</f>
+        <v>444</v>
+      </c>
+      <c r="D15" s="104">
+        <f>SUM(Ind_Summary!E4:E6)</f>
+        <v>1</v>
+      </c>
+      <c r="E15" s="104">
+        <f>SUM(Ind_Summary!F4:F6)</f>
+        <v>51</v>
+      </c>
+      <c r="F15" s="104">
+        <f>SUM(Ind_Summary!G4:G6)</f>
+        <v>155</v>
+      </c>
+      <c r="G15" s="104">
+        <f>SUM(Ind_Summary!H4:H6)</f>
+        <v>100</v>
+      </c>
+      <c r="H15" s="104">
+        <f>SUM(Ind_Summary!I4:I6)</f>
+        <v>35</v>
+      </c>
+      <c r="I15" s="104">
+        <f>SUM(Ind_Summary!J4:J6)</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="104">
+        <f>SUM(Ind_Summary!K4:K6)</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="104">
+        <f>SUM(Ind_Summary!L4:L6)</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="104">
+        <f>SUM(Ind_Summary!M4:M6)</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="104">
+        <f>SUM(Ind_Summary!N4:N6)</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="104">
+        <f>SUM(Ind_Summary!O4:O6)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="97"/>
-      <c r="B16" s="98"/>
-      <c r="C16" s="98"/>
-      <c r="D16" s="98"/>
-      <c r="E16" s="98"/>
-      <c r="F16" s="98"/>
-      <c r="G16" s="98"/>
-      <c r="H16" s="98"/>
-      <c r="I16" s="98"/>
-      <c r="J16" s="98"/>
-      <c r="K16" s="98"/>
-      <c r="L16" s="98"/>
-      <c r="M16" s="98"/>
-      <c r="N16" s="98"/>
+      <c r="A16" s="103"/>
+      <c r="B16" s="104" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="104">
+        <f>SUM(Ind_Summary!D7:D9)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="104">
+        <f>SUM(Ind_Summary!E7:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="104">
+        <f>SUM(Ind_Summary!F7:F9)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="104">
+        <f>SUM(Ind_Summary!G7:G9)</f>
+        <v>145</v>
+      </c>
+      <c r="G16" s="104">
+        <f>SUM(Ind_Summary!H7:H9)</f>
+        <v>29</v>
+      </c>
+      <c r="H16" s="104">
+        <f>SUM(Ind_Summary!I7:I9)</f>
+        <v>4</v>
+      </c>
+      <c r="I16" s="104">
+        <f>SUM(Ind_Summary!J7:J9)</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="104">
+        <f>SUM(Ind_Summary!K7:K9)</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="104">
+        <f>SUM(Ind_Summary!L7:L9)</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="104">
+        <f>SUM(Ind_Summary!M7:M9)</f>
+        <v>95</v>
+      </c>
+      <c r="M16" s="104">
+        <f>SUM(Ind_Summary!N7:N9)</f>
+        <v>2</v>
+      </c>
+      <c r="N16" s="104">
+        <f>SUM(Ind_Summary!O7:O9)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="97"/>
-      <c r="B17" s="98"/>
-      <c r="C17" s="98"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="98"/>
-      <c r="F17" s="98"/>
-      <c r="G17" s="98"/>
-      <c r="H17" s="98"/>
-      <c r="I17" s="98"/>
-      <c r="J17" s="98"/>
-      <c r="K17" s="98"/>
-      <c r="L17" s="98"/>
-      <c r="M17" s="98"/>
-      <c r="N17" s="98"/>
+      <c r="A17" s="103" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="104" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="104">
+        <f>SUM(Ind_Summary!D10:D13)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="104">
+        <f>SUM(Ind_Summary!E10:E13)</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="104">
+        <f>SUM(Ind_Summary!F10:F13)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="104">
+        <f>SUM(Ind_Summary!G10:G13)</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="104">
+        <f>SUM(Ind_Summary!H10:H13)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="104">
+        <f>SUM(Ind_Summary!I10:I13)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="104">
+        <f>SUM(Ind_Summary!J10:J13)</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="104">
+        <f>SUM(Ind_Summary!K10:K13)</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="104">
+        <f>SUM(Ind_Summary!L10:L13)</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="104">
+        <f>SUM(Ind_Summary!M10:M13)</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="104">
+        <f>SUM(Ind_Summary!N10:N13)</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="104">
+        <f>SUM(Ind_Summary!O10:O13)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="97"/>
-      <c r="B18" s="98"/>
-      <c r="C18" s="98"/>
-      <c r="D18" s="98"/>
-      <c r="E18" s="98"/>
-      <c r="F18" s="98"/>
-      <c r="G18" s="98"/>
-      <c r="H18" s="98"/>
-      <c r="I18" s="98"/>
-      <c r="J18" s="98"/>
-      <c r="K18" s="98"/>
-      <c r="L18" s="98"/>
-      <c r="M18" s="98"/>
-      <c r="N18" s="98"/>
+      <c r="A18" s="103"/>
+      <c r="B18" s="104" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="104">
+        <f>SUM(Ind_Summary!D14:D16)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="104">
+        <f>SUM(Ind_Summary!E14:E16)</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="104">
+        <f>SUM(Ind_Summary!F14:F16)</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="104">
+        <f>SUM(Ind_Summary!G14:G16)</f>
+        <v>147</v>
+      </c>
+      <c r="G18" s="104">
+        <f>SUM(Ind_Summary!H14:H16)</f>
+        <v>1</v>
+      </c>
+      <c r="H18" s="104">
+        <f>SUM(Ind_Summary!I14:I16)</f>
+        <v>48</v>
+      </c>
+      <c r="I18" s="104">
+        <f>SUM(Ind_Summary!J14:J16)</f>
+        <v>49</v>
+      </c>
+      <c r="J18" s="104">
+        <f>SUM(Ind_Summary!K14:K16)</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="104">
+        <f>SUM(Ind_Summary!L14:L16)</f>
+        <v>152</v>
+      </c>
+      <c r="L18" s="104">
+        <f>SUM(Ind_Summary!M14:M16)</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="104">
+        <f>SUM(Ind_Summary!N14:N16)</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="104">
+        <f>SUM(Ind_Summary!O14:O16)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="97"/>
-      <c r="B19" s="98"/>
-      <c r="C19" s="98"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="98"/>
-      <c r="F19" s="98"/>
-      <c r="G19" s="98"/>
-      <c r="H19" s="98"/>
-      <c r="I19" s="98"/>
-      <c r="J19" s="98"/>
-      <c r="K19" s="98"/>
-      <c r="L19" s="98"/>
-      <c r="M19" s="98"/>
-      <c r="N19" s="98"/>
+      <c r="A19" s="103"/>
+      <c r="B19" s="104" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="104">
+        <f>SUM(Ind_Summary!D17:D18)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="104">
+        <f>SUM(Ind_Summary!E17:E18)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="104">
+        <f>SUM(Ind_Summary!F17:F18)</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="104">
+        <f>SUM(Ind_Summary!G17:G18)</f>
+        <v>138</v>
+      </c>
+      <c r="G19" s="104">
+        <f>SUM(Ind_Summary!H17:H18)</f>
+        <v>119</v>
+      </c>
+      <c r="H19" s="104">
+        <f>SUM(Ind_Summary!I17:I18)</f>
+        <v>9</v>
+      </c>
+      <c r="I19" s="104">
+        <f>SUM(Ind_Summary!J17:J18)</f>
+        <v>266</v>
+      </c>
+      <c r="J19" s="104">
+        <f>SUM(Ind_Summary!K17:K18)</f>
+        <v>6</v>
+      </c>
+      <c r="K19" s="104">
+        <f>SUM(Ind_Summary!L17:L18)</f>
+        <v>1</v>
+      </c>
+      <c r="L19" s="104">
+        <f>SUM(Ind_Summary!M17:M18)</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="104">
+        <f>SUM(Ind_Summary!N17:N18)</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="104">
+        <f>SUM(Ind_Summary!O17:O18)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="97"/>
-      <c r="B20" s="98"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="98"/>
-      <c r="F20" s="98"/>
-      <c r="G20" s="98"/>
-      <c r="H20" s="98"/>
-      <c r="I20" s="98"/>
-      <c r="J20" s="98"/>
-      <c r="K20" s="98"/>
-      <c r="L20" s="98"/>
-      <c r="M20" s="98"/>
-      <c r="N20" s="98"/>
+      <c r="A20" s="103"/>
+      <c r="B20" s="104" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="104">
+        <f>SUM(Ind_Summary!D19:D22)</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="104">
+        <f>SUM(Ind_Summary!E19:E22)</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="104">
+        <f>SUM(Ind_Summary!F19:F22)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="104">
+        <f>SUM(Ind_Summary!G19:G22)</f>
+        <v>376</v>
+      </c>
+      <c r="G20" s="104">
+        <f>SUM(Ind_Summary!H19:H22)</f>
+        <v>130</v>
+      </c>
+      <c r="H20" s="104">
+        <f>SUM(Ind_Summary!I19:I22)</f>
+        <v>126</v>
+      </c>
+      <c r="I20" s="104">
+        <f>SUM(Ind_Summary!J19:J22)</f>
+        <v>134</v>
+      </c>
+      <c r="J20" s="104">
+        <f>SUM(Ind_Summary!K19:K22)</f>
+        <v>110</v>
+      </c>
+      <c r="K20" s="104">
+        <f>SUM(Ind_Summary!L19:L22)</f>
+        <v>0</v>
+      </c>
+      <c r="L20" s="104">
+        <f>SUM(Ind_Summary!M19:M22)</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="104">
+        <f>SUM(Ind_Summary!N19:N22)</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="104">
+        <f>SUM(Ind_Summary!O19:O22)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="97"/>
-      <c r="B21" s="98"/>
-      <c r="C21" s="98"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="98"/>
-      <c r="F21" s="98"/>
-      <c r="G21" s="98"/>
-      <c r="H21" s="98"/>
-      <c r="I21" s="98"/>
-      <c r="J21" s="98"/>
-      <c r="K21" s="98"/>
-      <c r="L21" s="98"/>
-      <c r="M21" s="98"/>
-      <c r="N21" s="98"/>
+      <c r="A21" s="105" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="104" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="104">
+        <f>SUM(Ind_Summary!D23:D24)</f>
+        <v>41</v>
+      </c>
+      <c r="D21" s="104">
+        <f>SUM(Ind_Summary!E23:E24)</f>
+        <v>56</v>
+      </c>
+      <c r="E21" s="104">
+        <f>SUM(Ind_Summary!F23:F24)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="104">
+        <f>SUM(Ind_Summary!G23:G24)</f>
+        <v>405</v>
+      </c>
+      <c r="G21" s="104">
+        <f>SUM(Ind_Summary!H23:H24)</f>
+        <v>4</v>
+      </c>
+      <c r="H21" s="104">
+        <f>SUM(Ind_Summary!I23:I24)</f>
+        <v>92</v>
+      </c>
+      <c r="I21" s="104">
+        <f>SUM(Ind_Summary!J23:J24)</f>
+        <v>250</v>
+      </c>
+      <c r="J21" s="104">
+        <f>SUM(Ind_Summary!K23:K24)</f>
+        <v>54</v>
+      </c>
+      <c r="K21" s="104">
+        <f>SUM(Ind_Summary!L23:L24)</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="104">
+        <f>SUM(Ind_Summary!M23:M24)</f>
+        <v>60</v>
+      </c>
+      <c r="M21" s="104">
+        <f>SUM(Ind_Summary!N23:N24)</f>
+        <v>43</v>
+      </c>
+      <c r="N21" s="104">
+        <f>SUM(Ind_Summary!O23:O24)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="97"/>
-      <c r="B22" s="98"/>
-      <c r="C22" s="98"/>
-      <c r="D22" s="98"/>
-      <c r="E22" s="98"/>
-      <c r="F22" s="98"/>
-      <c r="G22" s="98"/>
-      <c r="H22" s="98"/>
-      <c r="I22" s="98"/>
-      <c r="J22" s="98"/>
-      <c r="K22" s="98"/>
-      <c r="L22" s="98"/>
-      <c r="M22" s="98"/>
-      <c r="N22" s="98"/>
+      <c r="A22" s="105"/>
+      <c r="B22" s="104" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="26">
+        <f>SUM(Ind_Summary!D25:D26)</f>
+        <v>145</v>
+      </c>
+      <c r="D22" s="26">
+        <f>SUM(Ind_Summary!E25:E26)</f>
+        <v>6</v>
+      </c>
+      <c r="E22" s="26">
+        <f>SUM(Ind_Summary!F25:F26)</f>
+        <v>12</v>
+      </c>
+      <c r="F22" s="26">
+        <f>SUM(Ind_Summary!G25:G26)</f>
+        <v>51</v>
+      </c>
+      <c r="G22" s="26">
+        <f>SUM(Ind_Summary!H25:H26)</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="26">
+        <f>SUM(Ind_Summary!I25:I26)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="26">
+        <f>SUM(Ind_Summary!J25:J26)</f>
+        <v>11</v>
+      </c>
+      <c r="J22" s="26">
+        <f>SUM(Ind_Summary!K25:K26)</f>
+        <v>59</v>
+      </c>
+      <c r="K22" s="26">
+        <f>SUM(Ind_Summary!L25:L26)</f>
+        <v>13</v>
+      </c>
+      <c r="L22" s="26">
+        <f>SUM(Ind_Summary!M25:M26)</f>
+        <v>108</v>
+      </c>
+      <c r="M22" s="26">
+        <f>SUM(Ind_Summary!N25:N26)</f>
+        <v>3</v>
+      </c>
+      <c r="N22" s="26">
+        <f>SUM(Ind_Summary!O25:O26)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="97"/>
-      <c r="B23" s="98"/>
-      <c r="C23" s="98"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="98"/>
-      <c r="F23" s="98"/>
-      <c r="G23" s="98"/>
-      <c r="H23" s="98"/>
-      <c r="I23" s="98"/>
-      <c r="J23" s="98"/>
-      <c r="K23" s="98"/>
-      <c r="L23" s="98"/>
-      <c r="M23" s="98"/>
-      <c r="N23" s="98"/>
+      <c r="A23" s="105" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="104" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="26">
+        <f>SUM(Ind_Summary!D27:D28)</f>
+        <v>163</v>
+      </c>
+      <c r="D23" s="26">
+        <f>SUM(Ind_Summary!E27:E28)</f>
+        <v>155</v>
+      </c>
+      <c r="E23" s="26">
+        <f>SUM(Ind_Summary!F27:F28)</f>
+        <v>157</v>
+      </c>
+      <c r="F23" s="26">
+        <f>SUM(Ind_Summary!G27:G28)</f>
+        <v>29</v>
+      </c>
+      <c r="G23" s="26">
+        <f>SUM(Ind_Summary!H27:H28)</f>
+        <v>1</v>
+      </c>
+      <c r="H23" s="26">
+        <f>SUM(Ind_Summary!I27:I28)</f>
+        <v>124</v>
+      </c>
+      <c r="I23" s="26">
+        <f>SUM(Ind_Summary!J27:J28)</f>
+        <v>197</v>
+      </c>
+      <c r="J23" s="26">
+        <f>SUM(Ind_Summary!K27:K28)</f>
+        <v>112</v>
+      </c>
+      <c r="K23" s="26">
+        <f>SUM(Ind_Summary!L27:L28)</f>
+        <v>15</v>
+      </c>
+      <c r="L23" s="26">
+        <f>SUM(Ind_Summary!M27:M28)</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="26">
+        <f>SUM(Ind_Summary!N27:N28)</f>
+        <v>0</v>
+      </c>
+      <c r="N23" s="26">
+        <f>SUM(Ind_Summary!O27:O28)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="97"/>
-      <c r="B24" s="98"/>
-      <c r="C24" s="98"/>
-      <c r="D24" s="98"/>
-      <c r="E24" s="98"/>
-      <c r="F24" s="98"/>
-      <c r="G24" s="98"/>
-      <c r="H24" s="98"/>
-      <c r="I24" s="98"/>
-      <c r="J24" s="98"/>
-      <c r="K24" s="98"/>
-      <c r="L24" s="98"/>
-      <c r="M24" s="98"/>
-      <c r="N24" s="98"/>
+      <c r="A24" s="105"/>
+      <c r="B24" s="104" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="26">
+        <f>SUM(Ind_Summary!D29:D32)</f>
+        <v>153</v>
+      </c>
+      <c r="D24" s="26">
+        <f>SUM(Ind_Summary!E29:E32)</f>
+        <v>29</v>
+      </c>
+      <c r="E24" s="26">
+        <f>SUM(Ind_Summary!F29:F32)</f>
+        <v>186</v>
+      </c>
+      <c r="F24" s="26">
+        <f>SUM(Ind_Summary!G29:G32)</f>
+        <v>86</v>
+      </c>
+      <c r="G24" s="26">
+        <f>SUM(Ind_Summary!H29:H32)</f>
+        <v>13</v>
+      </c>
+      <c r="H24" s="26">
+        <f>SUM(Ind_Summary!I29:I32)</f>
+        <v>19</v>
+      </c>
+      <c r="I24" s="26">
+        <f>SUM(Ind_Summary!J29:J32)</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="26">
+        <f>SUM(Ind_Summary!K29:K32)</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="26">
+        <f>SUM(Ind_Summary!L29:L32)</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="26">
+        <f>SUM(Ind_Summary!M29:M32)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="26">
+        <f>SUM(Ind_Summary!N29:N32)</f>
+        <v>0</v>
+      </c>
+      <c r="N24" s="26">
+        <f>SUM(Ind_Summary!O29:O32)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="97"/>
-      <c r="B25" s="98"/>
-      <c r="C25" s="98"/>
-      <c r="D25" s="98"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="98"/>
-      <c r="G25" s="98"/>
-      <c r="H25" s="98"/>
-      <c r="I25" s="98"/>
-      <c r="J25" s="98"/>
-      <c r="K25" s="98"/>
-      <c r="L25" s="98"/>
-      <c r="M25" s="98"/>
-      <c r="N25" s="98"/>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="A26" s="97"/>
-      <c r="B26" s="98"/>
-      <c r="C26" s="98"/>
-      <c r="D26" s="98"/>
-      <c r="E26" s="98"/>
-      <c r="F26" s="98"/>
-      <c r="G26" s="98"/>
-      <c r="H26" s="98"/>
-      <c r="I26" s="98"/>
-      <c r="J26" s="98"/>
-      <c r="K26" s="98"/>
-      <c r="L26" s="98"/>
-      <c r="M26" s="98"/>
-      <c r="N26" s="98"/>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" s="97"/>
-      <c r="B27" s="98"/>
-      <c r="C27" s="98"/>
-      <c r="D27" s="98"/>
-      <c r="E27" s="98"/>
-      <c r="F27" s="98"/>
-      <c r="G27" s="98"/>
-      <c r="H27" s="98"/>
-      <c r="I27" s="98"/>
-      <c r="J27" s="98"/>
-      <c r="K27" s="98"/>
-      <c r="L27" s="98"/>
-      <c r="M27" s="98"/>
-      <c r="N27" s="98"/>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="97"/>
-      <c r="B28" s="98"/>
-      <c r="C28" s="98"/>
-      <c r="D28" s="98"/>
-      <c r="E28" s="98"/>
-      <c r="F28" s="98"/>
-      <c r="G28" s="98"/>
-      <c r="H28" s="98"/>
-      <c r="I28" s="98"/>
-      <c r="J28" s="98"/>
-      <c r="K28" s="98"/>
-      <c r="L28" s="98"/>
-      <c r="M28" s="98"/>
-      <c r="N28" s="98"/>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="97"/>
-      <c r="B29" s="98"/>
-      <c r="C29" s="98"/>
-      <c r="D29" s="98"/>
-      <c r="E29" s="98"/>
-      <c r="F29" s="98"/>
-      <c r="G29" s="98"/>
-      <c r="H29" s="98"/>
-      <c r="I29" s="98"/>
-      <c r="J29" s="98"/>
-      <c r="K29" s="98"/>
-      <c r="L29" s="98"/>
-      <c r="M29" s="98"/>
-      <c r="N29" s="98"/>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="97"/>
-      <c r="B30" s="98"/>
-      <c r="C30" s="98"/>
-      <c r="D30" s="98"/>
-      <c r="E30" s="98"/>
-      <c r="F30" s="98"/>
-      <c r="G30" s="98"/>
-      <c r="H30" s="98"/>
-      <c r="I30" s="98"/>
-      <c r="J30" s="98"/>
-      <c r="K30" s="98"/>
-      <c r="L30" s="98"/>
-      <c r="M30" s="98"/>
-      <c r="N30" s="98"/>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31" s="97"/>
-      <c r="B31" s="98"/>
-      <c r="C31" s="98"/>
-      <c r="D31" s="98"/>
-      <c r="E31" s="98"/>
-      <c r="F31" s="98"/>
-      <c r="G31" s="98"/>
-      <c r="H31" s="98"/>
-      <c r="I31" s="98"/>
-      <c r="J31" s="98"/>
-      <c r="K31" s="98"/>
-      <c r="L31" s="98"/>
-      <c r="M31" s="98"/>
-      <c r="N31" s="98"/>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" s="97"/>
-      <c r="B32" s="98"/>
-      <c r="C32" s="98"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="98"/>
-      <c r="F32" s="98"/>
-      <c r="G32" s="98"/>
-      <c r="H32" s="98"/>
-      <c r="I32" s="98"/>
-      <c r="J32" s="98"/>
-      <c r="K32" s="98"/>
-      <c r="L32" s="98"/>
-      <c r="M32" s="98"/>
-      <c r="N32" s="98"/>
-    </row>
-    <row r="33" spans="1:14">
-      <c r="A33" s="97"/>
-      <c r="B33" s="98"/>
-      <c r="C33" s="98"/>
-      <c r="D33" s="98"/>
-      <c r="E33" s="98"/>
-      <c r="F33" s="98"/>
-      <c r="G33" s="98"/>
-      <c r="H33" s="98"/>
-      <c r="I33" s="98"/>
-      <c r="J33" s="98"/>
-      <c r="K33" s="98"/>
-      <c r="L33" s="98"/>
-      <c r="M33" s="98"/>
-      <c r="N33" s="98"/>
-    </row>
-    <row r="34" spans="1:14">
-      <c r="A34" s="97"/>
-      <c r="B34" s="98"/>
-      <c r="C34" s="98"/>
-      <c r="D34" s="98"/>
-      <c r="E34" s="98"/>
-      <c r="F34" s="98"/>
-      <c r="G34" s="98"/>
-      <c r="H34" s="98"/>
-      <c r="I34" s="98"/>
-      <c r="J34" s="98"/>
-      <c r="K34" s="98"/>
-      <c r="L34" s="98"/>
-      <c r="M34" s="98"/>
-      <c r="N34" s="98"/>
-    </row>
-    <row r="35" spans="1:14" s="1" customFormat="1">
-      <c r="A35" s="98"/>
-      <c r="B35" s="98"/>
-      <c r="C35" s="98"/>
-      <c r="D35" s="98"/>
-      <c r="E35" s="98"/>
-      <c r="F35" s="98"/>
-      <c r="G35" s="98"/>
-      <c r="H35" s="98"/>
-      <c r="I35" s="98"/>
-      <c r="J35" s="98"/>
-      <c r="K35" s="98"/>
-      <c r="L35" s="98"/>
-      <c r="M35" s="98"/>
-      <c r="N35" s="98"/>
+      <c r="A25" s="105"/>
+      <c r="B25" s="104" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="26">
+        <f>SUM(Ind_Summary!D33:D35)</f>
+        <v>137</v>
+      </c>
+      <c r="D25" s="26">
+        <f>SUM(Ind_Summary!E33:E35)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="26">
+        <f>SUM(Ind_Summary!F33:F35)</f>
+        <v>41</v>
+      </c>
+      <c r="F25" s="26">
+        <f>SUM(Ind_Summary!G33:G35)</f>
+        <v>39</v>
+      </c>
+      <c r="G25" s="26">
+        <f>SUM(Ind_Summary!H33:H35)</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="26">
+        <f>SUM(Ind_Summary!I33:I35)</f>
+        <v>32</v>
+      </c>
+      <c r="I25" s="26">
+        <f>SUM(Ind_Summary!J33:J35)</f>
+        <v>50</v>
+      </c>
+      <c r="J25" s="26">
+        <f>SUM(Ind_Summary!K33:K35)</f>
+        <v>3</v>
+      </c>
+      <c r="K25" s="26">
+        <f>SUM(Ind_Summary!L33:L35)</f>
+        <v>162</v>
+      </c>
+      <c r="L25" s="26">
+        <f>SUM(Ind_Summary!M33:M35)</f>
+        <v>0</v>
+      </c>
+      <c r="M25" s="26">
+        <f>SUM(Ind_Summary!N33:N35)</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="26">
+        <f>SUM(Ind_Summary!O33:O35)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="17">
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="L13:N13"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:N11">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:N25">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Add code for companion summary statistics table for EP whole coast.
</commit_message>
<xml_diff>
--- a/data/sampleTable.xlsx
+++ b/data/sampleTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15280" windowHeight="17440" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28060" windowHeight="17540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -815,17 +815,26 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -839,26 +848,17 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1663,97 +1663,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="15" customFormat="1" ht="25">
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="81">
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="92">
         <v>2015</v>
       </c>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="83">
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="94">
         <v>2016</v>
       </c>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="85">
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="88">
         <v>2017</v>
       </c>
-      <c r="R1" s="85"/>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
-      <c r="U1" s="85"/>
-      <c r="V1" s="85"/>
-      <c r="W1" s="87">
+      <c r="R1" s="88"/>
+      <c r="S1" s="88"/>
+      <c r="T1" s="88"/>
+      <c r="U1" s="88"/>
+      <c r="V1" s="88"/>
+      <c r="W1" s="90">
         <v>2018</v>
       </c>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
+      <c r="X1" s="90"/>
+      <c r="Y1" s="90"/>
+      <c r="Z1" s="90"/>
+      <c r="AA1" s="90"/>
+      <c r="AB1" s="90"/>
       <c r="AC1" s="13"/>
     </row>
     <row r="2" spans="1:29" s="16" customFormat="1" ht="23">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="82" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82" t="s">
+      <c r="F2" s="93"/>
+      <c r="G2" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82" t="s">
+      <c r="H2" s="93"/>
+      <c r="I2" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="82"/>
-      <c r="K2" s="84" t="s">
+      <c r="J2" s="93"/>
+      <c r="K2" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84" t="s">
+      <c r="L2" s="95"/>
+      <c r="M2" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84" t="s">
+      <c r="N2" s="95"/>
+      <c r="O2" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="86" t="s">
+      <c r="P2" s="95"/>
+      <c r="Q2" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="86"/>
-      <c r="S2" s="86" t="s">
+      <c r="R2" s="89"/>
+      <c r="S2" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="86"/>
-      <c r="U2" s="86" t="s">
+      <c r="T2" s="89"/>
+      <c r="U2" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="86"/>
-      <c r="W2" s="88" t="s">
+      <c r="V2" s="89"/>
+      <c r="W2" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="88"/>
-      <c r="Y2" s="88" t="s">
+      <c r="X2" s="91"/>
+      <c r="Y2" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="Z2" s="88"/>
-      <c r="AA2" s="88" t="s">
+      <c r="Z2" s="91"/>
+      <c r="AA2" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="88"/>
+      <c r="AB2" s="91"/>
       <c r="AC2" s="14"/>
     </row>
     <row r="3" spans="1:29" s="22" customFormat="1" ht="20">
@@ -1844,13 +1844,13 @@
       <c r="AC3" s="21"/>
     </row>
     <row r="4" spans="1:29">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="82" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="23">
@@ -1918,9 +1918,9 @@
       <c r="AB4" s="24"/>
     </row>
     <row r="5" spans="1:29">
-      <c r="A5" s="89"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="91"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="82"/>
       <c r="D5" s="23">
         <v>183</v>
       </c>
@@ -1950,8 +1950,8 @@
       <c r="AB5" s="24"/>
     </row>
     <row r="6" spans="1:29">
-      <c r="A6" s="89"/>
-      <c r="B6" s="89"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="83"/>
       <c r="C6" s="25" t="s">
         <v>3</v>
       </c>
@@ -2008,8 +2008,8 @@
       <c r="AB6" s="26"/>
     </row>
     <row r="7" spans="1:29">
-      <c r="A7" s="89"/>
-      <c r="B7" s="89" t="s">
+      <c r="A7" s="83"/>
+      <c r="B7" s="83" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="23" t="s">
@@ -2068,9 +2068,9 @@
       <c r="AB7" s="24"/>
     </row>
     <row r="8" spans="1:29">
-      <c r="A8" s="89"/>
-      <c r="B8" s="89"/>
-      <c r="C8" s="89" t="s">
+      <c r="A8" s="83"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="25">
@@ -2126,9 +2126,9 @@
       </c>
     </row>
     <row r="9" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A9" s="90"/>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="84"/>
+      <c r="C9" s="84"/>
       <c r="D9" s="29">
         <v>171</v>
       </c>
@@ -2171,13 +2171,13 @@
       <c r="AC9" s="31"/>
     </row>
     <row r="10" spans="1:29" ht="16" thickTop="1">
-      <c r="A10" s="92" t="s">
+      <c r="A10" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="94" t="s">
+      <c r="C10" s="87" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="27">
@@ -2221,9 +2221,9 @@
       <c r="AB10" s="28"/>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="89"/>
-      <c r="B11" s="89"/>
-      <c r="C11" s="91"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="23">
         <v>139</v>
       </c>
@@ -2253,9 +2253,9 @@
       <c r="AB11" s="24"/>
     </row>
     <row r="12" spans="1:29">
-      <c r="A12" s="89"/>
-      <c r="B12" s="89"/>
-      <c r="C12" s="89" t="s">
+      <c r="A12" s="83"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="25">
@@ -2299,9 +2299,9 @@
       <c r="AB12" s="26"/>
     </row>
     <row r="13" spans="1:29">
-      <c r="A13" s="89"/>
-      <c r="B13" s="89"/>
-      <c r="C13" s="89"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="83"/>
       <c r="D13" s="25">
         <v>156</v>
       </c>
@@ -2331,11 +2331,11 @@
       <c r="AB13" s="26"/>
     </row>
     <row r="14" spans="1:29">
-      <c r="A14" s="89"/>
-      <c r="B14" s="89" t="s">
+      <c r="A14" s="83"/>
+      <c r="B14" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="91" t="s">
+      <c r="C14" s="82" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="23">
@@ -2379,9 +2379,9 @@
       <c r="AB14" s="24"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="A15" s="89"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="91"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="82"/>
       <c r="D15" s="23">
         <v>132</v>
       </c>
@@ -2411,8 +2411,8 @@
       <c r="AB15" s="24"/>
     </row>
     <row r="16" spans="1:29">
-      <c r="A16" s="89"/>
-      <c r="B16" s="89"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="25" t="s">
         <v>3</v>
       </c>
@@ -2469,8 +2469,8 @@
       <c r="AB16" s="26"/>
     </row>
     <row r="17" spans="1:29">
-      <c r="A17" s="89"/>
-      <c r="B17" s="89" t="s">
+      <c r="A17" s="83"/>
+      <c r="B17" s="83" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="23" t="s">
@@ -2517,8 +2517,8 @@
       <c r="AB17" s="24"/>
     </row>
     <row r="18" spans="1:29">
-      <c r="A18" s="89"/>
-      <c r="B18" s="89"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="83"/>
       <c r="C18" s="25" t="s">
         <v>3</v>
       </c>
@@ -2575,11 +2575,11 @@
       <c r="AB18" s="26"/>
     </row>
     <row r="19" spans="1:29">
-      <c r="A19" s="89"/>
-      <c r="B19" s="89" t="s">
+      <c r="A19" s="83"/>
+      <c r="B19" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="91" t="s">
+      <c r="C19" s="82" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="23">
@@ -2623,9 +2623,9 @@
       <c r="AB19" s="24"/>
     </row>
     <row r="20" spans="1:29">
-      <c r="A20" s="89"/>
-      <c r="B20" s="89"/>
-      <c r="C20" s="91"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="82"/>
       <c r="D20" s="23">
         <v>112</v>
       </c>
@@ -2667,9 +2667,9 @@
       <c r="AB20" s="24"/>
     </row>
     <row r="21" spans="1:29">
-      <c r="A21" s="89"/>
-      <c r="B21" s="89"/>
-      <c r="C21" s="89" t="s">
+      <c r="A21" s="83"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="83" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="25">
@@ -2713,9 +2713,9 @@
       <c r="AB21" s="26"/>
     </row>
     <row r="22" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A22" s="90"/>
-      <c r="B22" s="90"/>
-      <c r="C22" s="90"/>
+      <c r="A22" s="84"/>
+      <c r="B22" s="84"/>
+      <c r="C22" s="84"/>
       <c r="D22" s="29">
         <v>117</v>
       </c>
@@ -2770,10 +2770,10 @@
       <c r="AC22" s="31"/>
     </row>
     <row r="23" spans="1:29" ht="16" thickTop="1">
-      <c r="A23" s="92" t="s">
+      <c r="A23" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="92" t="s">
+      <c r="B23" s="85" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="35" t="s">
@@ -2856,8 +2856,8 @@
       </c>
     </row>
     <row r="24" spans="1:29">
-      <c r="A24" s="89"/>
-      <c r="B24" s="89"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="83"/>
       <c r="C24" s="25" t="s">
         <v>3</v>
       </c>
@@ -2914,8 +2914,8 @@
       <c r="AB24" s="26"/>
     </row>
     <row r="25" spans="1:29">
-      <c r="A25" s="89"/>
-      <c r="B25" s="89" t="s">
+      <c r="A25" s="83"/>
+      <c r="B25" s="83" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="23" t="s">
@@ -2962,8 +2962,8 @@
       <c r="AB25" s="24"/>
     </row>
     <row r="26" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A26" s="90"/>
-      <c r="B26" s="90"/>
+      <c r="A26" s="84"/>
+      <c r="B26" s="84"/>
       <c r="C26" s="29" t="s">
         <v>3</v>
       </c>
@@ -3045,10 +3045,10 @@
       <c r="AC26" s="31"/>
     </row>
     <row r="27" spans="1:29" ht="16" thickTop="1">
-      <c r="A27" s="93" t="s">
+      <c r="A27" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="93" t="s">
+      <c r="B27" s="86" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="27" t="s">
@@ -3119,8 +3119,8 @@
       <c r="AB27" s="28"/>
     </row>
     <row r="28" spans="1:29">
-      <c r="A28" s="89"/>
-      <c r="B28" s="89"/>
+      <c r="A28" s="83"/>
+      <c r="B28" s="83"/>
       <c r="C28" s="25" t="s">
         <v>3</v>
       </c>
@@ -3189,11 +3189,11 @@
       <c r="AB28" s="26"/>
     </row>
     <row r="29" spans="1:29">
-      <c r="A29" s="89"/>
-      <c r="B29" s="89" t="s">
+      <c r="A29" s="83"/>
+      <c r="B29" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="91" t="s">
+      <c r="C29" s="82" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="23">
@@ -3249,9 +3249,9 @@
       <c r="AB29" s="24"/>
     </row>
     <row r="30" spans="1:29">
-      <c r="A30" s="89"/>
-      <c r="B30" s="89"/>
-      <c r="C30" s="91"/>
+      <c r="A30" s="83"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="82"/>
       <c r="D30" s="23">
         <v>412</v>
       </c>
@@ -3293,9 +3293,9 @@
       <c r="AB30" s="24"/>
     </row>
     <row r="31" spans="1:29">
-      <c r="A31" s="89"/>
-      <c r="B31" s="89"/>
-      <c r="C31" s="89" t="s">
+      <c r="A31" s="83"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="83" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="25">
@@ -3339,9 +3339,9 @@
       <c r="AB31" s="26"/>
     </row>
     <row r="32" spans="1:29">
-      <c r="A32" s="89"/>
-      <c r="B32" s="89"/>
-      <c r="C32" s="89"/>
+      <c r="A32" s="83"/>
+      <c r="B32" s="83"/>
+      <c r="C32" s="83"/>
       <c r="D32" s="25">
         <v>414</v>
       </c>
@@ -3383,11 +3383,11 @@
       <c r="AB32" s="26"/>
     </row>
     <row r="33" spans="1:29">
-      <c r="A33" s="89"/>
-      <c r="B33" s="89" t="s">
+      <c r="A33" s="83"/>
+      <c r="B33" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="91" t="s">
+      <c r="C33" s="82" t="s">
         <v>2</v>
       </c>
       <c r="D33" s="23">
@@ -3431,9 +3431,9 @@
       <c r="AB33" s="24"/>
     </row>
     <row r="34" spans="1:29">
-      <c r="A34" s="89"/>
-      <c r="B34" s="89"/>
-      <c r="C34" s="91"/>
+      <c r="A34" s="83"/>
+      <c r="B34" s="83"/>
+      <c r="C34" s="82"/>
       <c r="D34" s="23">
         <v>482</v>
       </c>
@@ -3487,8 +3487,8 @@
       <c r="AB34" s="24"/>
     </row>
     <row r="35" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A35" s="90"/>
-      <c r="B35" s="90"/>
+      <c r="A35" s="84"/>
+      <c r="B35" s="84"/>
       <c r="C35" s="29" t="s">
         <v>3</v>
       </c>
@@ -3572,12 +3572,27 @@
     <row r="36" spans="1:29" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W1:AB1"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B7:B9"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A27:A35"/>
     <mergeCell ref="C21:C22"/>
@@ -3593,27 +3608,12 @@
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W1:AB1"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K1:P1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B33:B35"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3630,10 +3630,10 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R19" sqref="R19"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3724,10 +3724,10 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="82" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="23">
@@ -3783,8 +3783,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A5" s="89"/>
-      <c r="B5" s="91"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="82"/>
       <c r="C5" s="42">
         <v>183</v>
       </c>
@@ -3812,15 +3812,15 @@
         <f>SUM(Individuals!O5:P5)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="59">
+      <c r="J5" s="43">
         <f>SUM(Individuals!Q5:R5)</f>
         <v>0</v>
       </c>
-      <c r="K5" s="59">
+      <c r="K5" s="43">
         <f>SUM(Individuals!S5:T5)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="59">
+      <c r="L5" s="47">
         <f>SUM(Individuals!U5:V5)</f>
         <v>0</v>
       </c>
@@ -3838,7 +3838,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A6" s="89"/>
+      <c r="A6" s="83"/>
       <c r="B6" s="44" t="s">
         <v>3</v>
       </c>
@@ -3895,7 +3895,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="83" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="45" t="s">
@@ -3954,8 +3954,8 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="16" thickTop="1">
-      <c r="A8" s="89"/>
-      <c r="B8" s="89" t="s">
+      <c r="A8" s="83"/>
+      <c r="B8" s="83" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="33">
@@ -4011,8 +4011,8 @@
       </c>
     </row>
     <row r="9" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A9" s="89"/>
-      <c r="B9" s="89"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="34">
         <v>171</v>
       </c>
@@ -4066,10 +4066,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="16" thickTop="1">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="82" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="27">
@@ -4125,8 +4125,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A11" s="89"/>
-      <c r="B11" s="91"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="42">
         <v>139</v>
       </c>
@@ -4180,8 +4180,8 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="16" thickTop="1">
-      <c r="A12" s="89"/>
-      <c r="B12" s="89" t="s">
+      <c r="A12" s="83"/>
+      <c r="B12" s="83" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="33">
@@ -4237,8 +4237,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A13" s="89"/>
-      <c r="B13" s="89"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="34">
         <v>156</v>
       </c>
@@ -4292,10 +4292,10 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" thickTop="1">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="91" t="s">
+      <c r="B14" s="82" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="27">
@@ -4351,8 +4351,8 @@
       </c>
     </row>
     <row r="15" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A15" s="89"/>
-      <c r="B15" s="91"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="82"/>
       <c r="C15" s="42">
         <v>132</v>
       </c>
@@ -4406,7 +4406,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A16" s="89"/>
+      <c r="A16" s="83"/>
       <c r="B16" s="44" t="s">
         <v>3</v>
       </c>
@@ -4463,7 +4463,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="83" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="45" t="s">
@@ -4522,7 +4522,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A18" s="89"/>
+      <c r="A18" s="83"/>
       <c r="B18" s="44" t="s">
         <v>3</v>
       </c>
@@ -4579,10 +4579,10 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="16" thickTop="1">
-      <c r="A19" s="89" t="s">
+      <c r="A19" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="91" t="s">
+      <c r="B19" s="82" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="27">
@@ -4638,8 +4638,8 @@
       </c>
     </row>
     <row r="20" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A20" s="89"/>
-      <c r="B20" s="91"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="82"/>
       <c r="C20" s="42">
         <v>112</v>
       </c>
@@ -4693,8 +4693,8 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="16" thickTop="1">
-      <c r="A21" s="89"/>
-      <c r="B21" s="89" t="s">
+      <c r="A21" s="83"/>
+      <c r="B21" s="83" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="33">
@@ -4750,8 +4750,8 @@
       </c>
     </row>
     <row r="22" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A22" s="89"/>
-      <c r="B22" s="89"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="83"/>
       <c r="C22" s="34">
         <v>117</v>
       </c>
@@ -4805,7 +4805,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A23" s="89" t="s">
+      <c r="A23" s="83" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="45" t="s">
@@ -4864,7 +4864,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A24" s="89"/>
+      <c r="A24" s="83"/>
       <c r="B24" s="44" t="s">
         <v>3</v>
       </c>
@@ -4921,7 +4921,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A25" s="89" t="s">
+      <c r="A25" s="83" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="45" t="s">
@@ -4980,7 +4980,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A26" s="89"/>
+      <c r="A26" s="83"/>
       <c r="B26" s="44" t="s">
         <v>3</v>
       </c>
@@ -5037,7 +5037,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A27" s="89" t="s">
+      <c r="A27" s="83" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="45" t="s">
@@ -5096,7 +5096,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A28" s="89"/>
+      <c r="A28" s="83"/>
       <c r="B28" s="44" t="s">
         <v>3</v>
       </c>
@@ -5153,10 +5153,10 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="16" thickTop="1">
-      <c r="A29" s="89" t="s">
+      <c r="A29" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="91" t="s">
+      <c r="B29" s="82" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="27">
@@ -5212,8 +5212,8 @@
       </c>
     </row>
     <row r="30" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A30" s="89"/>
-      <c r="B30" s="91"/>
+      <c r="A30" s="83"/>
+      <c r="B30" s="82"/>
       <c r="C30" s="42">
         <v>412</v>
       </c>
@@ -5267,8 +5267,8 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="16" thickTop="1">
-      <c r="A31" s="89"/>
-      <c r="B31" s="89" t="s">
+      <c r="A31" s="83"/>
+      <c r="B31" s="83" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="33">
@@ -5324,8 +5324,8 @@
       </c>
     </row>
     <row r="32" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A32" s="89"/>
-      <c r="B32" s="89"/>
+      <c r="A32" s="83"/>
+      <c r="B32" s="83"/>
       <c r="C32" s="34">
         <v>414</v>
       </c>
@@ -5379,10 +5379,10 @@
       </c>
     </row>
     <row r="33" spans="1:15" ht="16" thickTop="1">
-      <c r="A33" s="89" t="s">
+      <c r="A33" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="91" t="s">
+      <c r="B33" s="82" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="27">
@@ -5438,8 +5438,8 @@
       </c>
     </row>
     <row r="34" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A34" s="89"/>
-      <c r="B34" s="91"/>
+      <c r="A34" s="83"/>
+      <c r="B34" s="82"/>
       <c r="C34" s="42">
         <v>482</v>
       </c>
@@ -5493,7 +5493,7 @@
       </c>
     </row>
     <row r="35" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A35" s="89"/>
+      <c r="A35" s="83"/>
       <c r="B35" s="44" t="s">
         <v>3</v>
       </c>
@@ -5552,6 +5552,16 @@
     <row r="36" spans="1:15" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="A4:A6"/>
@@ -5568,16 +5578,6 @@
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6897,14 +6897,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="L13:N13"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A21:A22"/>
@@ -6914,6 +6906,14 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="L13:N13"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:N11">
     <cfRule type="colorScale" priority="2">

</xml_diff>

<commit_message>
Restructure violin plots for better viewing by time or latitude. Saved accordingly.
</commit_message>
<xml_diff>
--- a/data/sampleTable.xlsx
+++ b/data/sampleTable.xlsx
@@ -677,7 +677,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -767,7 +767,6 @@
     <xf numFmtId="0" fontId="14" fillId="13" borderId="10" xfId="23" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="15" borderId="14" xfId="24" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="15" xfId="22" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="15" xfId="22" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="10" xfId="22" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="11" xfId="22" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="8" xfId="22" applyFill="1" applyBorder="1"/>
@@ -1333,34 +1332,34 @@
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76">
+      <c r="B1" s="75">
         <v>2015</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="78">
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="77">
         <v>2016</v>
       </c>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="79">
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="78">
         <v>2017</v>
       </c>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="80">
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="79">
         <v>2018</v>
       </c>
-      <c r="R1" s="80"/>
-      <c r="S1" s="80"/>
-      <c r="T1" s="80"/>
-      <c r="U1" s="80"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
     </row>
     <row r="2" spans="1:21" s="2" customFormat="1" ht="36">
       <c r="A2" s="6" t="s">
@@ -1663,97 +1662,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="15" customFormat="1" ht="25">
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="81">
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="80">
         <v>2015</v>
       </c>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="83">
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="82">
         <v>2016</v>
       </c>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="85">
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="84">
         <v>2017</v>
       </c>
-      <c r="R1" s="85"/>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
-      <c r="U1" s="85"/>
-      <c r="V1" s="85"/>
-      <c r="W1" s="87">
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="86">
         <v>2018</v>
       </c>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="86"/>
+      <c r="AA1" s="86"/>
+      <c r="AB1" s="86"/>
       <c r="AC1" s="13"/>
     </row>
     <row r="2" spans="1:29" s="16" customFormat="1" ht="23">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="82" t="s">
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82" t="s">
+      <c r="F2" s="81"/>
+      <c r="G2" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82" t="s">
+      <c r="H2" s="81"/>
+      <c r="I2" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="82"/>
-      <c r="K2" s="84" t="s">
+      <c r="J2" s="81"/>
+      <c r="K2" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84" t="s">
+      <c r="L2" s="83"/>
+      <c r="M2" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84" t="s">
+      <c r="N2" s="83"/>
+      <c r="O2" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="86" t="s">
+      <c r="P2" s="83"/>
+      <c r="Q2" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="86"/>
-      <c r="S2" s="86" t="s">
+      <c r="R2" s="85"/>
+      <c r="S2" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="86"/>
-      <c r="U2" s="86" t="s">
+      <c r="T2" s="85"/>
+      <c r="U2" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="86"/>
-      <c r="W2" s="88" t="s">
+      <c r="V2" s="85"/>
+      <c r="W2" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="88"/>
-      <c r="Y2" s="88" t="s">
+      <c r="X2" s="87"/>
+      <c r="Y2" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="Z2" s="88"/>
-      <c r="AA2" s="88" t="s">
+      <c r="Z2" s="87"/>
+      <c r="AA2" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="88"/>
+      <c r="AB2" s="87"/>
       <c r="AC2" s="14"/>
     </row>
     <row r="3" spans="1:29" s="22" customFormat="1" ht="20">
@@ -1844,13 +1843,13 @@
       <c r="AC3" s="21"/>
     </row>
     <row r="4" spans="1:29">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="90" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="23">
@@ -1918,9 +1917,9 @@
       <c r="AB4" s="24"/>
     </row>
     <row r="5" spans="1:29">
-      <c r="A5" s="89"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="91"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="90"/>
       <c r="D5" s="23">
         <v>183</v>
       </c>
@@ -1950,8 +1949,8 @@
       <c r="AB5" s="24"/>
     </row>
     <row r="6" spans="1:29">
-      <c r="A6" s="89"/>
-      <c r="B6" s="89"/>
+      <c r="A6" s="88"/>
+      <c r="B6" s="88"/>
       <c r="C6" s="25" t="s">
         <v>3</v>
       </c>
@@ -2008,8 +2007,8 @@
       <c r="AB6" s="26"/>
     </row>
     <row r="7" spans="1:29">
-      <c r="A7" s="89"/>
-      <c r="B7" s="89" t="s">
+      <c r="A7" s="88"/>
+      <c r="B7" s="88" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="23" t="s">
@@ -2080,9 +2079,9 @@
       </c>
     </row>
     <row r="8" spans="1:29">
-      <c r="A8" s="89"/>
-      <c r="B8" s="89"/>
-      <c r="C8" s="89" t="s">
+      <c r="A8" s="88"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="25">
@@ -2138,9 +2137,9 @@
       </c>
     </row>
     <row r="9" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A9" s="90"/>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
+      <c r="A9" s="89"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="89"/>
       <c r="D9" s="29">
         <v>171</v>
       </c>
@@ -2183,13 +2182,13 @@
       <c r="AC9" s="31"/>
     </row>
     <row r="10" spans="1:29" ht="16" thickTop="1">
-      <c r="A10" s="92" t="s">
+      <c r="A10" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="94" t="s">
+      <c r="C10" s="93" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="27">
@@ -2233,9 +2232,9 @@
       <c r="AB10" s="28"/>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="89"/>
-      <c r="B11" s="89"/>
-      <c r="C11" s="91"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="90"/>
       <c r="D11" s="23">
         <v>139</v>
       </c>
@@ -2265,9 +2264,9 @@
       <c r="AB11" s="24"/>
     </row>
     <row r="12" spans="1:29">
-      <c r="A12" s="89"/>
-      <c r="B12" s="89"/>
-      <c r="C12" s="89" t="s">
+      <c r="A12" s="88"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="25">
@@ -2311,9 +2310,9 @@
       <c r="AB12" s="26"/>
     </row>
     <row r="13" spans="1:29">
-      <c r="A13" s="89"/>
-      <c r="B13" s="89"/>
-      <c r="C13" s="89"/>
+      <c r="A13" s="88"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="88"/>
       <c r="D13" s="25">
         <v>156</v>
       </c>
@@ -2343,11 +2342,11 @@
       <c r="AB13" s="26"/>
     </row>
     <row r="14" spans="1:29">
-      <c r="A14" s="89"/>
-      <c r="B14" s="89" t="s">
+      <c r="A14" s="88"/>
+      <c r="B14" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="91" t="s">
+      <c r="C14" s="90" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="23">
@@ -2391,9 +2390,9 @@
       <c r="AB14" s="24"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="A15" s="89"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="91"/>
+      <c r="A15" s="88"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="90"/>
       <c r="D15" s="23">
         <v>132</v>
       </c>
@@ -2423,8 +2422,8 @@
       <c r="AB15" s="24"/>
     </row>
     <row r="16" spans="1:29">
-      <c r="A16" s="89"/>
-      <c r="B16" s="89"/>
+      <c r="A16" s="88"/>
+      <c r="B16" s="88"/>
       <c r="C16" s="25" t="s">
         <v>3</v>
       </c>
@@ -2481,8 +2480,8 @@
       <c r="AB16" s="26"/>
     </row>
     <row r="17" spans="1:29">
-      <c r="A17" s="89"/>
-      <c r="B17" s="89" t="s">
+      <c r="A17" s="88"/>
+      <c r="B17" s="88" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="23" t="s">
@@ -2541,8 +2540,8 @@
       <c r="AB17" s="24"/>
     </row>
     <row r="18" spans="1:29">
-      <c r="A18" s="89"/>
-      <c r="B18" s="89"/>
+      <c r="A18" s="88"/>
+      <c r="B18" s="88"/>
       <c r="C18" s="25" t="s">
         <v>3</v>
       </c>
@@ -2599,11 +2598,11 @@
       <c r="AB18" s="26"/>
     </row>
     <row r="19" spans="1:29">
-      <c r="A19" s="89"/>
-      <c r="B19" s="89" t="s">
+      <c r="A19" s="88"/>
+      <c r="B19" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="91" t="s">
+      <c r="C19" s="90" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="23">
@@ -2647,9 +2646,9 @@
       <c r="AB19" s="24"/>
     </row>
     <row r="20" spans="1:29">
-      <c r="A20" s="89"/>
-      <c r="B20" s="89"/>
-      <c r="C20" s="91"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="90"/>
       <c r="D20" s="23">
         <v>112</v>
       </c>
@@ -2691,9 +2690,9 @@
       <c r="AB20" s="24"/>
     </row>
     <row r="21" spans="1:29">
-      <c r="A21" s="89"/>
-      <c r="B21" s="89"/>
-      <c r="C21" s="89" t="s">
+      <c r="A21" s="88"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="88" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="25">
@@ -2737,9 +2736,9 @@
       <c r="AB21" s="26"/>
     </row>
     <row r="22" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A22" s="90"/>
-      <c r="B22" s="90"/>
-      <c r="C22" s="90"/>
+      <c r="A22" s="89"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="89"/>
       <c r="D22" s="29">
         <v>117</v>
       </c>
@@ -2806,10 +2805,10 @@
       <c r="AC22" s="31"/>
     </row>
     <row r="23" spans="1:29" ht="16" thickTop="1">
-      <c r="A23" s="92" t="s">
+      <c r="A23" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="92" t="s">
+      <c r="B23" s="91" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="35" t="s">
@@ -2892,8 +2891,8 @@
       </c>
     </row>
     <row r="24" spans="1:29">
-      <c r="A24" s="89"/>
-      <c r="B24" s="89"/>
+      <c r="A24" s="88"/>
+      <c r="B24" s="88"/>
       <c r="C24" s="25" t="s">
         <v>3</v>
       </c>
@@ -2950,8 +2949,8 @@
       <c r="AB24" s="26"/>
     </row>
     <row r="25" spans="1:29">
-      <c r="A25" s="89"/>
-      <c r="B25" s="89" t="s">
+      <c r="A25" s="88"/>
+      <c r="B25" s="88" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="23" t="s">
@@ -2998,8 +2997,8 @@
       <c r="AB25" s="24"/>
     </row>
     <row r="26" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A26" s="90"/>
-      <c r="B26" s="90"/>
+      <c r="A26" s="89"/>
+      <c r="B26" s="89"/>
       <c r="C26" s="29" t="s">
         <v>3</v>
       </c>
@@ -3081,10 +3080,10 @@
       <c r="AC26" s="31"/>
     </row>
     <row r="27" spans="1:29" ht="16" thickTop="1">
-      <c r="A27" s="93" t="s">
+      <c r="A27" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="93" t="s">
+      <c r="B27" s="92" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="27" t="s">
@@ -3167,8 +3166,8 @@
       </c>
     </row>
     <row r="28" spans="1:29">
-      <c r="A28" s="89"/>
-      <c r="B28" s="89"/>
+      <c r="A28" s="88"/>
+      <c r="B28" s="88"/>
       <c r="C28" s="25" t="s">
         <v>3</v>
       </c>
@@ -3249,11 +3248,11 @@
       </c>
     </row>
     <row r="29" spans="1:29">
-      <c r="A29" s="89"/>
-      <c r="B29" s="89" t="s">
+      <c r="A29" s="88"/>
+      <c r="B29" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="91" t="s">
+      <c r="C29" s="90" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="23">
@@ -3309,9 +3308,9 @@
       <c r="AB29" s="24"/>
     </row>
     <row r="30" spans="1:29">
-      <c r="A30" s="89"/>
-      <c r="B30" s="89"/>
-      <c r="C30" s="91"/>
+      <c r="A30" s="88"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="90"/>
       <c r="D30" s="23">
         <v>412</v>
       </c>
@@ -3353,9 +3352,9 @@
       <c r="AB30" s="24"/>
     </row>
     <row r="31" spans="1:29">
-      <c r="A31" s="89"/>
-      <c r="B31" s="89"/>
-      <c r="C31" s="89" t="s">
+      <c r="A31" s="88"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="88" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="25">
@@ -3411,9 +3410,9 @@
       </c>
     </row>
     <row r="32" spans="1:29">
-      <c r="A32" s="89"/>
-      <c r="B32" s="89"/>
-      <c r="C32" s="89"/>
+      <c r="A32" s="88"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="88"/>
       <c r="D32" s="25">
         <v>414</v>
       </c>
@@ -3455,11 +3454,11 @@
       <c r="AB32" s="26"/>
     </row>
     <row r="33" spans="1:29">
-      <c r="A33" s="89"/>
-      <c r="B33" s="89" t="s">
+      <c r="A33" s="88"/>
+      <c r="B33" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="91" t="s">
+      <c r="C33" s="90" t="s">
         <v>2</v>
       </c>
       <c r="D33" s="23">
@@ -3515,9 +3514,9 @@
       </c>
     </row>
     <row r="34" spans="1:29">
-      <c r="A34" s="89"/>
-      <c r="B34" s="89"/>
-      <c r="C34" s="91"/>
+      <c r="A34" s="88"/>
+      <c r="B34" s="88"/>
+      <c r="C34" s="90"/>
       <c r="D34" s="23">
         <v>482</v>
       </c>
@@ -3583,8 +3582,8 @@
       </c>
     </row>
     <row r="35" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A35" s="90"/>
-      <c r="B35" s="90"/>
+      <c r="A35" s="89"/>
+      <c r="B35" s="89"/>
       <c r="C35" s="29" t="s">
         <v>3</v>
       </c>
@@ -3726,10 +3725,10 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3738,39 +3737,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="48" customHeight="1">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
     </row>
     <row r="2" spans="1:15" ht="25">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
-      <c r="D2" s="96">
+      <c r="D2" s="95">
         <v>2015</v>
       </c>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="97">
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="96">
         <v>2016</v>
       </c>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="98">
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="97">
         <v>2017</v>
       </c>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="99">
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="98">
         <v>2018</v>
       </c>
-      <c r="N2" s="99"/>
-      <c r="O2" s="99"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
     </row>
     <row r="3" spans="1:15" ht="23">
       <c r="A3" s="36" t="s">
@@ -3820,10 +3819,10 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="90" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="23">
@@ -3865,22 +3864,22 @@
         <f>SUM(Individuals!U4:V4)</f>
         <v>0</v>
       </c>
-      <c r="M4" s="60">
+      <c r="M4" s="59">
         <f>SUM(Individuals!W4:X4)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="60">
+      <c r="N4" s="59">
         <f>SUM(Individuals!Y4:Z4)</f>
         <v>0</v>
       </c>
-      <c r="O4" s="60">
+      <c r="O4" s="59">
         <f>SUM(Individuals!AA4:BB4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A5" s="89"/>
-      <c r="B5" s="91"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="90"/>
       <c r="C5" s="42">
         <v>183</v>
       </c>
@@ -3920,21 +3919,21 @@
         <f>SUM(Individuals!U5:V5)</f>
         <v>0</v>
       </c>
-      <c r="M5" s="59">
+      <c r="M5" s="58">
         <f>SUM(Individuals!W5:X5)</f>
         <v>0</v>
       </c>
-      <c r="N5" s="59">
+      <c r="N5" s="58">
         <f>SUM(Individuals!Y5:Z5)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="59">
+      <c r="O5" s="58">
         <f>SUM(Individuals!AA5:BB5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A6" s="89"/>
+      <c r="A6" s="88"/>
       <c r="B6" s="44" t="s">
         <v>3</v>
       </c>
@@ -3991,7 +3990,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="88" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="45" t="s">
@@ -4036,22 +4035,22 @@
         <f>SUM(Individuals!U7:V7)</f>
         <v>0</v>
       </c>
-      <c r="M7" s="57">
+      <c r="M7" s="49">
         <f>SUM(Individuals!W7:X7)</f>
         <v>57</v>
       </c>
-      <c r="N7" s="57">
+      <c r="N7" s="50">
         <f>SUM(Individuals!Y7:Z7)</f>
         <v>0</v>
       </c>
-      <c r="O7" s="57">
+      <c r="O7" s="50">
         <f>SUM(Individuals!AA7:BB7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="16" thickTop="1">
-      <c r="A8" s="89"/>
-      <c r="B8" s="89" t="s">
+      <c r="A8" s="88"/>
+      <c r="B8" s="88" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="33">
@@ -4107,8 +4106,8 @@
       </c>
     </row>
     <row r="9" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A9" s="89"/>
-      <c r="B9" s="89"/>
+      <c r="A9" s="88"/>
+      <c r="B9" s="88"/>
       <c r="C9" s="34">
         <v>171</v>
       </c>
@@ -4162,10 +4161,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="16" thickTop="1">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="90" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="27">
@@ -4195,15 +4194,15 @@
         <f>SUM(Individuals!O10:P10)</f>
         <v>0</v>
       </c>
-      <c r="J10" s="58">
+      <c r="J10" s="57">
         <f>SUM(Individuals!Q10:R10)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="58">
+      <c r="K10" s="57">
         <f>SUM(Individuals!S10:T10)</f>
         <v>0</v>
       </c>
-      <c r="L10" s="58">
+      <c r="L10" s="57">
         <f>SUM(Individuals!U10:V10)</f>
         <v>0</v>
       </c>
@@ -4221,8 +4220,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A11" s="89"/>
-      <c r="B11" s="91"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="90"/>
       <c r="C11" s="42">
         <v>139</v>
       </c>
@@ -4250,15 +4249,15 @@
         <f>SUM(Individuals!O11:P11)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="59">
+      <c r="J11" s="58">
         <f>SUM(Individuals!Q11:R11)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="59">
+      <c r="K11" s="58">
         <f>SUM(Individuals!S11:T11)</f>
         <v>0</v>
       </c>
-      <c r="L11" s="59">
+      <c r="L11" s="58">
         <f>SUM(Individuals!U11:V11)</f>
         <v>0</v>
       </c>
@@ -4276,8 +4275,8 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="16" thickTop="1">
-      <c r="A12" s="89"/>
-      <c r="B12" s="89" t="s">
+      <c r="A12" s="88"/>
+      <c r="B12" s="88" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="33">
@@ -4307,15 +4306,15 @@
         <f>SUM(Individuals!O12:P12)</f>
         <v>0</v>
       </c>
-      <c r="J12" s="58">
+      <c r="J12" s="57">
         <f>SUM(Individuals!Q12:R12)</f>
         <v>0</v>
       </c>
-      <c r="K12" s="58">
+      <c r="K12" s="57">
         <f>SUM(Individuals!S12:T12)</f>
         <v>0</v>
       </c>
-      <c r="L12" s="58">
+      <c r="L12" s="57">
         <f>SUM(Individuals!U12:V12)</f>
         <v>0</v>
       </c>
@@ -4333,8 +4332,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A13" s="89"/>
-      <c r="B13" s="89"/>
+      <c r="A13" s="88"/>
+      <c r="B13" s="88"/>
       <c r="C13" s="34">
         <v>156</v>
       </c>
@@ -4362,15 +4361,15 @@
         <f>SUM(Individuals!O13:P13)</f>
         <v>0</v>
       </c>
-      <c r="J13" s="59">
+      <c r="J13" s="58">
         <f>SUM(Individuals!Q13:R13)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="59">
+      <c r="K13" s="58">
         <f>SUM(Individuals!S13:T13)</f>
         <v>0</v>
       </c>
-      <c r="L13" s="59">
+      <c r="L13" s="58">
         <f>SUM(Individuals!U13:V13)</f>
         <v>0</v>
       </c>
@@ -4388,10 +4387,10 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" thickTop="1">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="91" t="s">
+      <c r="B14" s="90" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="27">
@@ -4447,8 +4446,8 @@
       </c>
     </row>
     <row r="15" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A15" s="89"/>
-      <c r="B15" s="91"/>
+      <c r="A15" s="88"/>
+      <c r="B15" s="90"/>
       <c r="C15" s="42">
         <v>132</v>
       </c>
@@ -4502,7 +4501,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A16" s="89"/>
+      <c r="A16" s="88"/>
       <c r="B16" s="44" t="s">
         <v>3</v>
       </c>
@@ -4559,7 +4558,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="88" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="45" t="s">
@@ -4618,7 +4617,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A18" s="89"/>
+      <c r="A18" s="88"/>
       <c r="B18" s="44" t="s">
         <v>3</v>
       </c>
@@ -4675,10 +4674,10 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="16" thickTop="1">
-      <c r="A19" s="89" t="s">
+      <c r="A19" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="91" t="s">
+      <c r="B19" s="90" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="27">
@@ -4734,8 +4733,8 @@
       </c>
     </row>
     <row r="20" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A20" s="89"/>
-      <c r="B20" s="91"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="90"/>
       <c r="C20" s="42">
         <v>112</v>
       </c>
@@ -4789,8 +4788,8 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="16" thickTop="1">
-      <c r="A21" s="89"/>
-      <c r="B21" s="89" t="s">
+      <c r="A21" s="88"/>
+      <c r="B21" s="88" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="33">
@@ -4832,22 +4831,22 @@
         <f>SUM(Individuals!U21:V21)</f>
         <v>0</v>
       </c>
-      <c r="M21" s="52">
+      <c r="M21" s="53">
         <f>SUM(Individuals!W21:X21)</f>
         <v>0</v>
       </c>
-      <c r="N21" s="52">
+      <c r="N21" s="54">
         <f>SUM(Individuals!Y21:Z21)</f>
         <v>0</v>
       </c>
-      <c r="O21" s="52">
+      <c r="O21" s="54">
         <f>SUM(Individuals!AA21:BB21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A22" s="89"/>
-      <c r="B22" s="89"/>
+      <c r="A22" s="88"/>
+      <c r="B22" s="88"/>
       <c r="C22" s="34">
         <v>117</v>
       </c>
@@ -4887,21 +4886,21 @@
         <f>SUM(Individuals!U22:V22)</f>
         <v>0</v>
       </c>
-      <c r="M22" s="48">
+      <c r="M22" s="43">
         <f>SUM(Individuals!W22:X22)</f>
         <v>60</v>
       </c>
-      <c r="N22" s="48">
+      <c r="N22" s="47">
         <f>SUM(Individuals!Y22:Z22)</f>
         <v>3</v>
       </c>
-      <c r="O22" s="48">
+      <c r="O22" s="47">
         <f>SUM(Individuals!AA22:BB22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A23" s="89" t="s">
+      <c r="A23" s="88" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="45" t="s">
@@ -4960,7 +4959,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A24" s="89"/>
+      <c r="A24" s="88"/>
       <c r="B24" s="44" t="s">
         <v>3</v>
       </c>
@@ -5017,7 +5016,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A25" s="89" t="s">
+      <c r="A25" s="88" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="45" t="s">
@@ -5076,7 +5075,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A26" s="89"/>
+      <c r="A26" s="88"/>
       <c r="B26" s="44" t="s">
         <v>3</v>
       </c>
@@ -5133,7 +5132,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A27" s="89" t="s">
+      <c r="A27" s="88" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="45" t="s">
@@ -5178,21 +5177,21 @@
         <f>SUM(Individuals!U27:V27)</f>
         <v>3</v>
       </c>
-      <c r="M27" s="51">
+      <c r="M27" s="49">
         <f>SUM(Individuals!W27:X27)</f>
         <v>120</v>
       </c>
-      <c r="N27" s="51">
+      <c r="N27" s="50">
         <f>SUM(Individuals!Y27:Z27)</f>
         <v>6</v>
       </c>
-      <c r="O27" s="51">
+      <c r="O27" s="49">
         <f>SUM(Individuals!AA27:BB27)</f>
         <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A28" s="89"/>
+      <c r="A28" s="88"/>
       <c r="B28" s="44" t="s">
         <v>3</v>
       </c>
@@ -5235,24 +5234,24 @@
         <f>SUM(Individuals!U28:V28)</f>
         <v>12</v>
       </c>
-      <c r="M28" s="51">
+      <c r="M28" s="49">
         <f>SUM(Individuals!W28:X28)</f>
         <v>141</v>
       </c>
-      <c r="N28" s="51">
+      <c r="N28" s="49">
         <f>SUM(Individuals!Y28:Z28)</f>
         <v>69</v>
       </c>
-      <c r="O28" s="51">
+      <c r="O28" s="50">
         <f>SUM(Individuals!AA28:BB28)</f>
         <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="16" thickTop="1">
-      <c r="A29" s="89" t="s">
+      <c r="A29" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="91" t="s">
+      <c r="B29" s="90" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="27">
@@ -5308,8 +5307,8 @@
       </c>
     </row>
     <row r="30" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A30" s="89"/>
-      <c r="B30" s="91"/>
+      <c r="A30" s="88"/>
+      <c r="B30" s="90"/>
       <c r="C30" s="42">
         <v>412</v>
       </c>
@@ -5363,8 +5362,8 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="16" thickTop="1">
-      <c r="A31" s="89"/>
-      <c r="B31" s="89" t="s">
+      <c r="A31" s="88"/>
+      <c r="B31" s="88" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="33">
@@ -5394,34 +5393,34 @@
         <f>SUM(Individuals!O31:P31)</f>
         <v>0</v>
       </c>
-      <c r="J31" s="61">
+      <c r="J31" s="60">
         <f>SUM(Individuals!Q31:R31)</f>
         <v>0</v>
       </c>
-      <c r="K31" s="61">
+      <c r="K31" s="60">
         <f>SUM(Individuals!S31:T31)</f>
         <v>0</v>
       </c>
-      <c r="L31" s="61">
+      <c r="L31" s="60">
         <f>SUM(Individuals!U31:V31)</f>
         <v>0</v>
       </c>
-      <c r="M31" s="58">
+      <c r="M31" s="53">
         <f>SUM(Individuals!W31:X31)</f>
         <v>108</v>
       </c>
-      <c r="N31" s="58">
+      <c r="N31" s="54">
         <f>SUM(Individuals!Y31:Z31)</f>
         <v>0</v>
       </c>
-      <c r="O31" s="58">
+      <c r="O31" s="54">
         <f>SUM(Individuals!AA31:BB31)</f>
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A32" s="89"/>
-      <c r="B32" s="89"/>
+      <c r="A32" s="88"/>
+      <c r="B32" s="88"/>
       <c r="C32" s="34">
         <v>414</v>
       </c>
@@ -5449,36 +5448,36 @@
         <f>SUM(Individuals!O32:P32)</f>
         <v>1</v>
       </c>
-      <c r="J32" s="62">
+      <c r="J32" s="61">
         <f>SUM(Individuals!Q32:R32)</f>
         <v>0</v>
       </c>
-      <c r="K32" s="62">
+      <c r="K32" s="61">
         <f>SUM(Individuals!S32:T32)</f>
         <v>0</v>
       </c>
-      <c r="L32" s="62">
+      <c r="L32" s="61">
         <f>SUM(Individuals!U32:V32)</f>
         <v>0</v>
       </c>
-      <c r="M32" s="59">
+      <c r="M32" s="43">
         <f>SUM(Individuals!W32:X32)</f>
         <v>0</v>
       </c>
-      <c r="N32" s="59">
+      <c r="N32" s="47">
         <f>SUM(Individuals!Y32:Z32)</f>
         <v>0</v>
       </c>
-      <c r="O32" s="59">
+      <c r="O32" s="47">
         <f>SUM(Individuals!AA32:BB32)</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="16" thickTop="1">
-      <c r="A33" s="89" t="s">
+      <c r="A33" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="91" t="s">
+      <c r="B33" s="90" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="27">
@@ -5520,22 +5519,22 @@
         <f>SUM(Individuals!U33:V33)</f>
         <v>0</v>
       </c>
-      <c r="M33" s="58">
+      <c r="M33" s="54">
         <f>SUM(Individuals!W33:X33)</f>
         <v>5</v>
       </c>
-      <c r="N33" s="58">
+      <c r="N33" s="54">
         <f>SUM(Individuals!Y33:Z33)</f>
         <v>2</v>
       </c>
-      <c r="O33" s="58">
+      <c r="O33" s="53">
         <f>SUM(Individuals!AA33:BB33)</f>
         <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A34" s="89"/>
-      <c r="B34" s="91"/>
+      <c r="A34" s="88"/>
+      <c r="B34" s="90"/>
       <c r="C34" s="42">
         <v>482</v>
       </c>
@@ -5575,21 +5574,21 @@
         <f>SUM(Individuals!U34:V34)</f>
         <v>86</v>
       </c>
-      <c r="M34" s="59">
+      <c r="M34" s="47">
         <f>SUM(Individuals!W34:X34)</f>
         <v>7</v>
       </c>
-      <c r="N34" s="59">
+      <c r="N34" s="47">
         <f>SUM(Individuals!Y34:Z34)</f>
         <v>0</v>
       </c>
-      <c r="O34" s="59">
+      <c r="O34" s="43">
         <f>SUM(Individuals!AA34:BB34)</f>
         <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A35" s="89"/>
+      <c r="A35" s="88"/>
       <c r="B35" s="44" t="s">
         <v>3</v>
       </c>
@@ -5699,134 +5698,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="71" customHeight="1">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
     </row>
     <row r="2" spans="1:23" ht="25">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
-      <c r="C2" s="96">
+      <c r="C2" s="95">
         <v>2015</v>
       </c>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="97">
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="96">
         <v>2016</v>
       </c>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="98">
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="97">
         <v>2017</v>
       </c>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="99">
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="98">
         <v>2018</v>
       </c>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
     </row>
     <row r="3" spans="1:23" ht="23">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="64" t="s">
+      <c r="E3" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="65" t="s">
+      <c r="H3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="66" t="s">
+      <c r="I3" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="66" t="s">
+      <c r="J3" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="66" t="s">
+      <c r="K3" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="67" t="s">
+      <c r="L3" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="71" t="s">
+      <c r="M3" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="72" t="s">
+      <c r="N3" s="71" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:23">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="68">
+      <c r="C4" s="67">
         <f>SUM(Individuals!E4:F5,Individuals!E7:F7)</f>
         <v>134</v>
       </c>
-      <c r="D4" s="68">
+      <c r="D4" s="67">
         <f>SUM(Individuals!G4:H5,Individuals!G7:H7)</f>
         <v>1</v>
       </c>
-      <c r="E4" s="68">
+      <c r="E4" s="67">
         <f>SUM(Individuals!I4:J5,Individuals!I7:J7)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="68">
+      <c r="F4" s="67">
         <f>SUM(Individuals!K4:L5,Individuals!K7:L7)</f>
         <v>4</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="67">
         <f>SUM(Individuals!M4:N5,Individuals!M7:N7)</f>
         <v>43</v>
       </c>
-      <c r="H4" s="68">
+      <c r="H4" s="67">
         <f>SUM(Individuals!O4:P5,Individuals!O7:P7)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="68">
+      <c r="I4" s="67">
         <f>SUM(Individuals!Q4:R5,Individuals!Q7:R7)</f>
         <v>246</v>
       </c>
-      <c r="J4" s="68">
+      <c r="J4" s="67">
         <f>SUM(Individuals!S4:T5,Individuals!S7:T7)</f>
         <v>148</v>
       </c>
-      <c r="K4" s="68">
+      <c r="K4" s="67">
         <f>SUM(Individuals!U4:V5,Individuals!U7:V7)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="68">
+      <c r="L4" s="67">
         <f>SUM(Individuals!W4:X5,Individuals!W7:X7)</f>
         <v>57</v>
       </c>
-      <c r="M4" s="68">
+      <c r="M4" s="67">
         <f>SUM(Individuals!Y4:Z5,Individuals!Y7:Z7)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="68">
+      <c r="N4" s="67">
         <f>SUM(Individuals!AA4:BB5,Individuals!AA7:BB7)</f>
         <v>0</v>
       </c>
@@ -5841,55 +5840,55 @@
       <c r="W4" s="1"/>
     </row>
     <row r="5" spans="1:23">
-      <c r="A5" s="104"/>
-      <c r="B5" s="70" t="s">
+      <c r="A5" s="103"/>
+      <c r="B5" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="70">
+      <c r="C5" s="69">
         <f>SUM(Individuals!E6:F6,Individuals!E8:F9)</f>
         <v>310</v>
       </c>
-      <c r="D5" s="70">
+      <c r="D5" s="69">
         <f>SUM(Individuals!G6:H6,Individuals!G8:H9)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="70">
+      <c r="E5" s="69">
         <f>SUM(Individuals!I6:J6,Individuals!I8:J9)</f>
         <v>51</v>
       </c>
-      <c r="F5" s="70">
+      <c r="F5" s="69">
         <f>SUM(Individuals!K6:L6,Individuals!K8:L9)</f>
         <v>298</v>
       </c>
-      <c r="G5" s="70">
+      <c r="G5" s="69">
         <f>SUM(Individuals!M6:N6,Individuals!M8:N9)</f>
         <v>87</v>
       </c>
-      <c r="H5" s="70">
+      <c r="H5" s="69">
         <f>SUM(Individuals!O6:P6,Individuals!O8:P9)</f>
         <v>39</v>
       </c>
-      <c r="I5" s="70">
+      <c r="I5" s="69">
         <f>SUM(Individuals!Q6:R6,Individuals!Q8:R9)</f>
         <v>56</v>
       </c>
-      <c r="J5" s="70">
+      <c r="J5" s="69">
         <f>SUM(Individuals!S6:T6,Individuals!S8:T9)</f>
         <v>0</v>
       </c>
-      <c r="K5" s="70">
+      <c r="K5" s="69">
         <f>SUM(Individuals!U6:V6,Individuals!U8:V9)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="70">
+      <c r="L5" s="69">
         <f>SUM(Individuals!W6:X6,Individuals!W8:X9)</f>
         <v>95</v>
       </c>
-      <c r="M5" s="70">
+      <c r="M5" s="69">
         <f>SUM(Individuals!Y6:Z6,Individuals!Y8:Z9)</f>
         <v>2</v>
       </c>
-      <c r="N5" s="70">
+      <c r="N5" s="69">
         <f>SUM(Individuals!AA6:BB6,Individuals!AA8:BB9)</f>
         <v>0</v>
       </c>
@@ -5904,64 +5903,64 @@
       <c r="W5" s="1"/>
     </row>
     <row r="6" spans="1:23">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="73">
+      <c r="C6" s="72">
         <f>SUM(Individuals!E10:F11,Individuals!E14:F15,Individuals!E17:F17,Individuals!E19:F20)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="73">
+      <c r="D6" s="72">
         <f>SUM(Individuals!G10:H11,Individuals!G14:H15,Individuals!G17:H17,Individuals!G19:H20)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="73">
+      <c r="E6" s="72">
         <f>SUM(Individuals!I10:J11,Individuals!I14:J15,Individuals!I17:J17,Individuals!I19:J20)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="68">
+      <c r="F6" s="67">
         <f>SUM(Individuals!K10:L11,Individuals!K14:L15,Individuals!K17:L17,Individuals!K19:L20)</f>
         <v>261</v>
       </c>
-      <c r="G6" s="68">
+      <c r="G6" s="67">
         <f>SUM(Individuals!M10:N11,Individuals!M14:N15,Individuals!M17:N17,Individuals!M19:N20)</f>
         <v>140</v>
       </c>
-      <c r="H6" s="68">
+      <c r="H6" s="67">
         <f>SUM(Individuals!O10:P11,Individuals!O14:P15,Individuals!O17:P17,Individuals!O19:P20)</f>
         <v>2</v>
       </c>
-      <c r="I6" s="68">
+      <c r="I6" s="67">
         <f>SUM(Individuals!Q10:R11,Individuals!Q14:R15,Individuals!Q17:R17,Individuals!Q19:R20)</f>
         <v>127</v>
       </c>
-      <c r="J6" s="68">
+      <c r="J6" s="67">
         <f>SUM(Individuals!S10:T11,Individuals!S14:T15,Individuals!S17:T17,Individuals!S19:T20)</f>
         <v>110</v>
       </c>
-      <c r="K6" s="68">
+      <c r="K6" s="67">
         <f>SUM(Individuals!U10:V11,Individuals!U14:V15,Individuals!U17:V17,Individuals!U19:V20)</f>
         <v>0</v>
       </c>
-      <c r="L6" s="68">
+      <c r="L6" s="67">
         <f>SUM(Individuals!W10:X11,Individuals!W14:X15,Individuals!W17:X17,Individuals!W19:X20)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="68">
+      <c r="M6" s="67">
         <f>SUM(Individuals!Y10:Z11,Individuals!Y14:Z15,Individuals!Y17:Z17,Individuals!Y19:Z20)</f>
         <v>0</v>
       </c>
-      <c r="N6" s="68">
+      <c r="N6" s="67">
         <f>SUM(Individuals!AA10:AB11,Individuals!AA14:AB15,Individuals!AA17:AB17,Individuals!AA19:AB20)</f>
         <v>0</v>
       </c>
       <c r="O6" s="1"/>
-      <c r="P6" s="70"/>
+      <c r="P6" s="69"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="70"/>
+      <c r="R6" s="69"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -5969,62 +5968,62 @@
       <c r="W6" s="1"/>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="104"/>
-      <c r="B7" s="70" t="s">
+      <c r="A7" s="103"/>
+      <c r="B7" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="74">
+      <c r="C7" s="73">
         <f>SUM(Individuals!E12:F13,Individuals!E16:F16,Individuals!E18:F18,Individuals!E21:F22)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="74">
+      <c r="D7" s="73">
         <f>SUM(Individuals!G12:H13,Individuals!G16:H16,Individuals!G18:H18,Individuals!G21:H22)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="74">
+      <c r="E7" s="73">
         <f>SUM(Individuals!I12:J13,Individuals!I16:J16,Individuals!I18:J18,Individuals!I21:J22)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="70">
+      <c r="F7" s="69">
         <f>SUM(Individuals!K12:L13,Individuals!K16:L16,Individuals!K18:L18,Individuals!K21:L22)</f>
         <v>517</v>
       </c>
-      <c r="G7" s="70">
+      <c r="G7" s="69">
         <f>SUM(Individuals!M12:N13,Individuals!M16:N16,Individuals!M18:N18,Individuals!M21:N22)</f>
         <v>116</v>
       </c>
-      <c r="H7" s="70">
+      <c r="H7" s="69">
         <f>SUM(Individuals!O12:P13,Individuals!O16:P16,Individuals!O18:P18,Individuals!O21:P22)</f>
         <v>183</v>
       </c>
-      <c r="I7" s="70">
+      <c r="I7" s="69">
         <f>SUM(Individuals!Q12:R13,Individuals!Q16:R16,Individuals!Q18:R18,Individuals!Q21:R22)</f>
         <v>322</v>
       </c>
-      <c r="J7" s="70">
+      <c r="J7" s="69">
         <f>SUM(Individuals!S12:T13,Individuals!S16:T16,Individuals!S18:T18,Individuals!S21:T22)</f>
         <v>6</v>
       </c>
-      <c r="K7" s="70">
+      <c r="K7" s="69">
         <f>SUM(Individuals!U12:V13,Individuals!U16:V16,Individuals!U18:V18,Individuals!U21:V22)</f>
         <v>153</v>
       </c>
-      <c r="L7" s="70">
+      <c r="L7" s="69">
         <f>SUM(Individuals!W12:X13,Individuals!W16:X16,Individuals!W18:X18,Individuals!W21:X22)</f>
         <v>60</v>
       </c>
-      <c r="M7" s="70">
+      <c r="M7" s="69">
         <f>SUM(Individuals!Y12:Z13,Individuals!Y16:Z16,Individuals!Y18:Z18,Individuals!Y21:Z22)</f>
         <v>3</v>
       </c>
-      <c r="N7" s="70">
+      <c r="N7" s="69">
         <f>SUM(Individuals!AA12:AB13,Individuals!AA16:AB16,Individuals!AA18:AB18,Individuals!AA21:AB22)</f>
         <v>0</v>
       </c>
       <c r="O7" s="1"/>
-      <c r="P7" s="70"/>
+      <c r="P7" s="69"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="70"/>
+      <c r="R7" s="69"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
@@ -6032,276 +6031,276 @@
       <c r="W7" s="1"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="104" t="s">
+      <c r="A8" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="68">
+      <c r="C8" s="67">
         <f>SUM(Individuals!E23:F23,Individuals!E25:F25)</f>
         <v>41</v>
       </c>
-      <c r="D8" s="68">
+      <c r="D8" s="67">
         <f>SUM(Individuals!G23:H23,Individuals!G25:H25)</f>
         <v>56</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="67">
         <f>SUM(Individuals!I23:J23,Individuals!I25:J25)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="68">
+      <c r="F8" s="67">
         <f>SUM(Individuals!K23:L23,Individuals!K25:L25)</f>
         <v>402</v>
       </c>
-      <c r="G8" s="68">
+      <c r="G8" s="67">
         <f>SUM(Individuals!M23:N23,Individuals!M25:N25)</f>
         <v>1</v>
       </c>
-      <c r="H8" s="68">
+      <c r="H8" s="67">
         <f>SUM(Individuals!O23:P23,Individuals!O25:P25)</f>
         <v>8</v>
       </c>
-      <c r="I8" s="68">
+      <c r="I8" s="67">
         <f>SUM(Individuals!Q23:R23,Individuals!Q25:R25)</f>
         <v>284</v>
       </c>
-      <c r="J8" s="68">
+      <c r="J8" s="67">
         <f>SUM(Individuals!S23:T23,Individuals!S25:T25)</f>
         <v>115</v>
       </c>
-      <c r="K8" s="68">
+      <c r="K8" s="67">
         <f>SUM(Individuals!U23:V23,Individuals!U25:V25)</f>
         <v>0</v>
       </c>
-      <c r="L8" s="68">
+      <c r="L8" s="67">
         <f>SUM(Individuals!W23:X23,Individuals!W25:X25)</f>
         <v>60</v>
       </c>
-      <c r="M8" s="68">
+      <c r="M8" s="67">
         <f>SUM(Individuals!Y23:Z23,Individuals!Y25:Z25)</f>
         <v>43</v>
       </c>
-      <c r="N8" s="68">
+      <c r="N8" s="67">
         <f>SUM(Individuals!AA23:AB23,Individuals!AA25:AB25)</f>
         <v>0</v>
       </c>
       <c r="O8" s="1"/>
-      <c r="P8" s="70"/>
-      <c r="Q8" s="70"/>
-      <c r="R8" s="70"/>
-      <c r="S8" s="70"/>
-      <c r="T8" s="70"/>
-      <c r="U8" s="70"/>
-      <c r="V8" s="70"/>
-      <c r="W8" s="70"/>
+      <c r="P8" s="69"/>
+      <c r="Q8" s="69"/>
+      <c r="R8" s="69"/>
+      <c r="S8" s="69"/>
+      <c r="T8" s="69"/>
+      <c r="U8" s="69"/>
+      <c r="V8" s="69"/>
+      <c r="W8" s="69"/>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="104"/>
-      <c r="B9" s="70" t="s">
+      <c r="A9" s="103"/>
+      <c r="B9" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="70">
+      <c r="C9" s="69">
         <f>SUM(Individuals!E24:F24,Individuals!E26:F26)</f>
         <v>145</v>
       </c>
-      <c r="D9" s="70">
+      <c r="D9" s="69">
         <f>SUM(Individuals!G24:H24,Individuals!G26:H26)</f>
         <v>6</v>
       </c>
-      <c r="E9" s="70">
+      <c r="E9" s="69">
         <f>SUM(Individuals!I24:J24,Individuals!I26:J26)</f>
         <v>12</v>
       </c>
-      <c r="F9" s="70">
+      <c r="F9" s="69">
         <f>SUM(Individuals!K24:L24,Individuals!K26:L26)</f>
         <v>85</v>
       </c>
-      <c r="G9" s="70">
+      <c r="G9" s="69">
         <f>SUM(Individuals!M24:N24,Individuals!M26:N26)</f>
         <v>3</v>
       </c>
-      <c r="H9" s="70">
+      <c r="H9" s="69">
         <f>SUM(Individuals!O24:P24,Individuals!O26:P26)</f>
         <v>84</v>
       </c>
-      <c r="I9" s="70">
+      <c r="I9" s="69">
         <f>SUM(Individuals!Q24:R24,Individuals!Q26:R26)</f>
         <v>173</v>
       </c>
-      <c r="J9" s="70">
+      <c r="J9" s="69">
         <f>SUM(Individuals!S24:T24,Individuals!S26:T26)</f>
         <v>38</v>
       </c>
-      <c r="K9" s="70">
+      <c r="K9" s="69">
         <f>SUM(Individuals!U24:V24,Individuals!U26:V26)</f>
         <v>60</v>
       </c>
-      <c r="L9" s="70">
+      <c r="L9" s="69">
         <f>SUM(Individuals!W24:X24,Individuals!W26:X26)</f>
         <v>108</v>
       </c>
-      <c r="M9" s="70">
+      <c r="M9" s="69">
         <f>SUM(Individuals!Y24:Z24,Individuals!Y26:Z26)</f>
         <v>3</v>
       </c>
-      <c r="N9" s="70">
+      <c r="N9" s="69">
         <f>SUM(Individuals!AA24:AB24,Individuals!AA26:AB26)</f>
         <v>0</v>
       </c>
       <c r="O9" s="1"/>
-      <c r="P9" s="70"/>
-      <c r="Q9" s="70"/>
-      <c r="R9" s="70"/>
-      <c r="S9" s="70"/>
-      <c r="T9" s="70"/>
-      <c r="U9" s="70"/>
-      <c r="V9" s="70"/>
-      <c r="W9" s="70"/>
+      <c r="P9" s="69"/>
+      <c r="Q9" s="69"/>
+      <c r="R9" s="69"/>
+      <c r="S9" s="69"/>
+      <c r="T9" s="69"/>
+      <c r="U9" s="69"/>
+      <c r="V9" s="69"/>
+      <c r="W9" s="69"/>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="104" t="s">
+      <c r="A10" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="68">
+      <c r="C10" s="67">
         <f>SUM(Individuals!E27:F27,Individuals!E29:F30,Individuals!E33:F34)</f>
         <v>298</v>
       </c>
-      <c r="D10" s="68">
+      <c r="D10" s="67">
         <f>SUM(Individuals!G27:H27,Individuals!G29:H30,Individuals!G33:H34)</f>
         <v>81</v>
       </c>
-      <c r="E10" s="68">
+      <c r="E10" s="67">
         <f>SUM(Individuals!I27:J27,Individuals!I29:J30,Individuals!I33:J34)</f>
         <v>137</v>
       </c>
-      <c r="F10" s="68">
+      <c r="F10" s="67">
         <f>SUM(Individuals!K27:L27,Individuals!K29:L30,Individuals!K33:L34)</f>
         <v>29</v>
       </c>
-      <c r="G10" s="68">
+      <c r="G10" s="67">
         <f>SUM(Individuals!M27:N27,Individuals!M29:N30,Individuals!M33:N34)</f>
         <v>6</v>
       </c>
-      <c r="H10" s="68">
+      <c r="H10" s="67">
         <f>SUM(Individuals!O27:P27,Individuals!O29:P30,Individuals!O33:P34)</f>
         <v>44</v>
       </c>
-      <c r="I10" s="68">
+      <c r="I10" s="67">
         <f>SUM(Individuals!Q27:R27,Individuals!Q29:R30,Individuals!Q33:R34)</f>
         <v>209</v>
       </c>
-      <c r="J10" s="68">
+      <c r="J10" s="67">
         <f>SUM(Individuals!S27:T27,Individuals!S29:T30,Individuals!S33:T34)</f>
         <v>87</v>
       </c>
-      <c r="K10" s="68">
+      <c r="K10" s="67">
         <f>SUM(Individuals!U27:V27,Individuals!U29:V30,Individuals!U33:V34)</f>
         <v>159</v>
       </c>
-      <c r="L10" s="68">
+      <c r="L10" s="67">
         <f>SUM(Individuals!W27:X27,Individuals!W29:X30,Individuals!W33:X34)</f>
         <v>132</v>
       </c>
-      <c r="M10" s="68">
+      <c r="M10" s="67">
         <f>SUM(Individuals!Y27:Z27,Individuals!Y29:Z30,Individuals!Y33:Z34)</f>
         <v>8</v>
       </c>
-      <c r="N10" s="68">
+      <c r="N10" s="67">
         <f>SUM(Individuals!AA27:AB27,Individuals!AA29:AB30,Individuals!AA33:AB34)</f>
         <v>253</v>
       </c>
       <c r="O10" s="1"/>
-      <c r="P10" s="70"/>
-      <c r="Q10" s="70"/>
-      <c r="R10" s="70"/>
-      <c r="S10" s="70"/>
-      <c r="T10" s="70"/>
-      <c r="U10" s="70"/>
-      <c r="V10" s="70"/>
-      <c r="W10" s="70"/>
+      <c r="P10" s="69"/>
+      <c r="Q10" s="69"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="69"/>
+      <c r="T10" s="69"/>
+      <c r="U10" s="69"/>
+      <c r="V10" s="69"/>
+      <c r="W10" s="69"/>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="104"/>
-      <c r="B11" s="70" t="s">
+      <c r="A11" s="103"/>
+      <c r="B11" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="70">
+      <c r="C11" s="69">
         <f>SUM(Individuals!E28:F28,Individuals!E31:F32,Individuals!E35:F35)</f>
         <v>175</v>
       </c>
-      <c r="D11" s="70">
+      <c r="D11" s="69">
         <f>SUM(Individuals!G28:H28,Individuals!G31:H32,Individuals!G35:H35)</f>
         <v>162</v>
       </c>
-      <c r="E11" s="70">
+      <c r="E11" s="69">
         <f>SUM(Individuals!I28:J28,Individuals!I31:J32,Individuals!I35:J35)</f>
         <v>224</v>
       </c>
-      <c r="F11" s="70">
+      <c r="F11" s="69">
         <f>SUM(Individuals!K28:L28,Individuals!K31:L32,Individuals!K35:L35)</f>
         <v>125</v>
       </c>
-      <c r="G11" s="70">
+      <c r="G11" s="69">
         <f>SUM(Individuals!M28:N28,Individuals!M31:N32,Individuals!M35:N35)</f>
         <v>8</v>
       </c>
-      <c r="H11" s="70">
+      <c r="H11" s="69">
         <f>SUM(Individuals!O28:P28,Individuals!O31:P32,Individuals!O35:P35)</f>
         <v>131</v>
       </c>
-      <c r="I11" s="70">
+      <c r="I11" s="69">
         <f>SUM(Individuals!Q28:R28,Individuals!Q31:R32,Individuals!Q35:R35)</f>
         <v>96</v>
       </c>
-      <c r="J11" s="70">
+      <c r="J11" s="69">
         <f>SUM(Individuals!S28:T28,Individuals!S31:T32,Individuals!S35:T35)</f>
         <v>28</v>
       </c>
-      <c r="K11" s="70">
+      <c r="K11" s="69">
         <f>SUM(Individuals!U28:V28,Individuals!U31:V32,Individuals!U35:V35)</f>
         <v>88</v>
       </c>
-      <c r="L11" s="70">
+      <c r="L11" s="69">
         <f>SUM(Individuals!W28:X28,Individuals!W31:X32,Individuals!W35:X35)</f>
         <v>283</v>
       </c>
-      <c r="M11" s="70">
+      <c r="M11" s="69">
         <f>SUM(Individuals!Y28:Z28,Individuals!Y31:Z32,Individuals!Y35:Z35)</f>
         <v>106</v>
       </c>
-      <c r="N11" s="70">
+      <c r="N11" s="69">
         <f>SUM(Individuals!AA28:AB28,Individuals!AA31:AB32,Individuals!AA35:AB35)</f>
         <v>52</v>
       </c>
       <c r="O11" s="1"/>
-      <c r="P11" s="70"/>
-      <c r="Q11" s="70"/>
-      <c r="R11" s="70"/>
-      <c r="S11" s="70"/>
-      <c r="T11" s="70"/>
-      <c r="U11" s="70"/>
-      <c r="V11" s="70"/>
-      <c r="W11" s="70"/>
+      <c r="P11" s="69"/>
+      <c r="Q11" s="69"/>
+      <c r="R11" s="69"/>
+      <c r="S11" s="69"/>
+      <c r="T11" s="69"/>
+      <c r="U11" s="69"/>
+      <c r="V11" s="69"/>
+      <c r="W11" s="69"/>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="69"/>
-      <c r="B12" s="70"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="70"/>
-      <c r="M12" s="70"/>
-      <c r="N12" s="70"/>
+      <c r="A12" s="68"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="69"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -6313,28 +6312,28 @@
       <c r="W12" s="1"/>
     </row>
     <row r="13" spans="1:23" ht="25">
-      <c r="A13" s="69"/>
-      <c r="B13" s="70"/>
-      <c r="C13" s="96">
+      <c r="A13" s="68"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="95">
         <v>2015</v>
       </c>
-      <c r="D13" s="96"/>
-      <c r="E13" s="96"/>
-      <c r="F13" s="97">
+      <c r="D13" s="95"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="96">
         <v>2016</v>
       </c>
-      <c r="G13" s="97"/>
-      <c r="H13" s="97"/>
-      <c r="I13" s="98">
+      <c r="G13" s="96"/>
+      <c r="H13" s="96"/>
+      <c r="I13" s="97">
         <v>2017</v>
       </c>
-      <c r="J13" s="98"/>
-      <c r="K13" s="98"/>
-      <c r="L13" s="99">
+      <c r="J13" s="97"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="98">
         <v>2018</v>
       </c>
-      <c r="M13" s="99"/>
-      <c r="N13" s="99"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -6346,436 +6345,436 @@
       <c r="W13" s="1"/>
     </row>
     <row r="14" spans="1:23" ht="23">
-      <c r="A14" s="63" t="s">
+      <c r="A14" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="64" t="s">
+      <c r="C14" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="64" t="s">
+      <c r="D14" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="64" t="s">
+      <c r="E14" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="65" t="s">
+      <c r="F14" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="65" t="s">
+      <c r="G14" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="65" t="s">
+      <c r="H14" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="66" t="s">
+      <c r="I14" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="66" t="s">
+      <c r="J14" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="66" t="s">
+      <c r="K14" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="67" t="s">
+      <c r="L14" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="M14" s="71" t="s">
+      <c r="M14" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="N14" s="72" t="s">
+      <c r="N14" s="71" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:23">
-      <c r="A15" s="101" t="s">
+      <c r="A15" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="75">
+      <c r="C15" s="74">
         <f>SUM(Ind_Summary!D4:D6)</f>
         <v>444</v>
       </c>
-      <c r="D15" s="75">
+      <c r="D15" s="74">
         <f>SUM(Ind_Summary!E4:E6)</f>
         <v>1</v>
       </c>
-      <c r="E15" s="75">
+      <c r="E15" s="74">
         <f>SUM(Ind_Summary!F4:F6)</f>
         <v>51</v>
       </c>
-      <c r="F15" s="75">
+      <c r="F15" s="74">
         <f>SUM(Ind_Summary!G4:G6)</f>
         <v>155</v>
       </c>
-      <c r="G15" s="75">
+      <c r="G15" s="74">
         <f>SUM(Ind_Summary!H4:H6)</f>
         <v>100</v>
       </c>
-      <c r="H15" s="75">
+      <c r="H15" s="74">
         <f>SUM(Ind_Summary!I4:I6)</f>
         <v>35</v>
       </c>
-      <c r="I15" s="75">
+      <c r="I15" s="74">
         <f>SUM(Ind_Summary!J4:J6)</f>
         <v>124</v>
       </c>
-      <c r="J15" s="75">
+      <c r="J15" s="74">
         <f>SUM(Ind_Summary!K4:K6)</f>
         <v>41</v>
       </c>
-      <c r="K15" s="75">
+      <c r="K15" s="74">
         <f>SUM(Ind_Summary!L4:L6)</f>
         <v>0</v>
       </c>
-      <c r="L15" s="75">
+      <c r="L15" s="74">
         <f>SUM(Ind_Summary!M4:M6)</f>
         <v>0</v>
       </c>
-      <c r="M15" s="75">
+      <c r="M15" s="74">
         <f>SUM(Ind_Summary!N4:N6)</f>
         <v>0</v>
       </c>
-      <c r="N15" s="75">
+      <c r="N15" s="74">
         <f>SUM(Ind_Summary!O4:O6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="101"/>
-      <c r="B16" s="75" t="s">
+      <c r="A16" s="100"/>
+      <c r="B16" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="75">
+      <c r="C16" s="74">
         <f>SUM(Ind_Summary!D7:D9)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="75">
+      <c r="D16" s="74">
         <f>SUM(Ind_Summary!E7:E9)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="75">
+      <c r="E16" s="74">
         <f>SUM(Ind_Summary!F7:F9)</f>
         <v>0</v>
       </c>
-      <c r="F16" s="75">
+      <c r="F16" s="74">
         <f>SUM(Ind_Summary!G7:G9)</f>
         <v>147</v>
       </c>
-      <c r="G16" s="75">
+      <c r="G16" s="74">
         <f>SUM(Ind_Summary!H7:H9)</f>
         <v>30</v>
       </c>
-      <c r="H16" s="75">
+      <c r="H16" s="74">
         <f>SUM(Ind_Summary!I7:I9)</f>
         <v>4</v>
       </c>
-      <c r="I16" s="75">
+      <c r="I16" s="74">
         <f>SUM(Ind_Summary!J7:J9)</f>
         <v>178</v>
       </c>
-      <c r="J16" s="75">
+      <c r="J16" s="74">
         <f>SUM(Ind_Summary!K7:K9)</f>
         <v>107</v>
       </c>
-      <c r="K16" s="75">
+      <c r="K16" s="74">
         <f>SUM(Ind_Summary!L7:L9)</f>
         <v>0</v>
       </c>
-      <c r="L16" s="75">
+      <c r="L16" s="74">
         <f>SUM(Ind_Summary!M7:M9)</f>
         <v>152</v>
       </c>
-      <c r="M16" s="75">
+      <c r="M16" s="74">
         <f>SUM(Ind_Summary!N7:N9)</f>
         <v>2</v>
       </c>
-      <c r="N16" s="75">
+      <c r="N16" s="74">
         <f>SUM(Ind_Summary!O7:O9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="101" t="s">
+      <c r="A17" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="75">
+      <c r="C17" s="74">
         <f>SUM(Ind_Summary!D10:D13)</f>
         <v>0</v>
       </c>
-      <c r="D17" s="75">
+      <c r="D17" s="74">
         <f>SUM(Ind_Summary!E10:E13)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="75">
+      <c r="E17" s="74">
         <f>SUM(Ind_Summary!F10:F13)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="75">
+      <c r="F17" s="74">
         <f>SUM(Ind_Summary!G10:G13)</f>
         <v>115</v>
       </c>
-      <c r="G17" s="75">
+      <c r="G17" s="74">
         <f>SUM(Ind_Summary!H10:H13)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="75">
+      <c r="H17" s="74">
         <f>SUM(Ind_Summary!I10:I13)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="75">
+      <c r="I17" s="74">
         <f>SUM(Ind_Summary!J10:J13)</f>
         <v>0</v>
       </c>
-      <c r="J17" s="75">
+      <c r="J17" s="74">
         <f>SUM(Ind_Summary!K10:K13)</f>
         <v>0</v>
       </c>
-      <c r="K17" s="75">
+      <c r="K17" s="74">
         <f>SUM(Ind_Summary!L10:L13)</f>
         <v>0</v>
       </c>
-      <c r="L17" s="75">
+      <c r="L17" s="74">
         <f>SUM(Ind_Summary!M10:M13)</f>
         <v>0</v>
       </c>
-      <c r="M17" s="75">
+      <c r="M17" s="74">
         <f>SUM(Ind_Summary!N10:N13)</f>
         <v>0</v>
       </c>
-      <c r="N17" s="75">
+      <c r="N17" s="74">
         <f>SUM(Ind_Summary!O10:O13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="101"/>
-      <c r="B18" s="75" t="s">
+      <c r="A18" s="100"/>
+      <c r="B18" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="75">
+      <c r="C18" s="74">
         <f>SUM(Ind_Summary!D14:D16)</f>
         <v>0</v>
       </c>
-      <c r="D18" s="75">
+      <c r="D18" s="74">
         <f>SUM(Ind_Summary!E14:E16)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="75">
+      <c r="E18" s="74">
         <f>SUM(Ind_Summary!F14:F16)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="75">
+      <c r="F18" s="74">
         <f>SUM(Ind_Summary!G14:G16)</f>
         <v>149</v>
       </c>
-      <c r="G18" s="75">
+      <c r="G18" s="74">
         <f>SUM(Ind_Summary!H14:H16)</f>
         <v>7</v>
       </c>
-      <c r="H18" s="75">
+      <c r="H18" s="74">
         <f>SUM(Ind_Summary!I14:I16)</f>
         <v>48</v>
       </c>
-      <c r="I18" s="75">
+      <c r="I18" s="74">
         <f>SUM(Ind_Summary!J14:J16)</f>
         <v>49</v>
       </c>
-      <c r="J18" s="75">
+      <c r="J18" s="74">
         <f>SUM(Ind_Summary!K14:K16)</f>
         <v>0</v>
       </c>
-      <c r="K18" s="75">
+      <c r="K18" s="74">
         <f>SUM(Ind_Summary!L14:L16)</f>
         <v>152</v>
       </c>
-      <c r="L18" s="75">
+      <c r="L18" s="74">
         <f>SUM(Ind_Summary!M14:M16)</f>
         <v>0</v>
       </c>
-      <c r="M18" s="75">
+      <c r="M18" s="74">
         <f>SUM(Ind_Summary!N14:N16)</f>
         <v>0</v>
       </c>
-      <c r="N18" s="75">
+      <c r="N18" s="74">
         <f>SUM(Ind_Summary!O14:O16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="101"/>
-      <c r="B19" s="75" t="s">
+      <c r="A19" s="100"/>
+      <c r="B19" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="75">
+      <c r="C19" s="74">
         <f>SUM(Ind_Summary!D17:D18)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="75">
+      <c r="D19" s="74">
         <f>SUM(Ind_Summary!E17:E18)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="75">
+      <c r="E19" s="74">
         <f>SUM(Ind_Summary!F17:F18)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="75">
+      <c r="F19" s="74">
         <f>SUM(Ind_Summary!G17:G18)</f>
         <v>138</v>
       </c>
-      <c r="G19" s="75">
+      <c r="G19" s="74">
         <f>SUM(Ind_Summary!H17:H18)</f>
         <v>119</v>
       </c>
-      <c r="H19" s="75">
+      <c r="H19" s="74">
         <f>SUM(Ind_Summary!I17:I18)</f>
         <v>9</v>
       </c>
-      <c r="I19" s="75">
+      <c r="I19" s="74">
         <f>SUM(Ind_Summary!J17:J18)</f>
         <v>266</v>
       </c>
-      <c r="J19" s="75">
+      <c r="J19" s="74">
         <f>SUM(Ind_Summary!K17:K18)</f>
         <v>6</v>
       </c>
-      <c r="K19" s="75">
+      <c r="K19" s="74">
         <f>SUM(Ind_Summary!L17:L18)</f>
         <v>1</v>
       </c>
-      <c r="L19" s="75">
+      <c r="L19" s="74">
         <f>SUM(Ind_Summary!M17:M18)</f>
         <v>0</v>
       </c>
-      <c r="M19" s="75">
+      <c r="M19" s="74">
         <f>SUM(Ind_Summary!N17:N18)</f>
         <v>0</v>
       </c>
-      <c r="N19" s="75">
+      <c r="N19" s="74">
         <f>SUM(Ind_Summary!O17:O18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="101"/>
-      <c r="B20" s="75" t="s">
+      <c r="A20" s="100"/>
+      <c r="B20" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="75">
+      <c r="C20" s="74">
         <f>SUM(Ind_Summary!D19:D22)</f>
         <v>0</v>
       </c>
-      <c r="D20" s="75">
+      <c r="D20" s="74">
         <f>SUM(Ind_Summary!E19:E22)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="75">
+      <c r="E20" s="74">
         <f>SUM(Ind_Summary!F19:F22)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="75">
+      <c r="F20" s="74">
         <f>SUM(Ind_Summary!G19:G22)</f>
         <v>376</v>
       </c>
-      <c r="G20" s="75">
+      <c r="G20" s="74">
         <f>SUM(Ind_Summary!H19:H22)</f>
         <v>130</v>
       </c>
-      <c r="H20" s="75">
+      <c r="H20" s="74">
         <f>SUM(Ind_Summary!I19:I22)</f>
         <v>128</v>
       </c>
-      <c r="I20" s="75">
+      <c r="I20" s="74">
         <f>SUM(Ind_Summary!J19:J22)</f>
         <v>134</v>
       </c>
-      <c r="J20" s="75">
+      <c r="J20" s="74">
         <f>SUM(Ind_Summary!K19:K22)</f>
         <v>110</v>
       </c>
-      <c r="K20" s="75">
+      <c r="K20" s="74">
         <f>SUM(Ind_Summary!L19:L22)</f>
         <v>0</v>
       </c>
-      <c r="L20" s="75">
+      <c r="L20" s="74">
         <f>SUM(Ind_Summary!M19:M22)</f>
         <v>60</v>
       </c>
-      <c r="M20" s="75">
+      <c r="M20" s="74">
         <f>SUM(Ind_Summary!N19:N22)</f>
         <v>3</v>
       </c>
-      <c r="N20" s="75">
+      <c r="N20" s="74">
         <f>SUM(Ind_Summary!O19:O22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="102" t="s">
+      <c r="A21" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="75">
+      <c r="C21" s="74">
         <f>SUM(Ind_Summary!D23:D24)</f>
         <v>41</v>
       </c>
-      <c r="D21" s="75">
+      <c r="D21" s="74">
         <f>SUM(Ind_Summary!E23:E24)</f>
         <v>56</v>
       </c>
-      <c r="E21" s="75">
+      <c r="E21" s="74">
         <f>SUM(Ind_Summary!F23:F24)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="75">
+      <c r="F21" s="74">
         <f>SUM(Ind_Summary!G23:G24)</f>
         <v>405</v>
       </c>
-      <c r="G21" s="75">
+      <c r="G21" s="74">
         <f>SUM(Ind_Summary!H23:H24)</f>
         <v>4</v>
       </c>
-      <c r="H21" s="75">
+      <c r="H21" s="74">
         <f>SUM(Ind_Summary!I23:I24)</f>
         <v>92</v>
       </c>
-      <c r="I21" s="75">
+      <c r="I21" s="74">
         <f>SUM(Ind_Summary!J23:J24)</f>
         <v>297</v>
       </c>
-      <c r="J21" s="75">
+      <c r="J21" s="74">
         <f>SUM(Ind_Summary!K23:K24)</f>
         <v>54</v>
       </c>
-      <c r="K21" s="75">
+      <c r="K21" s="74">
         <f>SUM(Ind_Summary!L23:L24)</f>
         <v>47</v>
       </c>
-      <c r="L21" s="75">
+      <c r="L21" s="74">
         <f>SUM(Ind_Summary!M23:M24)</f>
         <v>60</v>
       </c>
-      <c r="M21" s="75">
+      <c r="M21" s="74">
         <f>SUM(Ind_Summary!N23:N24)</f>
         <v>43</v>
       </c>
-      <c r="N21" s="75">
+      <c r="N21" s="74">
         <f>SUM(Ind_Summary!O23:O24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="102"/>
-      <c r="B22" s="75" t="s">
+      <c r="A22" s="101"/>
+      <c r="B22" s="74" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="26">
@@ -6828,10 +6827,10 @@
       </c>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="102" t="s">
+      <c r="A23" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="75" t="s">
+      <c r="B23" s="74" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="26">
@@ -6884,8 +6883,8 @@
       </c>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="102"/>
-      <c r="B24" s="75" t="s">
+      <c r="A24" s="101"/>
+      <c r="B24" s="74" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="26">
@@ -6938,8 +6937,8 @@
       </c>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="102"/>
-      <c r="B25" s="75" t="s">
+      <c r="A25" s="101"/>
+      <c r="B25" s="74" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="26">

</xml_diff>

<commit_message>
Update lengths and sample table.
</commit_message>
<xml_diff>
--- a/data/sampleTable.xlsx
+++ b/data/sampleTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15560" windowHeight="17540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="15560" windowHeight="17540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -677,7 +677,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -769,7 +769,6 @@
     <xf numFmtId="0" fontId="13" fillId="15" borderId="15" xfId="22" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="10" xfId="22" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="11" xfId="22" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="8" xfId="22" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="10" xfId="22" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="11" xfId="22" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -814,17 +813,26 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -838,26 +846,17 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1332,34 +1331,34 @@
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75">
+      <c r="B1" s="74">
         <v>2015</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="77">
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="76">
         <v>2016</v>
       </c>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="78">
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="77">
         <v>2017</v>
       </c>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="79">
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="78">
         <v>2018</v>
       </c>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
     </row>
     <row r="2" spans="1:21" s="2" customFormat="1" ht="36">
       <c r="A2" s="6" t="s">
@@ -1643,11 +1642,11 @@
   <dimension ref="A1:AC36"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="P4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="V18" sqref="V18"/>
+      <selection pane="bottomRight" activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1662,97 +1661,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="15" customFormat="1" ht="25">
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="80">
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="90">
         <v>2015</v>
       </c>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="82">
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="92">
         <v>2016</v>
       </c>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="84">
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="86">
         <v>2017</v>
       </c>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="86">
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
+      <c r="U1" s="86"/>
+      <c r="V1" s="86"/>
+      <c r="W1" s="88">
         <v>2018</v>
       </c>
-      <c r="X1" s="86"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="86"/>
-      <c r="AA1" s="86"/>
-      <c r="AB1" s="86"/>
+      <c r="X1" s="88"/>
+      <c r="Y1" s="88"/>
+      <c r="Z1" s="88"/>
+      <c r="AA1" s="88"/>
+      <c r="AB1" s="88"/>
       <c r="AC1" s="13"/>
     </row>
     <row r="2" spans="1:29" s="16" customFormat="1" ht="23">
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="81" t="s">
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81" t="s">
+      <c r="F2" s="91"/>
+      <c r="G2" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81" t="s">
+      <c r="H2" s="91"/>
+      <c r="I2" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="81"/>
-      <c r="K2" s="83" t="s">
+      <c r="J2" s="91"/>
+      <c r="K2" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83" t="s">
+      <c r="L2" s="93"/>
+      <c r="M2" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83" t="s">
+      <c r="N2" s="93"/>
+      <c r="O2" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="85" t="s">
+      <c r="P2" s="93"/>
+      <c r="Q2" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85" t="s">
+      <c r="R2" s="87"/>
+      <c r="S2" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="85"/>
-      <c r="U2" s="85" t="s">
+      <c r="T2" s="87"/>
+      <c r="U2" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="85"/>
-      <c r="W2" s="87" t="s">
+      <c r="V2" s="87"/>
+      <c r="W2" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="87"/>
-      <c r="Y2" s="87" t="s">
+      <c r="X2" s="89"/>
+      <c r="Y2" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="Z2" s="87"/>
-      <c r="AA2" s="87" t="s">
+      <c r="Z2" s="89"/>
+      <c r="AA2" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="87"/>
+      <c r="AB2" s="89"/>
       <c r="AC2" s="14"/>
     </row>
     <row r="3" spans="1:29" s="22" customFormat="1" ht="20">
@@ -1843,13 +1842,13 @@
       <c r="AC3" s="21"/>
     </row>
     <row r="4" spans="1:29">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="80" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="23">
@@ -1917,9 +1916,9 @@
       <c r="AB4" s="24"/>
     </row>
     <row r="5" spans="1:29">
-      <c r="A5" s="88"/>
-      <c r="B5" s="88"/>
-      <c r="C5" s="90"/>
+      <c r="A5" s="81"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="23">
         <v>183</v>
       </c>
@@ -1941,16 +1940,28 @@
       <c r="T5" s="24"/>
       <c r="U5" s="24"/>
       <c r="V5" s="24"/>
-      <c r="W5" s="24"/>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="24"/>
-      <c r="Z5" s="24"/>
-      <c r="AA5" s="24"/>
-      <c r="AB5" s="24"/>
+      <c r="W5" s="24">
+        <v>0</v>
+      </c>
+      <c r="X5" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="24">
+        <v>26</v>
+      </c>
+      <c r="Z5" s="24">
+        <v>26</v>
+      </c>
+      <c r="AA5" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:29">
-      <c r="A6" s="88"/>
-      <c r="B6" s="88"/>
+      <c r="A6" s="81"/>
+      <c r="B6" s="81"/>
       <c r="C6" s="25" t="s">
         <v>3</v>
       </c>
@@ -2007,8 +2018,8 @@
       <c r="AB6" s="26"/>
     </row>
     <row r="7" spans="1:29">
-      <c r="A7" s="88"/>
-      <c r="B7" s="88" t="s">
+      <c r="A7" s="81"/>
+      <c r="B7" s="81" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="23" t="s">
@@ -2079,9 +2090,9 @@
       </c>
     </row>
     <row r="8" spans="1:29">
-      <c r="A8" s="88"/>
-      <c r="B8" s="88"/>
-      <c r="C8" s="88" t="s">
+      <c r="A8" s="81"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="25">
@@ -2137,9 +2148,9 @@
       </c>
     </row>
     <row r="9" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A9" s="89"/>
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
+      <c r="A9" s="82"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
       <c r="D9" s="29">
         <v>171</v>
       </c>
@@ -2156,10 +2167,10 @@
       <c r="O9" s="30"/>
       <c r="P9" s="30"/>
       <c r="Q9" s="30">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="R9" s="30">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="S9" s="30">
         <v>0</v>
@@ -2182,13 +2193,13 @@
       <c r="AC9" s="31"/>
     </row>
     <row r="10" spans="1:29" ht="16" thickTop="1">
-      <c r="A10" s="91" t="s">
+      <c r="A10" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="93" t="s">
+      <c r="C10" s="85" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="27">
@@ -2232,9 +2243,9 @@
       <c r="AB10" s="28"/>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="88"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="90"/>
+      <c r="A11" s="81"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="23">
         <v>139</v>
       </c>
@@ -2264,9 +2275,9 @@
       <c r="AB11" s="24"/>
     </row>
     <row r="12" spans="1:29">
-      <c r="A12" s="88"/>
-      <c r="B12" s="88"/>
-      <c r="C12" s="88" t="s">
+      <c r="A12" s="81"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="25">
@@ -2310,9 +2321,9 @@
       <c r="AB12" s="26"/>
     </row>
     <row r="13" spans="1:29">
-      <c r="A13" s="88"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
+      <c r="A13" s="81"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
       <c r="D13" s="25">
         <v>156</v>
       </c>
@@ -2342,11 +2353,11 @@
       <c r="AB13" s="26"/>
     </row>
     <row r="14" spans="1:29">
-      <c r="A14" s="88"/>
-      <c r="B14" s="88" t="s">
+      <c r="A14" s="81"/>
+      <c r="B14" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="90" t="s">
+      <c r="C14" s="80" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="23">
@@ -2382,17 +2393,29 @@
       <c r="T14" s="24"/>
       <c r="U14" s="24"/>
       <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
-      <c r="X14" s="24"/>
-      <c r="Y14" s="24"/>
-      <c r="Z14" s="24"/>
-      <c r="AA14" s="24"/>
-      <c r="AB14" s="24"/>
+      <c r="W14" s="24">
+        <v>2</v>
+      </c>
+      <c r="X14" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="24">
+        <v>59</v>
+      </c>
+      <c r="Z14" s="24">
+        <v>42</v>
+      </c>
+      <c r="AA14" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:29">
-      <c r="A15" s="88"/>
-      <c r="B15" s="88"/>
-      <c r="C15" s="90"/>
+      <c r="A15" s="81"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="80"/>
       <c r="D15" s="23">
         <v>132</v>
       </c>
@@ -2414,16 +2437,28 @@
       <c r="T15" s="24"/>
       <c r="U15" s="24"/>
       <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
-      <c r="X15" s="24"/>
-      <c r="Y15" s="24"/>
-      <c r="Z15" s="24"/>
-      <c r="AA15" s="24"/>
-      <c r="AB15" s="24"/>
+      <c r="W15" s="24">
+        <v>66</v>
+      </c>
+      <c r="X15" s="24">
+        <v>42</v>
+      </c>
+      <c r="Y15" s="24">
+        <v>37</v>
+      </c>
+      <c r="Z15" s="24">
+        <v>26</v>
+      </c>
+      <c r="AA15" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:29">
-      <c r="A16" s="88"/>
-      <c r="B16" s="88"/>
+      <c r="A16" s="81"/>
+      <c r="B16" s="81"/>
       <c r="C16" s="25" t="s">
         <v>3</v>
       </c>
@@ -2472,16 +2507,28 @@
       <c r="V16" s="26">
         <v>52</v>
       </c>
-      <c r="W16" s="26"/>
-      <c r="X16" s="26"/>
-      <c r="Y16" s="26"/>
-      <c r="Z16" s="26"/>
-      <c r="AA16" s="26"/>
-      <c r="AB16" s="26"/>
+      <c r="W16" s="26">
+        <v>74</v>
+      </c>
+      <c r="X16" s="26">
+        <v>73</v>
+      </c>
+      <c r="Y16" s="26">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="26">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="26">
+        <v>3</v>
+      </c>
+      <c r="AB16" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:29">
-      <c r="A17" s="88"/>
-      <c r="B17" s="88" t="s">
+      <c r="A17" s="81"/>
+      <c r="B17" s="81" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="23" t="s">
@@ -2540,8 +2587,8 @@
       <c r="AB17" s="24"/>
     </row>
     <row r="18" spans="1:29">
-      <c r="A18" s="88"/>
-      <c r="B18" s="88"/>
+      <c r="A18" s="81"/>
+      <c r="B18" s="81"/>
       <c r="C18" s="25" t="s">
         <v>3</v>
       </c>
@@ -2598,11 +2645,11 @@
       <c r="AB18" s="26"/>
     </row>
     <row r="19" spans="1:29">
-      <c r="A19" s="88"/>
-      <c r="B19" s="88" t="s">
+      <c r="A19" s="81"/>
+      <c r="B19" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="90" t="s">
+      <c r="C19" s="80" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="23">
@@ -2638,17 +2685,29 @@
       <c r="T19" s="24"/>
       <c r="U19" s="24"/>
       <c r="V19" s="24"/>
-      <c r="W19" s="24"/>
-      <c r="X19" s="24"/>
-      <c r="Y19" s="24"/>
-      <c r="Z19" s="24"/>
-      <c r="AA19" s="24"/>
-      <c r="AB19" s="24"/>
+      <c r="W19" s="24">
+        <v>33</v>
+      </c>
+      <c r="X19" s="24">
+        <v>19</v>
+      </c>
+      <c r="Y19" s="24">
+        <v>128</v>
+      </c>
+      <c r="Z19" s="24">
+        <v>54</v>
+      </c>
+      <c r="AA19" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:29">
-      <c r="A20" s="88"/>
-      <c r="B20" s="88"/>
-      <c r="C20" s="90"/>
+      <c r="A20" s="81"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="80"/>
       <c r="D20" s="23">
         <v>112</v>
       </c>
@@ -2690,9 +2749,9 @@
       <c r="AB20" s="24"/>
     </row>
     <row r="21" spans="1:29">
-      <c r="A21" s="88"/>
-      <c r="B21" s="88"/>
-      <c r="C21" s="88" t="s">
+      <c r="A21" s="81"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="25">
@@ -2728,17 +2787,29 @@
       <c r="T21" s="26"/>
       <c r="U21" s="26"/>
       <c r="V21" s="26"/>
-      <c r="W21" s="26"/>
-      <c r="X21" s="26"/>
-      <c r="Y21" s="26"/>
-      <c r="Z21" s="26"/>
-      <c r="AA21" s="26"/>
-      <c r="AB21" s="26"/>
+      <c r="W21" s="26">
+        <v>99</v>
+      </c>
+      <c r="X21" s="26">
+        <v>11</v>
+      </c>
+      <c r="Y21" s="26">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="26">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="26">
+        <v>13</v>
+      </c>
+      <c r="AB21" s="26">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A22" s="89"/>
-      <c r="B22" s="89"/>
-      <c r="C22" s="89"/>
+      <c r="A22" s="82"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="82"/>
       <c r="D22" s="29">
         <v>117</v>
       </c>
@@ -2788,7 +2859,7 @@
         <v>60</v>
       </c>
       <c r="X22" s="30">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="Y22" s="30">
         <v>3</v>
@@ -2805,10 +2876,10 @@
       <c r="AC22" s="31"/>
     </row>
     <row r="23" spans="1:29" ht="16" thickTop="1">
-      <c r="A23" s="91" t="s">
+      <c r="A23" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="91" t="s">
+      <c r="B23" s="83" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="35" t="s">
@@ -2891,8 +2962,8 @@
       </c>
     </row>
     <row r="24" spans="1:29">
-      <c r="A24" s="88"/>
-      <c r="B24" s="88"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="81"/>
       <c r="C24" s="25" t="s">
         <v>3</v>
       </c>
@@ -2949,8 +3020,8 @@
       <c r="AB24" s="26"/>
     </row>
     <row r="25" spans="1:29">
-      <c r="A25" s="88"/>
-      <c r="B25" s="88" t="s">
+      <c r="A25" s="81"/>
+      <c r="B25" s="81" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="23" t="s">
@@ -2997,8 +3068,8 @@
       <c r="AB25" s="24"/>
     </row>
     <row r="26" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A26" s="89"/>
-      <c r="B26" s="89"/>
+      <c r="A26" s="82"/>
+      <c r="B26" s="82"/>
       <c r="C26" s="29" t="s">
         <v>3</v>
       </c>
@@ -3080,10 +3151,10 @@
       <c r="AC26" s="31"/>
     </row>
     <row r="27" spans="1:29" ht="16" thickTop="1">
-      <c r="A27" s="92" t="s">
+      <c r="A27" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="92" t="s">
+      <c r="B27" s="84" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="27" t="s">
@@ -3166,8 +3237,8 @@
       </c>
     </row>
     <row r="28" spans="1:29">
-      <c r="A28" s="88"/>
-      <c r="B28" s="88"/>
+      <c r="A28" s="81"/>
+      <c r="B28" s="81"/>
       <c r="C28" s="25" t="s">
         <v>3</v>
       </c>
@@ -3248,11 +3319,11 @@
       </c>
     </row>
     <row r="29" spans="1:29">
-      <c r="A29" s="88"/>
-      <c r="B29" s="88" t="s">
+      <c r="A29" s="81"/>
+      <c r="B29" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="90" t="s">
+      <c r="C29" s="80" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="23">
@@ -3308,9 +3379,9 @@
       <c r="AB29" s="24"/>
     </row>
     <row r="30" spans="1:29">
-      <c r="A30" s="88"/>
-      <c r="B30" s="88"/>
-      <c r="C30" s="90"/>
+      <c r="A30" s="81"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="80"/>
       <c r="D30" s="23">
         <v>412</v>
       </c>
@@ -3352,9 +3423,9 @@
       <c r="AB30" s="24"/>
     </row>
     <row r="31" spans="1:29">
-      <c r="A31" s="88"/>
-      <c r="B31" s="88"/>
-      <c r="C31" s="88" t="s">
+      <c r="A31" s="81"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="81" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="25">
@@ -3410,9 +3481,9 @@
       </c>
     </row>
     <row r="32" spans="1:29">
-      <c r="A32" s="88"/>
-      <c r="B32" s="88"/>
-      <c r="C32" s="88"/>
+      <c r="A32" s="81"/>
+      <c r="B32" s="81"/>
+      <c r="C32" s="81"/>
       <c r="D32" s="25">
         <v>414</v>
       </c>
@@ -3454,11 +3525,11 @@
       <c r="AB32" s="26"/>
     </row>
     <row r="33" spans="1:29">
-      <c r="A33" s="88"/>
-      <c r="B33" s="88" t="s">
+      <c r="A33" s="81"/>
+      <c r="B33" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="90" t="s">
+      <c r="C33" s="80" t="s">
         <v>2</v>
       </c>
       <c r="D33" s="23">
@@ -3514,9 +3585,9 @@
       </c>
     </row>
     <row r="34" spans="1:29">
-      <c r="A34" s="88"/>
-      <c r="B34" s="88"/>
-      <c r="C34" s="90"/>
+      <c r="A34" s="81"/>
+      <c r="B34" s="81"/>
+      <c r="C34" s="80"/>
       <c r="D34" s="23">
         <v>482</v>
       </c>
@@ -3582,8 +3653,8 @@
       </c>
     </row>
     <row r="35" spans="1:29" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A35" s="89"/>
-      <c r="B35" s="89"/>
+      <c r="A35" s="82"/>
+      <c r="B35" s="82"/>
       <c r="C35" s="29" t="s">
         <v>3</v>
       </c>
@@ -3667,12 +3738,27 @@
     <row r="36" spans="1:29" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W1:AB1"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B7:B9"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A27:A35"/>
     <mergeCell ref="C21:C22"/>
@@ -3688,27 +3774,12 @@
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W1:AB1"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K1:P1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B33:B35"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3728,7 +3799,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3737,39 +3808,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="48" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
     </row>
     <row r="2" spans="1:15" ht="25">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
-      <c r="D2" s="95">
+      <c r="D2" s="94">
         <v>2015</v>
       </c>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="96">
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="95">
         <v>2016</v>
       </c>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="97">
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="96">
         <v>2017</v>
       </c>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="98">
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="97">
         <v>2018</v>
       </c>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
     </row>
     <row r="3" spans="1:15" ht="23">
       <c r="A3" s="36" t="s">
@@ -3819,10 +3890,10 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="80" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="23">
@@ -3864,22 +3935,22 @@
         <f>SUM(Individuals!U4:V4)</f>
         <v>0</v>
       </c>
-      <c r="M4" s="59">
+      <c r="M4" s="46">
         <f>SUM(Individuals!W4:X4)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="59">
+      <c r="N4" s="41">
         <f>SUM(Individuals!Y4:Z4)</f>
         <v>0</v>
       </c>
-      <c r="O4" s="59">
+      <c r="O4" s="46">
         <f>SUM(Individuals!AA4:BB4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A5" s="88"/>
-      <c r="B5" s="90"/>
+      <c r="A5" s="81"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="42">
         <v>183</v>
       </c>
@@ -3919,21 +3990,21 @@
         <f>SUM(Individuals!U5:V5)</f>
         <v>0</v>
       </c>
-      <c r="M5" s="58">
+      <c r="M5" s="47">
         <f>SUM(Individuals!W5:X5)</f>
         <v>0</v>
       </c>
-      <c r="N5" s="58">
+      <c r="N5" s="43">
         <f>SUM(Individuals!Y5:Z5)</f>
-        <v>0</v>
-      </c>
-      <c r="O5" s="58">
+        <v>52</v>
+      </c>
+      <c r="O5" s="47">
         <f>SUM(Individuals!AA5:BB5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A6" s="88"/>
+      <c r="A6" s="81"/>
       <c r="B6" s="44" t="s">
         <v>3</v>
       </c>
@@ -3990,7 +4061,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A7" s="88" t="s">
+      <c r="A7" s="81" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="45" t="s">
@@ -4049,8 +4120,8 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="16" thickTop="1">
-      <c r="A8" s="88"/>
-      <c r="B8" s="88" t="s">
+      <c r="A8" s="81"/>
+      <c r="B8" s="81" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="33">
@@ -4106,8 +4177,8 @@
       </c>
     </row>
     <row r="9" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A9" s="88"/>
-      <c r="B9" s="88"/>
+      <c r="A9" s="81"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="34">
         <v>171</v>
       </c>
@@ -4137,7 +4208,7 @@
       </c>
       <c r="J9" s="43">
         <f>SUM(Individuals!Q9:R9)</f>
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="K9" s="47">
         <f>SUM(Individuals!S9:T9)</f>
@@ -4161,10 +4232,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="16" thickTop="1">
-      <c r="A10" s="88" t="s">
+      <c r="A10" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="90" t="s">
+      <c r="B10" s="80" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="27">
@@ -4220,8 +4291,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A11" s="88"/>
-      <c r="B11" s="90"/>
+      <c r="A11" s="81"/>
+      <c r="B11" s="80"/>
       <c r="C11" s="42">
         <v>139</v>
       </c>
@@ -4275,8 +4346,8 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="16" thickTop="1">
-      <c r="A12" s="88"/>
-      <c r="B12" s="88" t="s">
+      <c r="A12" s="81"/>
+      <c r="B12" s="81" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="33">
@@ -4332,8 +4403,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A13" s="88"/>
-      <c r="B13" s="88"/>
+      <c r="A13" s="81"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="34">
         <v>156</v>
       </c>
@@ -4387,10 +4458,10 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" thickTop="1">
-      <c r="A14" s="88" t="s">
+      <c r="A14" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="80" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="27">
@@ -4432,22 +4503,22 @@
         <f>SUM(Individuals!U14:V14)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="52">
+      <c r="M14" s="53">
         <f>SUM(Individuals!W14:X14)</f>
-        <v>0</v>
-      </c>
-      <c r="N14" s="52">
+        <v>2</v>
+      </c>
+      <c r="N14" s="53">
         <f>SUM(Individuals!Y14:Z14)</f>
-        <v>0</v>
-      </c>
-      <c r="O14" s="52">
+        <v>101</v>
+      </c>
+      <c r="O14" s="54">
         <f>SUM(Individuals!AA14:BB14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A15" s="88"/>
-      <c r="B15" s="90"/>
+      <c r="A15" s="81"/>
+      <c r="B15" s="80"/>
       <c r="C15" s="42">
         <v>132</v>
       </c>
@@ -4487,21 +4558,21 @@
         <f>SUM(Individuals!U15:V15)</f>
         <v>0</v>
       </c>
-      <c r="M15" s="48">
+      <c r="M15" s="43">
         <f>SUM(Individuals!W15:X15)</f>
-        <v>0</v>
-      </c>
-      <c r="N15" s="48">
+        <v>108</v>
+      </c>
+      <c r="N15" s="43">
         <f>SUM(Individuals!Y15:Z15)</f>
-        <v>0</v>
-      </c>
-      <c r="O15" s="48">
+        <v>63</v>
+      </c>
+      <c r="O15" s="47">
         <f>SUM(Individuals!AA15:BB15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A16" s="88"/>
+      <c r="A16" s="81"/>
       <c r="B16" s="44" t="s">
         <v>3</v>
       </c>
@@ -4544,21 +4615,21 @@
         <f>SUM(Individuals!U16:V16)</f>
         <v>152</v>
       </c>
-      <c r="M16" s="51">
+      <c r="M16" s="49">
         <f>SUM(Individuals!W16:X16)</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="51">
+        <v>147</v>
+      </c>
+      <c r="N16" s="50">
         <f>SUM(Individuals!Y16:Z16)</f>
-        <v>0</v>
-      </c>
-      <c r="O16" s="51">
+        <v>1</v>
+      </c>
+      <c r="O16" s="50">
         <f>SUM(Individuals!AA16:BB16)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A17" s="88" t="s">
+      <c r="A17" s="81" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="45" t="s">
@@ -4617,7 +4688,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A18" s="88"/>
+      <c r="A18" s="81"/>
       <c r="B18" s="44" t="s">
         <v>3</v>
       </c>
@@ -4674,10 +4745,10 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="16" thickTop="1">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="90" t="s">
+      <c r="B19" s="80" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="27">
@@ -4719,22 +4790,22 @@
         <f>SUM(Individuals!U19:V19)</f>
         <v>0</v>
       </c>
-      <c r="M19" s="52">
+      <c r="M19" s="53">
         <f>SUM(Individuals!W19:X19)</f>
-        <v>0</v>
-      </c>
-      <c r="N19" s="52">
+        <v>52</v>
+      </c>
+      <c r="N19" s="53">
         <f>SUM(Individuals!Y19:Z19)</f>
-        <v>0</v>
-      </c>
-      <c r="O19" s="52">
+        <v>182</v>
+      </c>
+      <c r="O19" s="54">
         <f>SUM(Individuals!AA19:BB19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A20" s="88"/>
-      <c r="B20" s="90"/>
+      <c r="A20" s="81"/>
+      <c r="B20" s="80"/>
       <c r="C20" s="42">
         <v>112</v>
       </c>
@@ -4774,22 +4845,22 @@
         <f>SUM(Individuals!U20:V20)</f>
         <v>0</v>
       </c>
-      <c r="M20" s="48">
+      <c r="M20" s="43">
         <f>SUM(Individuals!W20:X20)</f>
         <v>0</v>
       </c>
-      <c r="N20" s="48">
+      <c r="N20" s="43">
         <f>SUM(Individuals!Y20:Z20)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="48">
+      <c r="O20" s="47">
         <f>SUM(Individuals!AA20:BB20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="16" thickTop="1">
-      <c r="A21" s="88"/>
-      <c r="B21" s="88" t="s">
+      <c r="A21" s="81"/>
+      <c r="B21" s="81" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="33">
@@ -4833,7 +4904,7 @@
       </c>
       <c r="M21" s="53">
         <f>SUM(Individuals!W21:X21)</f>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="N21" s="54">
         <f>SUM(Individuals!Y21:Z21)</f>
@@ -4841,12 +4912,12 @@
       </c>
       <c r="O21" s="54">
         <f>SUM(Individuals!AA21:BB21)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A22" s="88"/>
-      <c r="B22" s="88"/>
+      <c r="A22" s="81"/>
+      <c r="B22" s="81"/>
       <c r="C22" s="34">
         <v>117</v>
       </c>
@@ -4888,7 +4959,7 @@
       </c>
       <c r="M22" s="43">
         <f>SUM(Individuals!W22:X22)</f>
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="N22" s="47">
         <f>SUM(Individuals!Y22:Z22)</f>
@@ -4900,7 +4971,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A23" s="88" t="s">
+      <c r="A23" s="81" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="45" t="s">
@@ -4959,7 +5030,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A24" s="88"/>
+      <c r="A24" s="81"/>
       <c r="B24" s="44" t="s">
         <v>3</v>
       </c>
@@ -5016,7 +5087,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A25" s="88" t="s">
+      <c r="A25" s="81" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="45" t="s">
@@ -5075,7 +5146,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A26" s="88"/>
+      <c r="A26" s="81"/>
       <c r="B26" s="44" t="s">
         <v>3</v>
       </c>
@@ -5132,7 +5203,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A27" s="88" t="s">
+      <c r="A27" s="81" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="45" t="s">
@@ -5191,7 +5262,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A28" s="88"/>
+      <c r="A28" s="81"/>
       <c r="B28" s="44" t="s">
         <v>3</v>
       </c>
@@ -5248,10 +5319,10 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="16" thickTop="1">
-      <c r="A29" s="88" t="s">
+      <c r="A29" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="90" t="s">
+      <c r="B29" s="80" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="27">
@@ -5307,8 +5378,8 @@
       </c>
     </row>
     <row r="30" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A30" s="88"/>
-      <c r="B30" s="90"/>
+      <c r="A30" s="81"/>
+      <c r="B30" s="80"/>
       <c r="C30" s="42">
         <v>412</v>
       </c>
@@ -5362,8 +5433,8 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="16" thickTop="1">
-      <c r="A31" s="88"/>
-      <c r="B31" s="88" t="s">
+      <c r="A31" s="81"/>
+      <c r="B31" s="81" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="33">
@@ -5393,15 +5464,15 @@
         <f>SUM(Individuals!O31:P31)</f>
         <v>0</v>
       </c>
-      <c r="J31" s="60">
+      <c r="J31" s="59">
         <f>SUM(Individuals!Q31:R31)</f>
         <v>0</v>
       </c>
-      <c r="K31" s="60">
+      <c r="K31" s="59">
         <f>SUM(Individuals!S31:T31)</f>
         <v>0</v>
       </c>
-      <c r="L31" s="60">
+      <c r="L31" s="59">
         <f>SUM(Individuals!U31:V31)</f>
         <v>0</v>
       </c>
@@ -5419,8 +5490,8 @@
       </c>
     </row>
     <row r="32" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A32" s="88"/>
-      <c r="B32" s="88"/>
+      <c r="A32" s="81"/>
+      <c r="B32" s="81"/>
       <c r="C32" s="34">
         <v>414</v>
       </c>
@@ -5448,15 +5519,15 @@
         <f>SUM(Individuals!O32:P32)</f>
         <v>1</v>
       </c>
-      <c r="J32" s="61">
+      <c r="J32" s="60">
         <f>SUM(Individuals!Q32:R32)</f>
         <v>0</v>
       </c>
-      <c r="K32" s="61">
+      <c r="K32" s="60">
         <f>SUM(Individuals!S32:T32)</f>
         <v>0</v>
       </c>
-      <c r="L32" s="61">
+      <c r="L32" s="60">
         <f>SUM(Individuals!U32:V32)</f>
         <v>0</v>
       </c>
@@ -5474,10 +5545,10 @@
       </c>
     </row>
     <row r="33" spans="1:15" ht="16" thickTop="1">
-      <c r="A33" s="88" t="s">
+      <c r="A33" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="90" t="s">
+      <c r="B33" s="80" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="27">
@@ -5533,8 +5604,8 @@
       </c>
     </row>
     <row r="34" spans="1:15" s="32" customFormat="1" ht="16" thickBot="1">
-      <c r="A34" s="88"/>
-      <c r="B34" s="90"/>
+      <c r="A34" s="81"/>
+      <c r="B34" s="80"/>
       <c r="C34" s="42">
         <v>482</v>
       </c>
@@ -5588,7 +5659,7 @@
       </c>
     </row>
     <row r="35" spans="1:15" s="32" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="A35" s="88"/>
+      <c r="A35" s="81"/>
       <c r="B35" s="44" t="s">
         <v>3</v>
       </c>
@@ -5635,7 +5706,7 @@
         <f>SUM(Individuals!W35:X35)</f>
         <v>34</v>
       </c>
-      <c r="N35" s="50">
+      <c r="N35" s="49">
         <f>SUM(Individuals!Y35:Z35)</f>
         <v>37</v>
       </c>
@@ -5647,6 +5718,16 @@
     <row r="36" spans="1:15" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="A4:A6"/>
@@ -5663,16 +5744,6 @@
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5698,134 +5769,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="71" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
     </row>
     <row r="2" spans="1:23" ht="25">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
-      <c r="C2" s="95">
+      <c r="C2" s="94">
         <v>2015</v>
       </c>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="96">
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="95">
         <v>2016</v>
       </c>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="97">
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="96">
         <v>2017</v>
       </c>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="98">
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="97">
         <v>2018</v>
       </c>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="1:23" ht="23">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="63" t="s">
+      <c r="E3" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="64" t="s">
+      <c r="F3" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="64" t="s">
+      <c r="G3" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="64" t="s">
+      <c r="H3" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="65" t="s">
+      <c r="I3" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="65" t="s">
+      <c r="J3" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="65" t="s">
+      <c r="K3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="66" t="s">
+      <c r="L3" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="70" t="s">
+      <c r="M3" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="71" t="s">
+      <c r="N3" s="70" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:23">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="67">
+      <c r="C4" s="66">
         <f>SUM(Individuals!E4:F5,Individuals!E7:F7)</f>
         <v>134</v>
       </c>
-      <c r="D4" s="67">
+      <c r="D4" s="66">
         <f>SUM(Individuals!G4:H5,Individuals!G7:H7)</f>
         <v>1</v>
       </c>
-      <c r="E4" s="67">
+      <c r="E4" s="66">
         <f>SUM(Individuals!I4:J5,Individuals!I7:J7)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="67">
+      <c r="F4" s="66">
         <f>SUM(Individuals!K4:L5,Individuals!K7:L7)</f>
         <v>4</v>
       </c>
-      <c r="G4" s="67">
+      <c r="G4" s="66">
         <f>SUM(Individuals!M4:N5,Individuals!M7:N7)</f>
         <v>43</v>
       </c>
-      <c r="H4" s="67">
+      <c r="H4" s="66">
         <f>SUM(Individuals!O4:P5,Individuals!O7:P7)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="67">
+      <c r="I4" s="66">
         <f>SUM(Individuals!Q4:R5,Individuals!Q7:R7)</f>
         <v>246</v>
       </c>
-      <c r="J4" s="67">
+      <c r="J4" s="66">
         <f>SUM(Individuals!S4:T5,Individuals!S7:T7)</f>
         <v>148</v>
       </c>
-      <c r="K4" s="67">
+      <c r="K4" s="66">
         <f>SUM(Individuals!U4:V5,Individuals!U7:V7)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="67">
+      <c r="L4" s="66">
         <f>SUM(Individuals!W4:X5,Individuals!W7:X7)</f>
         <v>57</v>
       </c>
-      <c r="M4" s="67">
+      <c r="M4" s="66">
         <f>SUM(Individuals!Y4:Z5,Individuals!Y7:Z7)</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="67">
+        <v>52</v>
+      </c>
+      <c r="N4" s="66">
         <f>SUM(Individuals!AA4:BB5,Individuals!AA7:BB7)</f>
         <v>0</v>
       </c>
@@ -5840,55 +5911,55 @@
       <c r="W4" s="1"/>
     </row>
     <row r="5" spans="1:23">
-      <c r="A5" s="103"/>
-      <c r="B5" s="69" t="s">
+      <c r="A5" s="102"/>
+      <c r="B5" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="69">
+      <c r="C5" s="68">
         <f>SUM(Individuals!E6:F6,Individuals!E8:F9)</f>
         <v>310</v>
       </c>
-      <c r="D5" s="69">
+      <c r="D5" s="68">
         <f>SUM(Individuals!G6:H6,Individuals!G8:H9)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="69">
+      <c r="E5" s="68">
         <f>SUM(Individuals!I6:J6,Individuals!I8:J9)</f>
         <v>51</v>
       </c>
-      <c r="F5" s="69">
+      <c r="F5" s="68">
         <f>SUM(Individuals!K6:L6,Individuals!K8:L9)</f>
         <v>298</v>
       </c>
-      <c r="G5" s="69">
+      <c r="G5" s="68">
         <f>SUM(Individuals!M6:N6,Individuals!M8:N9)</f>
         <v>87</v>
       </c>
-      <c r="H5" s="69">
+      <c r="H5" s="68">
         <f>SUM(Individuals!O6:P6,Individuals!O8:P9)</f>
         <v>39</v>
       </c>
-      <c r="I5" s="69">
+      <c r="I5" s="68">
         <f>SUM(Individuals!Q6:R6,Individuals!Q8:R9)</f>
-        <v>56</v>
-      </c>
-      <c r="J5" s="69">
+        <v>107</v>
+      </c>
+      <c r="J5" s="68">
         <f>SUM(Individuals!S6:T6,Individuals!S8:T9)</f>
         <v>0</v>
       </c>
-      <c r="K5" s="69">
+      <c r="K5" s="68">
         <f>SUM(Individuals!U6:V6,Individuals!U8:V9)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="69">
+      <c r="L5" s="68">
         <f>SUM(Individuals!W6:X6,Individuals!W8:X9)</f>
         <v>95</v>
       </c>
-      <c r="M5" s="69">
+      <c r="M5" s="68">
         <f>SUM(Individuals!Y6:Z6,Individuals!Y8:Z9)</f>
         <v>2</v>
       </c>
-      <c r="N5" s="69">
+      <c r="N5" s="68">
         <f>SUM(Individuals!AA6:BB6,Individuals!AA8:BB9)</f>
         <v>0</v>
       </c>
@@ -5903,64 +5974,64 @@
       <c r="W5" s="1"/>
     </row>
     <row r="6" spans="1:23">
-      <c r="A6" s="103" t="s">
+      <c r="A6" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="72">
+      <c r="C6" s="71">
         <f>SUM(Individuals!E10:F11,Individuals!E14:F15,Individuals!E17:F17,Individuals!E19:F20)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="72">
+      <c r="D6" s="71">
         <f>SUM(Individuals!G10:H11,Individuals!G14:H15,Individuals!G17:H17,Individuals!G19:H20)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="72">
+      <c r="E6" s="71">
         <f>SUM(Individuals!I10:J11,Individuals!I14:J15,Individuals!I17:J17,Individuals!I19:J20)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="67">
+      <c r="F6" s="66">
         <f>SUM(Individuals!K10:L11,Individuals!K14:L15,Individuals!K17:L17,Individuals!K19:L20)</f>
         <v>261</v>
       </c>
-      <c r="G6" s="67">
+      <c r="G6" s="66">
         <f>SUM(Individuals!M10:N11,Individuals!M14:N15,Individuals!M17:N17,Individuals!M19:N20)</f>
         <v>140</v>
       </c>
-      <c r="H6" s="67">
+      <c r="H6" s="66">
         <f>SUM(Individuals!O10:P11,Individuals!O14:P15,Individuals!O17:P17,Individuals!O19:P20)</f>
         <v>2</v>
       </c>
-      <c r="I6" s="67">
+      <c r="I6" s="66">
         <f>SUM(Individuals!Q10:R11,Individuals!Q14:R15,Individuals!Q17:R17,Individuals!Q19:R20)</f>
         <v>127</v>
       </c>
-      <c r="J6" s="67">
+      <c r="J6" s="66">
         <f>SUM(Individuals!S10:T11,Individuals!S14:T15,Individuals!S17:T17,Individuals!S19:T20)</f>
         <v>110</v>
       </c>
-      <c r="K6" s="67">
+      <c r="K6" s="66">
         <f>SUM(Individuals!U10:V11,Individuals!U14:V15,Individuals!U17:V17,Individuals!U19:V20)</f>
         <v>0</v>
       </c>
-      <c r="L6" s="67">
+      <c r="L6" s="66">
         <f>SUM(Individuals!W10:X11,Individuals!W14:X15,Individuals!W17:X17,Individuals!W19:X20)</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="67">
+        <v>162</v>
+      </c>
+      <c r="M6" s="66">
         <f>SUM(Individuals!Y10:Z11,Individuals!Y14:Z15,Individuals!Y17:Z17,Individuals!Y19:Z20)</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="67">
+        <v>346</v>
+      </c>
+      <c r="N6" s="66">
         <f>SUM(Individuals!AA10:AB11,Individuals!AA14:AB15,Individuals!AA17:AB17,Individuals!AA19:AB20)</f>
         <v>0</v>
       </c>
       <c r="O6" s="1"/>
-      <c r="P6" s="69"/>
+      <c r="P6" s="68"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="69"/>
+      <c r="R6" s="68"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -5968,62 +6039,62 @@
       <c r="W6" s="1"/>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="103"/>
-      <c r="B7" s="69" t="s">
+      <c r="A7" s="102"/>
+      <c r="B7" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="73">
+      <c r="C7" s="72">
         <f>SUM(Individuals!E12:F13,Individuals!E16:F16,Individuals!E18:F18,Individuals!E21:F22)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="73">
+      <c r="D7" s="72">
         <f>SUM(Individuals!G12:H13,Individuals!G16:H16,Individuals!G18:H18,Individuals!G21:H22)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="73">
+      <c r="E7" s="72">
         <f>SUM(Individuals!I12:J13,Individuals!I16:J16,Individuals!I18:J18,Individuals!I21:J22)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="69">
+      <c r="F7" s="68">
         <f>SUM(Individuals!K12:L13,Individuals!K16:L16,Individuals!K18:L18,Individuals!K21:L22)</f>
         <v>517</v>
       </c>
-      <c r="G7" s="69">
+      <c r="G7" s="68">
         <f>SUM(Individuals!M12:N13,Individuals!M16:N16,Individuals!M18:N18,Individuals!M21:N22)</f>
         <v>116</v>
       </c>
-      <c r="H7" s="69">
+      <c r="H7" s="68">
         <f>SUM(Individuals!O12:P13,Individuals!O16:P16,Individuals!O18:P18,Individuals!O21:P22)</f>
         <v>183</v>
       </c>
-      <c r="I7" s="69">
+      <c r="I7" s="68">
         <f>SUM(Individuals!Q12:R13,Individuals!Q16:R16,Individuals!Q18:R18,Individuals!Q21:R22)</f>
         <v>322</v>
       </c>
-      <c r="J7" s="69">
+      <c r="J7" s="68">
         <f>SUM(Individuals!S12:T13,Individuals!S16:T16,Individuals!S18:T18,Individuals!S21:T22)</f>
         <v>6</v>
       </c>
-      <c r="K7" s="69">
+      <c r="K7" s="68">
         <f>SUM(Individuals!U12:V13,Individuals!U16:V16,Individuals!U18:V18,Individuals!U21:V22)</f>
         <v>153</v>
       </c>
-      <c r="L7" s="69">
+      <c r="L7" s="68">
         <f>SUM(Individuals!W12:X13,Individuals!W16:X16,Individuals!W18:X18,Individuals!W21:X22)</f>
-        <v>60</v>
-      </c>
-      <c r="M7" s="69">
+        <v>364</v>
+      </c>
+      <c r="M7" s="68">
         <f>SUM(Individuals!Y12:Z13,Individuals!Y16:Z16,Individuals!Y18:Z18,Individuals!Y21:Z22)</f>
-        <v>3</v>
-      </c>
-      <c r="N7" s="69">
+        <v>4</v>
+      </c>
+      <c r="N7" s="68">
         <f>SUM(Individuals!AA12:AB13,Individuals!AA16:AB16,Individuals!AA18:AB18,Individuals!AA21:AB22)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="O7" s="1"/>
-      <c r="P7" s="69"/>
+      <c r="P7" s="68"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="69"/>
+      <c r="R7" s="68"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
@@ -6031,276 +6102,276 @@
       <c r="W7" s="1"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="103" t="s">
+      <c r="A8" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="67">
+      <c r="C8" s="66">
         <f>SUM(Individuals!E23:F23,Individuals!E25:F25)</f>
         <v>41</v>
       </c>
-      <c r="D8" s="67">
+      <c r="D8" s="66">
         <f>SUM(Individuals!G23:H23,Individuals!G25:H25)</f>
         <v>56</v>
       </c>
-      <c r="E8" s="67">
+      <c r="E8" s="66">
         <f>SUM(Individuals!I23:J23,Individuals!I25:J25)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="67">
+      <c r="F8" s="66">
         <f>SUM(Individuals!K23:L23,Individuals!K25:L25)</f>
         <v>402</v>
       </c>
-      <c r="G8" s="67">
+      <c r="G8" s="66">
         <f>SUM(Individuals!M23:N23,Individuals!M25:N25)</f>
         <v>1</v>
       </c>
-      <c r="H8" s="67">
+      <c r="H8" s="66">
         <f>SUM(Individuals!O23:P23,Individuals!O25:P25)</f>
         <v>8</v>
       </c>
-      <c r="I8" s="67">
+      <c r="I8" s="66">
         <f>SUM(Individuals!Q23:R23,Individuals!Q25:R25)</f>
         <v>284</v>
       </c>
-      <c r="J8" s="67">
+      <c r="J8" s="66">
         <f>SUM(Individuals!S23:T23,Individuals!S25:T25)</f>
         <v>115</v>
       </c>
-      <c r="K8" s="67">
+      <c r="K8" s="66">
         <f>SUM(Individuals!U23:V23,Individuals!U25:V25)</f>
         <v>0</v>
       </c>
-      <c r="L8" s="67">
+      <c r="L8" s="66">
         <f>SUM(Individuals!W23:X23,Individuals!W25:X25)</f>
         <v>60</v>
       </c>
-      <c r="M8" s="67">
+      <c r="M8" s="66">
         <f>SUM(Individuals!Y23:Z23,Individuals!Y25:Z25)</f>
         <v>43</v>
       </c>
-      <c r="N8" s="67">
+      <c r="N8" s="66">
         <f>SUM(Individuals!AA23:AB23,Individuals!AA25:AB25)</f>
         <v>0</v>
       </c>
       <c r="O8" s="1"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="69"/>
-      <c r="S8" s="69"/>
-      <c r="T8" s="69"/>
-      <c r="U8" s="69"/>
-      <c r="V8" s="69"/>
-      <c r="W8" s="69"/>
+      <c r="P8" s="68"/>
+      <c r="Q8" s="68"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="68"/>
+      <c r="T8" s="68"/>
+      <c r="U8" s="68"/>
+      <c r="V8" s="68"/>
+      <c r="W8" s="68"/>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="103"/>
-      <c r="B9" s="69" t="s">
+      <c r="A9" s="102"/>
+      <c r="B9" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="68">
         <f>SUM(Individuals!E24:F24,Individuals!E26:F26)</f>
         <v>145</v>
       </c>
-      <c r="D9" s="69">
+      <c r="D9" s="68">
         <f>SUM(Individuals!G24:H24,Individuals!G26:H26)</f>
         <v>6</v>
       </c>
-      <c r="E9" s="69">
+      <c r="E9" s="68">
         <f>SUM(Individuals!I24:J24,Individuals!I26:J26)</f>
         <v>12</v>
       </c>
-      <c r="F9" s="69">
+      <c r="F9" s="68">
         <f>SUM(Individuals!K24:L24,Individuals!K26:L26)</f>
         <v>85</v>
       </c>
-      <c r="G9" s="69">
+      <c r="G9" s="68">
         <f>SUM(Individuals!M24:N24,Individuals!M26:N26)</f>
         <v>3</v>
       </c>
-      <c r="H9" s="69">
+      <c r="H9" s="68">
         <f>SUM(Individuals!O24:P24,Individuals!O26:P26)</f>
         <v>84</v>
       </c>
-      <c r="I9" s="69">
+      <c r="I9" s="68">
         <f>SUM(Individuals!Q24:R24,Individuals!Q26:R26)</f>
         <v>173</v>
       </c>
-      <c r="J9" s="69">
+      <c r="J9" s="68">
         <f>SUM(Individuals!S24:T24,Individuals!S26:T26)</f>
         <v>38</v>
       </c>
-      <c r="K9" s="69">
+      <c r="K9" s="68">
         <f>SUM(Individuals!U24:V24,Individuals!U26:V26)</f>
         <v>60</v>
       </c>
-      <c r="L9" s="69">
+      <c r="L9" s="68">
         <f>SUM(Individuals!W24:X24,Individuals!W26:X26)</f>
         <v>108</v>
       </c>
-      <c r="M9" s="69">
+      <c r="M9" s="68">
         <f>SUM(Individuals!Y24:Z24,Individuals!Y26:Z26)</f>
         <v>3</v>
       </c>
-      <c r="N9" s="69">
+      <c r="N9" s="68">
         <f>SUM(Individuals!AA24:AB24,Individuals!AA26:AB26)</f>
         <v>0</v>
       </c>
       <c r="O9" s="1"/>
-      <c r="P9" s="69"/>
-      <c r="Q9" s="69"/>
-      <c r="R9" s="69"/>
-      <c r="S9" s="69"/>
-      <c r="T9" s="69"/>
-      <c r="U9" s="69"/>
-      <c r="V9" s="69"/>
-      <c r="W9" s="69"/>
+      <c r="P9" s="68"/>
+      <c r="Q9" s="68"/>
+      <c r="R9" s="68"/>
+      <c r="S9" s="68"/>
+      <c r="T9" s="68"/>
+      <c r="U9" s="68"/>
+      <c r="V9" s="68"/>
+      <c r="W9" s="68"/>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="67">
+      <c r="C10" s="66">
         <f>SUM(Individuals!E27:F27,Individuals!E29:F30,Individuals!E33:F34)</f>
         <v>298</v>
       </c>
-      <c r="D10" s="67">
+      <c r="D10" s="66">
         <f>SUM(Individuals!G27:H27,Individuals!G29:H30,Individuals!G33:H34)</f>
         <v>81</v>
       </c>
-      <c r="E10" s="67">
+      <c r="E10" s="66">
         <f>SUM(Individuals!I27:J27,Individuals!I29:J30,Individuals!I33:J34)</f>
         <v>137</v>
       </c>
-      <c r="F10" s="67">
+      <c r="F10" s="66">
         <f>SUM(Individuals!K27:L27,Individuals!K29:L30,Individuals!K33:L34)</f>
         <v>29</v>
       </c>
-      <c r="G10" s="67">
+      <c r="G10" s="66">
         <f>SUM(Individuals!M27:N27,Individuals!M29:N30,Individuals!M33:N34)</f>
         <v>6</v>
       </c>
-      <c r="H10" s="67">
+      <c r="H10" s="66">
         <f>SUM(Individuals!O27:P27,Individuals!O29:P30,Individuals!O33:P34)</f>
         <v>44</v>
       </c>
-      <c r="I10" s="67">
+      <c r="I10" s="66">
         <f>SUM(Individuals!Q27:R27,Individuals!Q29:R30,Individuals!Q33:R34)</f>
         <v>209</v>
       </c>
-      <c r="J10" s="67">
+      <c r="J10" s="66">
         <f>SUM(Individuals!S27:T27,Individuals!S29:T30,Individuals!S33:T34)</f>
         <v>87</v>
       </c>
-      <c r="K10" s="67">
+      <c r="K10" s="66">
         <f>SUM(Individuals!U27:V27,Individuals!U29:V30,Individuals!U33:V34)</f>
         <v>159</v>
       </c>
-      <c r="L10" s="67">
+      <c r="L10" s="66">
         <f>SUM(Individuals!W27:X27,Individuals!W29:X30,Individuals!W33:X34)</f>
         <v>132</v>
       </c>
-      <c r="M10" s="67">
+      <c r="M10" s="66">
         <f>SUM(Individuals!Y27:Z27,Individuals!Y29:Z30,Individuals!Y33:Z34)</f>
         <v>8</v>
       </c>
-      <c r="N10" s="67">
+      <c r="N10" s="66">
         <f>SUM(Individuals!AA27:AB27,Individuals!AA29:AB30,Individuals!AA33:AB34)</f>
         <v>253</v>
       </c>
       <c r="O10" s="1"/>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="69"/>
-      <c r="R10" s="69"/>
-      <c r="S10" s="69"/>
-      <c r="T10" s="69"/>
-      <c r="U10" s="69"/>
-      <c r="V10" s="69"/>
-      <c r="W10" s="69"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="68"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="68"/>
+      <c r="T10" s="68"/>
+      <c r="U10" s="68"/>
+      <c r="V10" s="68"/>
+      <c r="W10" s="68"/>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="103"/>
-      <c r="B11" s="69" t="s">
+      <c r="A11" s="102"/>
+      <c r="B11" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="69">
+      <c r="C11" s="68">
         <f>SUM(Individuals!E28:F28,Individuals!E31:F32,Individuals!E35:F35)</f>
         <v>175</v>
       </c>
-      <c r="D11" s="69">
+      <c r="D11" s="68">
         <f>SUM(Individuals!G28:H28,Individuals!G31:H32,Individuals!G35:H35)</f>
         <v>162</v>
       </c>
-      <c r="E11" s="69">
+      <c r="E11" s="68">
         <f>SUM(Individuals!I28:J28,Individuals!I31:J32,Individuals!I35:J35)</f>
         <v>224</v>
       </c>
-      <c r="F11" s="69">
+      <c r="F11" s="68">
         <f>SUM(Individuals!K28:L28,Individuals!K31:L32,Individuals!K35:L35)</f>
         <v>125</v>
       </c>
-      <c r="G11" s="69">
+      <c r="G11" s="68">
         <f>SUM(Individuals!M28:N28,Individuals!M31:N32,Individuals!M35:N35)</f>
         <v>8</v>
       </c>
-      <c r="H11" s="69">
+      <c r="H11" s="68">
         <f>SUM(Individuals!O28:P28,Individuals!O31:P32,Individuals!O35:P35)</f>
         <v>131</v>
       </c>
-      <c r="I11" s="69">
+      <c r="I11" s="68">
         <f>SUM(Individuals!Q28:R28,Individuals!Q31:R32,Individuals!Q35:R35)</f>
         <v>96</v>
       </c>
-      <c r="J11" s="69">
+      <c r="J11" s="68">
         <f>SUM(Individuals!S28:T28,Individuals!S31:T32,Individuals!S35:T35)</f>
         <v>28</v>
       </c>
-      <c r="K11" s="69">
+      <c r="K11" s="68">
         <f>SUM(Individuals!U28:V28,Individuals!U31:V32,Individuals!U35:V35)</f>
         <v>88</v>
       </c>
-      <c r="L11" s="69">
+      <c r="L11" s="68">
         <f>SUM(Individuals!W28:X28,Individuals!W31:X32,Individuals!W35:X35)</f>
         <v>283</v>
       </c>
-      <c r="M11" s="69">
+      <c r="M11" s="68">
         <f>SUM(Individuals!Y28:Z28,Individuals!Y31:Z32,Individuals!Y35:Z35)</f>
         <v>106</v>
       </c>
-      <c r="N11" s="69">
+      <c r="N11" s="68">
         <f>SUM(Individuals!AA28:AB28,Individuals!AA31:AB32,Individuals!AA35:AB35)</f>
         <v>52</v>
       </c>
       <c r="O11" s="1"/>
-      <c r="P11" s="69"/>
-      <c r="Q11" s="69"/>
-      <c r="R11" s="69"/>
-      <c r="S11" s="69"/>
-      <c r="T11" s="69"/>
-      <c r="U11" s="69"/>
-      <c r="V11" s="69"/>
-      <c r="W11" s="69"/>
+      <c r="P11" s="68"/>
+      <c r="Q11" s="68"/>
+      <c r="R11" s="68"/>
+      <c r="S11" s="68"/>
+      <c r="T11" s="68"/>
+      <c r="U11" s="68"/>
+      <c r="V11" s="68"/>
+      <c r="W11" s="68"/>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="68"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="69"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="68"/>
+      <c r="L12" s="68"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="68"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -6312,28 +6383,28 @@
       <c r="W12" s="1"/>
     </row>
     <row r="13" spans="1:23" ht="25">
-      <c r="A13" s="68"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="95">
+      <c r="A13" s="67"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="94">
         <v>2015</v>
       </c>
-      <c r="D13" s="95"/>
-      <c r="E13" s="95"/>
-      <c r="F13" s="96">
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="95">
         <v>2016</v>
       </c>
-      <c r="G13" s="96"/>
-      <c r="H13" s="96"/>
-      <c r="I13" s="97">
+      <c r="G13" s="95"/>
+      <c r="H13" s="95"/>
+      <c r="I13" s="96">
         <v>2017</v>
       </c>
-      <c r="J13" s="97"/>
-      <c r="K13" s="97"/>
-      <c r="L13" s="98">
+      <c r="J13" s="96"/>
+      <c r="K13" s="96"/>
+      <c r="L13" s="97">
         <v>2018</v>
       </c>
-      <c r="M13" s="98"/>
-      <c r="N13" s="98"/>
+      <c r="M13" s="97"/>
+      <c r="N13" s="97"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -6345,436 +6416,436 @@
       <c r="W13" s="1"/>
     </row>
     <row r="14" spans="1:23" ht="23">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="63" t="s">
+      <c r="C14" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="63" t="s">
+      <c r="D14" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="63" t="s">
+      <c r="E14" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="64" t="s">
+      <c r="F14" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="64" t="s">
+      <c r="G14" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="64" t="s">
+      <c r="H14" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="65" t="s">
+      <c r="I14" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="65" t="s">
+      <c r="J14" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="65" t="s">
+      <c r="K14" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="66" t="s">
+      <c r="L14" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="M14" s="70" t="s">
+      <c r="M14" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="N14" s="71" t="s">
+      <c r="N14" s="70" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:23">
-      <c r="A15" s="100" t="s">
+      <c r="A15" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="74" t="s">
+      <c r="B15" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="74">
+      <c r="C15" s="73">
         <f>SUM(Ind_Summary!D4:D6)</f>
         <v>444</v>
       </c>
-      <c r="D15" s="74">
+      <c r="D15" s="73">
         <f>SUM(Ind_Summary!E4:E6)</f>
         <v>1</v>
       </c>
-      <c r="E15" s="74">
+      <c r="E15" s="73">
         <f>SUM(Ind_Summary!F4:F6)</f>
         <v>51</v>
       </c>
-      <c r="F15" s="74">
+      <c r="F15" s="73">
         <f>SUM(Ind_Summary!G4:G6)</f>
         <v>155</v>
       </c>
-      <c r="G15" s="74">
+      <c r="G15" s="73">
         <f>SUM(Ind_Summary!H4:H6)</f>
         <v>100</v>
       </c>
-      <c r="H15" s="74">
+      <c r="H15" s="73">
         <f>SUM(Ind_Summary!I4:I6)</f>
         <v>35</v>
       </c>
-      <c r="I15" s="74">
+      <c r="I15" s="73">
         <f>SUM(Ind_Summary!J4:J6)</f>
         <v>124</v>
       </c>
-      <c r="J15" s="74">
+      <c r="J15" s="73">
         <f>SUM(Ind_Summary!K4:K6)</f>
         <v>41</v>
       </c>
-      <c r="K15" s="74">
+      <c r="K15" s="73">
         <f>SUM(Ind_Summary!L4:L6)</f>
         <v>0</v>
       </c>
-      <c r="L15" s="74">
+      <c r="L15" s="73">
         <f>SUM(Ind_Summary!M4:M6)</f>
         <v>0</v>
       </c>
-      <c r="M15" s="74">
+      <c r="M15" s="73">
         <f>SUM(Ind_Summary!N4:N6)</f>
-        <v>0</v>
-      </c>
-      <c r="N15" s="74">
+        <v>52</v>
+      </c>
+      <c r="N15" s="73">
         <f>SUM(Ind_Summary!O4:O6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="100"/>
-      <c r="B16" s="74" t="s">
+      <c r="A16" s="99"/>
+      <c r="B16" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="74">
+      <c r="C16" s="73">
         <f>SUM(Ind_Summary!D7:D9)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="74">
+      <c r="D16" s="73">
         <f>SUM(Ind_Summary!E7:E9)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="74">
+      <c r="E16" s="73">
         <f>SUM(Ind_Summary!F7:F9)</f>
         <v>0</v>
       </c>
-      <c r="F16" s="74">
+      <c r="F16" s="73">
         <f>SUM(Ind_Summary!G7:G9)</f>
         <v>147</v>
       </c>
-      <c r="G16" s="74">
+      <c r="G16" s="73">
         <f>SUM(Ind_Summary!H7:H9)</f>
         <v>30</v>
       </c>
-      <c r="H16" s="74">
+      <c r="H16" s="73">
         <f>SUM(Ind_Summary!I7:I9)</f>
         <v>4</v>
       </c>
-      <c r="I16" s="74">
+      <c r="I16" s="73">
         <f>SUM(Ind_Summary!J7:J9)</f>
-        <v>178</v>
-      </c>
-      <c r="J16" s="74">
+        <v>229</v>
+      </c>
+      <c r="J16" s="73">
         <f>SUM(Ind_Summary!K7:K9)</f>
         <v>107</v>
       </c>
-      <c r="K16" s="74">
+      <c r="K16" s="73">
         <f>SUM(Ind_Summary!L7:L9)</f>
         <v>0</v>
       </c>
-      <c r="L16" s="74">
+      <c r="L16" s="73">
         <f>SUM(Ind_Summary!M7:M9)</f>
         <v>152</v>
       </c>
-      <c r="M16" s="74">
+      <c r="M16" s="73">
         <f>SUM(Ind_Summary!N7:N9)</f>
         <v>2</v>
       </c>
-      <c r="N16" s="74">
+      <c r="N16" s="73">
         <f>SUM(Ind_Summary!O7:O9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="100" t="s">
+      <c r="A17" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="74">
+      <c r="C17" s="73">
         <f>SUM(Ind_Summary!D10:D13)</f>
         <v>0</v>
       </c>
-      <c r="D17" s="74">
+      <c r="D17" s="73">
         <f>SUM(Ind_Summary!E10:E13)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="74">
+      <c r="E17" s="73">
         <f>SUM(Ind_Summary!F10:F13)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="74">
+      <c r="F17" s="73">
         <f>SUM(Ind_Summary!G10:G13)</f>
         <v>115</v>
       </c>
-      <c r="G17" s="74">
+      <c r="G17" s="73">
         <f>SUM(Ind_Summary!H10:H13)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="74">
+      <c r="H17" s="73">
         <f>SUM(Ind_Summary!I10:I13)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="74">
+      <c r="I17" s="73">
         <f>SUM(Ind_Summary!J10:J13)</f>
         <v>0</v>
       </c>
-      <c r="J17" s="74">
+      <c r="J17" s="73">
         <f>SUM(Ind_Summary!K10:K13)</f>
         <v>0</v>
       </c>
-      <c r="K17" s="74">
+      <c r="K17" s="73">
         <f>SUM(Ind_Summary!L10:L13)</f>
         <v>0</v>
       </c>
-      <c r="L17" s="74">
+      <c r="L17" s="73">
         <f>SUM(Ind_Summary!M10:M13)</f>
         <v>0</v>
       </c>
-      <c r="M17" s="74">
+      <c r="M17" s="73">
         <f>SUM(Ind_Summary!N10:N13)</f>
         <v>0</v>
       </c>
-      <c r="N17" s="74">
+      <c r="N17" s="73">
         <f>SUM(Ind_Summary!O10:O13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="100"/>
-      <c r="B18" s="74" t="s">
+      <c r="A18" s="99"/>
+      <c r="B18" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="74">
+      <c r="C18" s="73">
         <f>SUM(Ind_Summary!D14:D16)</f>
         <v>0</v>
       </c>
-      <c r="D18" s="74">
+      <c r="D18" s="73">
         <f>SUM(Ind_Summary!E14:E16)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="74">
+      <c r="E18" s="73">
         <f>SUM(Ind_Summary!F14:F16)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="74">
+      <c r="F18" s="73">
         <f>SUM(Ind_Summary!G14:G16)</f>
         <v>149</v>
       </c>
-      <c r="G18" s="74">
+      <c r="G18" s="73">
         <f>SUM(Ind_Summary!H14:H16)</f>
         <v>7</v>
       </c>
-      <c r="H18" s="74">
+      <c r="H18" s="73">
         <f>SUM(Ind_Summary!I14:I16)</f>
         <v>48</v>
       </c>
-      <c r="I18" s="74">
+      <c r="I18" s="73">
         <f>SUM(Ind_Summary!J14:J16)</f>
         <v>49</v>
       </c>
-      <c r="J18" s="74">
+      <c r="J18" s="73">
         <f>SUM(Ind_Summary!K14:K16)</f>
         <v>0</v>
       </c>
-      <c r="K18" s="74">
+      <c r="K18" s="73">
         <f>SUM(Ind_Summary!L14:L16)</f>
         <v>152</v>
       </c>
-      <c r="L18" s="74">
+      <c r="L18" s="73">
         <f>SUM(Ind_Summary!M14:M16)</f>
-        <v>0</v>
-      </c>
-      <c r="M18" s="74">
+        <v>257</v>
+      </c>
+      <c r="M18" s="73">
         <f>SUM(Ind_Summary!N14:N16)</f>
-        <v>0</v>
-      </c>
-      <c r="N18" s="74">
+        <v>165</v>
+      </c>
+      <c r="N18" s="73">
         <f>SUM(Ind_Summary!O14:O16)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="100"/>
-      <c r="B19" s="74" t="s">
+      <c r="A19" s="99"/>
+      <c r="B19" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="74">
+      <c r="C19" s="73">
         <f>SUM(Ind_Summary!D17:D18)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="74">
+      <c r="D19" s="73">
         <f>SUM(Ind_Summary!E17:E18)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="74">
+      <c r="E19" s="73">
         <f>SUM(Ind_Summary!F17:F18)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="74">
+      <c r="F19" s="73">
         <f>SUM(Ind_Summary!G17:G18)</f>
         <v>138</v>
       </c>
-      <c r="G19" s="74">
+      <c r="G19" s="73">
         <f>SUM(Ind_Summary!H17:H18)</f>
         <v>119</v>
       </c>
-      <c r="H19" s="74">
+      <c r="H19" s="73">
         <f>SUM(Ind_Summary!I17:I18)</f>
         <v>9</v>
       </c>
-      <c r="I19" s="74">
+      <c r="I19" s="73">
         <f>SUM(Ind_Summary!J17:J18)</f>
         <v>266</v>
       </c>
-      <c r="J19" s="74">
+      <c r="J19" s="73">
         <f>SUM(Ind_Summary!K17:K18)</f>
         <v>6</v>
       </c>
-      <c r="K19" s="74">
+      <c r="K19" s="73">
         <f>SUM(Ind_Summary!L17:L18)</f>
         <v>1</v>
       </c>
-      <c r="L19" s="74">
+      <c r="L19" s="73">
         <f>SUM(Ind_Summary!M17:M18)</f>
         <v>0</v>
       </c>
-      <c r="M19" s="74">
+      <c r="M19" s="73">
         <f>SUM(Ind_Summary!N17:N18)</f>
         <v>0</v>
       </c>
-      <c r="N19" s="74">
+      <c r="N19" s="73">
         <f>SUM(Ind_Summary!O17:O18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="100"/>
-      <c r="B20" s="74" t="s">
+      <c r="A20" s="99"/>
+      <c r="B20" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="74">
+      <c r="C20" s="73">
         <f>SUM(Ind_Summary!D19:D22)</f>
         <v>0</v>
       </c>
-      <c r="D20" s="74">
+      <c r="D20" s="73">
         <f>SUM(Ind_Summary!E19:E22)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="74">
+      <c r="E20" s="73">
         <f>SUM(Ind_Summary!F19:F22)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="74">
+      <c r="F20" s="73">
         <f>SUM(Ind_Summary!G19:G22)</f>
         <v>376</v>
       </c>
-      <c r="G20" s="74">
+      <c r="G20" s="73">
         <f>SUM(Ind_Summary!H19:H22)</f>
         <v>130</v>
       </c>
-      <c r="H20" s="74">
+      <c r="H20" s="73">
         <f>SUM(Ind_Summary!I19:I22)</f>
         <v>128</v>
       </c>
-      <c r="I20" s="74">
+      <c r="I20" s="73">
         <f>SUM(Ind_Summary!J19:J22)</f>
         <v>134</v>
       </c>
-      <c r="J20" s="74">
+      <c r="J20" s="73">
         <f>SUM(Ind_Summary!K19:K22)</f>
         <v>110</v>
       </c>
-      <c r="K20" s="74">
+      <c r="K20" s="73">
         <f>SUM(Ind_Summary!L19:L22)</f>
         <v>0</v>
       </c>
-      <c r="L20" s="74">
+      <c r="L20" s="73">
         <f>SUM(Ind_Summary!M19:M22)</f>
-        <v>60</v>
-      </c>
-      <c r="M20" s="74">
+        <v>269</v>
+      </c>
+      <c r="M20" s="73">
         <f>SUM(Ind_Summary!N19:N22)</f>
-        <v>3</v>
-      </c>
-      <c r="N20" s="74">
+        <v>185</v>
+      </c>
+      <c r="N20" s="73">
         <f>SUM(Ind_Summary!O19:O22)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="101" t="s">
+      <c r="A21" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="74" t="s">
+      <c r="B21" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="74">
+      <c r="C21" s="73">
         <f>SUM(Ind_Summary!D23:D24)</f>
         <v>41</v>
       </c>
-      <c r="D21" s="74">
+      <c r="D21" s="73">
         <f>SUM(Ind_Summary!E23:E24)</f>
         <v>56</v>
       </c>
-      <c r="E21" s="74">
+      <c r="E21" s="73">
         <f>SUM(Ind_Summary!F23:F24)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="74">
+      <c r="F21" s="73">
         <f>SUM(Ind_Summary!G23:G24)</f>
         <v>405</v>
       </c>
-      <c r="G21" s="74">
+      <c r="G21" s="73">
         <f>SUM(Ind_Summary!H23:H24)</f>
         <v>4</v>
       </c>
-      <c r="H21" s="74">
+      <c r="H21" s="73">
         <f>SUM(Ind_Summary!I23:I24)</f>
         <v>92</v>
       </c>
-      <c r="I21" s="74">
+      <c r="I21" s="73">
         <f>SUM(Ind_Summary!J23:J24)</f>
         <v>297</v>
       </c>
-      <c r="J21" s="74">
+      <c r="J21" s="73">
         <f>SUM(Ind_Summary!K23:K24)</f>
         <v>54</v>
       </c>
-      <c r="K21" s="74">
+      <c r="K21" s="73">
         <f>SUM(Ind_Summary!L23:L24)</f>
         <v>47</v>
       </c>
-      <c r="L21" s="74">
+      <c r="L21" s="73">
         <f>SUM(Ind_Summary!M23:M24)</f>
         <v>60</v>
       </c>
-      <c r="M21" s="74">
+      <c r="M21" s="73">
         <f>SUM(Ind_Summary!N23:N24)</f>
         <v>43</v>
       </c>
-      <c r="N21" s="74">
+      <c r="N21" s="73">
         <f>SUM(Ind_Summary!O23:O24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="101"/>
-      <c r="B22" s="74" t="s">
+      <c r="A22" s="100"/>
+      <c r="B22" s="73" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="26">
@@ -6827,10 +6898,10 @@
       </c>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="101" t="s">
+      <c r="A23" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="73" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="26">
@@ -6883,8 +6954,8 @@
       </c>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="101"/>
-      <c r="B24" s="74" t="s">
+      <c r="A24" s="100"/>
+      <c r="B24" s="73" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="26">
@@ -6937,8 +7008,8 @@
       </c>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="101"/>
-      <c r="B25" s="74" t="s">
+      <c r="A25" s="100"/>
+      <c r="B25" s="73" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="26">
@@ -6992,14 +7063,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="L13:N13"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A21:A22"/>
@@ -7009,6 +7072,14 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="L13:N13"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:N11">
     <cfRule type="colorScale" priority="2">

</xml_diff>